<commit_message>
Update capture code according to RS.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7702" uniqueCount="2416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7710" uniqueCount="2417">
   <si>
     <t>Req ID</t>
   </si>
@@ -7365,18 +7365,6 @@
     <t>[In Processing a RopSetSearchCriteria ROP Request] Implementation does stop the initial population of the search folder if the STOP_SEARCH bit is set in the SearchFlags field. (Exchange 2007 and above follow this behavior).</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] If OpenSoftDeleted bit in OpenModeFlags is set, implementation ignores the OpenSoftDeleted bit and always opens an existing folder in processing the RopOpenFolder ROP request. [In Appendix A: Product Behavior] &lt;1&gt; Section 2.2.1.1.1: Exchange 2013 and Exchange 2016 ignores the OpenSoftDeleted bit and always opens an existing folder.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] If the specified folder has been hard deleted, implementation does not fail the RopOpenFolder ROP ([MS-OXCROPS] section 2.2.4.1), but no folder is opened. [In Appendix A: Product Behavior] &lt;10&gt; Section 3.2.5.1: If the specified folder has been hard deleted, Exchange 2007 does not fail the RopOpenFolder ROP ([MS-OXCROPS] section 2.2.4.1), but no folder is opened.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does ignore invalid bits instead of failing the ROP [RopDeleteFolder], if the client sets an invalid bit in the DeleteFolderFlags field of the ROP request buffer. (&lt;13&gt; Section 3.2.5.3:  Exchange 2010, Exchange 2013 and Exchange 2016 ignore invalid bits instead of failing the ROP.)</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] If the client sets an invalid bit in the TableFlags field, implementation does not fail the ROP[RopGetHierarchyTable]. (&lt;19&gt; Section 3.2.5.13:  Exchange 2007 ignores invalid bits instead of failing the ROP.)</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does not be regardless of the value of the STATIC_SEARCH bit in the RopSetSearchCriteria ROP request.(Exchange 2010 SP3 and above follow this hebavior).</t>
   </si>
   <si>
@@ -7506,9 +7494,6 @@
     <t>[In Appendix A: Product Behavior] The implementation does not support the PidTagAddressBookEntryId property. &lt;8&gt; Section 2.2.2.2.1.4:  Exchange 2013 and Exchange 2016 do not support the PidTagAddressBookEntryId property.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] The implementation does not support the PidTagAddressBookEntryId property. (Exchange 2007 and Exchange 2010 follow this behavior).</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does not support the RopCopyFolder ROP ([MS-OXCROPS] section 2.2.4.8) between public folder and private mailbox. &lt;4&gt; Section 2.2.1.8: Exchange 2013 and Exchange 2016 do not support the RopCopyFolder ROP ([MS-OXCROPS] section 2.2.4.8) for public folders.</t>
   </si>
   <si>
@@ -7549,6 +7534,24 @@
   </si>
   <si>
     <t>[In PidTagFolderFlags Property] The value is a bitwise OR of zero or more values [1: IPM, 2: SEARCH, 4: NORMAL, 8: RULES] from the following table.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If OpenSoftDeleted bit in OpenModeFlags is set, implementation ignores the OpenSoftDeleted bit and always opens an existing folder in processing the RopOpenFolder ROP request. &lt;1&gt; Section 2.2.1.1.1: Exchange 2013 and Exchange 2016 ignores the OpenSoftDeleted bit and always opens an existing folder.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation does support the PidTagAddressBookEntryId property. (Exchange 2007 and Exchange 2010 follow this behavior).</t>
+  </si>
+  <si>
+    <t>Partially verified by derived requirement: MS-OXCFOLD_R350002.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If the specified folder has been hard deleted, implementation does not fail the RopOpenFolder ROP ([MS-OXCROPS] section 2.2.4.1), but no folder is opened. &lt;10&gt; Section 3.2.5.1: If the specified folder has been hard deleted, Exchange 2007 does not fail the RopOpenFolder ROP ([MS-OXCROPS] section 2.2.4.1), but no folder is opened.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does ignore invalid bits instead of failing the ROP [RopDeleteFolder], if the client sets an invalid bit in the DeleteFolderFlags field of the ROP request buffer. &lt;13&gt; Section 3.2.5.3:  Exchange 2010, Exchange 2013 and Exchange 2016 ignore invalid bits instead of failing the ROP.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If the client sets an invalid bit in the TableFlags field, implementation does not fail the ROP[RopGetHierarchyTable]. &lt;19&gt; Section 3.2.5.13:  Exchange 2007 ignores invalid bits instead of failing the ROP.</t>
   </si>
 </sst>
 </file>
@@ -7842,6 +7845,21 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7866,26 +7884,41 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="63">
+  <dxfs count="69">
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8589,34 +8622,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1083" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1083" tableType="xml" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23" connectionId="1">
   <autoFilter ref="A19:I1083"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="22">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="21">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="20">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="19">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="18">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="17">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8625,12 +8658,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="13" dataDxfId="11" headerRowBorderDxfId="12" tableBorderDxfId="10" totalsRowBorderDxfId="9">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="2"/>
-    <tableColumn id="2" name="Test" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Scope" dataDxfId="8"/>
+    <tableColumn id="2" name="Test" dataDxfId="7"/>
+    <tableColumn id="3" name="Description" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8926,8 +8959,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1084"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A511" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C522" sqref="C522"/>
+    <sheetView tabSelected="1" topLeftCell="B1000" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1003" sqref="C1003"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -8982,127 +9015,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9115,12 +9148,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9133,12 +9166,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9151,12 +9184,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9169,60 +9202,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -12375,7 +12408,7 @@
         <v>1081</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>2410</v>
+        <v>2405</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -13831,7 +13864,7 @@
         <v>1085</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>2412</v>
+        <v>2407</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -20885,7 +20918,7 @@
       <c r="H480" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="I480" s="31" t="s">
+      <c r="I480" s="20" t="s">
         <v>2164</v>
       </c>
     </row>
@@ -21620,7 +21653,7 @@
       </c>
       <c r="I509" s="31"/>
     </row>
-    <row r="510" spans="1:9">
+    <row r="510" spans="1:9" ht="45">
       <c r="A510" s="22" t="s">
         <v>523</v>
       </c>
@@ -21640,10 +21673,12 @@
       <c r="G510" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H510" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I510" s="31"/>
+      <c r="H510" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="I510" s="20" t="s">
+        <v>2413</v>
+      </c>
     </row>
     <row r="511" spans="1:9" ht="30">
       <c r="A511" s="29" t="s">
@@ -21728,7 +21763,7 @@
         <v>1121</v>
       </c>
       <c r="C514" s="35" t="s">
-        <v>2415</v>
+        <v>2410</v>
       </c>
       <c r="D514" s="34"/>
       <c r="E514" s="29" t="s">
@@ -27168,7 +27203,7 @@
         <v>17</v>
       </c>
       <c r="I728" s="20" t="s">
-        <v>2368</v>
+        <v>2364</v>
       </c>
     </row>
     <row r="729" spans="1:9" ht="30">
@@ -28312,7 +28347,7 @@
         <v>1157</v>
       </c>
       <c r="C774" s="20" t="s">
-        <v>2411</v>
+        <v>2406</v>
       </c>
       <c r="D774" s="29"/>
       <c r="E774" s="29" t="s">
@@ -28528,7 +28563,7 @@
         <v>17</v>
       </c>
       <c r="I782" s="20" t="s">
-        <v>2396</v>
+        <v>2392</v>
       </c>
     </row>
     <row r="783" spans="1:9" ht="45">
@@ -31190,7 +31225,7 @@
         <v>1162</v>
       </c>
       <c r="C888" s="20" t="s">
-        <v>2369</v>
+        <v>2365</v>
       </c>
       <c r="D888" s="29"/>
       <c r="E888" s="29" t="s">
@@ -31217,7 +31252,7 @@
         <v>1162</v>
       </c>
       <c r="C889" s="20" t="s">
-        <v>2370</v>
+        <v>2366</v>
       </c>
       <c r="D889" s="29"/>
       <c r="E889" s="29" t="s">
@@ -33336,7 +33371,7 @@
         <v>17</v>
       </c>
       <c r="I972" s="20" t="s">
-        <v>2389</v>
+        <v>2385</v>
       </c>
     </row>
     <row r="973" spans="1:9" ht="45">
@@ -33413,7 +33448,7 @@
         <v>17</v>
       </c>
       <c r="I975" s="20" t="s">
-        <v>2390</v>
+        <v>2386</v>
       </c>
     </row>
     <row r="976" spans="1:9" ht="60">
@@ -33674,7 +33709,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="986" spans="1:9" ht="75">
+    <row r="986" spans="1:9" ht="60">
       <c r="A986" s="29" t="s">
         <v>988</v>
       </c>
@@ -33682,7 +33717,7 @@
         <v>1168</v>
       </c>
       <c r="C986" s="20" t="s">
-        <v>2354</v>
+        <v>2411</v>
       </c>
       <c r="D986" s="29" t="s">
         <v>2106</v>
@@ -33711,7 +33746,7 @@
         <v>1168</v>
       </c>
       <c r="C987" s="20" t="s">
-        <v>2409</v>
+        <v>2404</v>
       </c>
       <c r="D987" s="29" t="s">
         <v>2106</v>
@@ -33796,7 +33831,7 @@
         <v>1168</v>
       </c>
       <c r="C990" s="20" t="s">
-        <v>2408</v>
+        <v>2403</v>
       </c>
       <c r="D990" s="29" t="s">
         <v>2107</v>
@@ -33825,7 +33860,7 @@
         <v>1168</v>
       </c>
       <c r="C991" s="20" t="s">
-        <v>2406</v>
+        <v>2401</v>
       </c>
       <c r="D991" s="29" t="s">
         <v>2107</v>
@@ -33854,7 +33889,7 @@
         <v>1168</v>
       </c>
       <c r="C992" s="20" t="s">
-        <v>2407</v>
+        <v>2402</v>
       </c>
       <c r="D992" s="29" t="s">
         <v>2108</v>
@@ -33912,7 +33947,7 @@
         <v>1168</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2403</v>
+        <v>2398</v>
       </c>
       <c r="D994" s="29" t="s">
         <v>2109</v>
@@ -33968,7 +34003,7 @@
         <v>1168</v>
       </c>
       <c r="C996" s="20" t="s">
-        <v>2402</v>
+        <v>2397</v>
       </c>
       <c r="D996" s="29" t="s">
         <v>2110</v>
@@ -34022,7 +34057,7 @@
         <v>1168</v>
       </c>
       <c r="C998" s="20" t="s">
-        <v>2404</v>
+        <v>2399</v>
       </c>
       <c r="D998" s="29" t="s">
         <v>2111</v>
@@ -34078,7 +34113,7 @@
         <v>1168</v>
       </c>
       <c r="C1000" s="20" t="s">
-        <v>2405</v>
+        <v>2400</v>
       </c>
       <c r="D1000" s="29" t="s">
         <v>2112</v>
@@ -34128,45 +34163,59 @@
     </row>
     <row r="1002" spans="1:9" ht="45">
       <c r="A1002" s="34" t="s">
-        <v>2397</v>
+        <v>2393</v>
       </c>
       <c r="B1002" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1002" s="35" t="s">
-        <v>2400</v>
+        <v>2396</v>
       </c>
       <c r="D1002" s="34" t="s">
-        <v>2399</v>
+        <v>2395</v>
       </c>
       <c r="E1002" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1002" s="34"/>
-      <c r="G1002" s="34"/>
-      <c r="H1002" s="34"/>
+      <c r="F1002" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1002" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1002" s="34" t="s">
+        <v>18</v>
+      </c>
       <c r="I1002" s="35"/>
     </row>
     <row r="1003" spans="1:9" ht="45">
       <c r="A1003" s="34" t="s">
-        <v>2398</v>
+        <v>2394</v>
       </c>
       <c r="B1003" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1003" s="35" t="s">
-        <v>2401</v>
+        <v>2412</v>
       </c>
       <c r="D1003" s="34" t="s">
-        <v>2399</v>
+        <v>2395</v>
       </c>
       <c r="E1003" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1003" s="34"/>
-      <c r="G1003" s="34"/>
-      <c r="H1003" s="34"/>
-      <c r="I1003" s="35"/>
+      <c r="F1003" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1003" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1003" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1003" s="31" t="s">
+        <v>2208</v>
+      </c>
     </row>
     <row r="1004" spans="1:9" ht="75">
       <c r="A1004" s="29" t="s">
@@ -34176,7 +34225,7 @@
         <v>1168</v>
       </c>
       <c r="C1004" s="20" t="s">
-        <v>2355</v>
+        <v>2414</v>
       </c>
       <c r="D1004" s="29" t="s">
         <v>2113</v>
@@ -34204,7 +34253,7 @@
       <c r="B1005" s="30" t="s">
         <v>1168</v>
       </c>
-      <c r="C1005" s="31" t="s">
+      <c r="C1005" s="20" t="s">
         <v>2046</v>
       </c>
       <c r="D1005" s="29" t="s">
@@ -34234,7 +34283,7 @@
         <v>1168</v>
       </c>
       <c r="C1006" s="20" t="s">
-        <v>2362</v>
+        <v>2358</v>
       </c>
       <c r="D1006" s="29" t="s">
         <v>2114</v>
@@ -34263,7 +34312,7 @@
         <v>1168</v>
       </c>
       <c r="C1007" s="20" t="s">
-        <v>2363</v>
+        <v>2359</v>
       </c>
       <c r="D1007" s="29" t="s">
         <v>2114</v>
@@ -34286,16 +34335,16 @@
     </row>
     <row r="1008" spans="1:9" ht="45">
       <c r="A1008" s="22" t="s">
-        <v>2364</v>
+        <v>2360</v>
       </c>
       <c r="B1008" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1008" s="35" t="s">
-        <v>2366</v>
+        <v>2362</v>
       </c>
       <c r="D1008" s="34" t="s">
-        <v>2365</v>
+        <v>2361</v>
       </c>
       <c r="E1008" s="29" t="s">
         <v>22</v>
@@ -34315,16 +34364,16 @@
     </row>
     <row r="1009" spans="1:9" ht="45">
       <c r="A1009" s="22" t="s">
-        <v>2414</v>
+        <v>2409</v>
       </c>
       <c r="B1009" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1009" s="35" t="s">
-        <v>2367</v>
+        <v>2363</v>
       </c>
       <c r="D1009" s="34" t="s">
-        <v>2365</v>
+        <v>2361</v>
       </c>
       <c r="E1009" s="29" t="s">
         <v>22</v>
@@ -34379,7 +34428,7 @@
         <v>1168</v>
       </c>
       <c r="C1011" s="20" t="s">
-        <v>2356</v>
+        <v>2415</v>
       </c>
       <c r="D1011" s="22" t="s">
         <v>2115</v>
@@ -34402,16 +34451,16 @@
     </row>
     <row r="1012" spans="1:9" ht="60">
       <c r="A1012" s="34" t="s">
-        <v>2391</v>
+        <v>2387</v>
       </c>
       <c r="B1012" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1012" s="35" t="s">
-        <v>2359</v>
+        <v>2355</v>
       </c>
       <c r="D1012" s="34" t="s">
-        <v>2393</v>
+        <v>2389</v>
       </c>
       <c r="E1012" s="29" t="s">
         <v>22</v>
@@ -34431,16 +34480,16 @@
     </row>
     <row r="1013" spans="1:9" ht="45">
       <c r="A1013" s="34" t="s">
-        <v>2392</v>
+        <v>2388</v>
       </c>
       <c r="B1013" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1013" s="35" t="s">
-        <v>2358</v>
+        <v>2354</v>
       </c>
       <c r="D1013" s="34" t="s">
-        <v>2393</v>
+        <v>2389</v>
       </c>
       <c r="E1013" s="29" t="s">
         <v>22</v>
@@ -34466,7 +34515,7 @@
         <v>1168</v>
       </c>
       <c r="C1014" s="20" t="s">
-        <v>2371</v>
+        <v>2367</v>
       </c>
       <c r="D1014" s="29" t="s">
         <v>2116</v>
@@ -34495,7 +34544,7 @@
         <v>1168</v>
       </c>
       <c r="C1015" s="20" t="s">
-        <v>2372</v>
+        <v>2368</v>
       </c>
       <c r="D1015" s="29" t="s">
         <v>2116</v>
@@ -34524,7 +34573,7 @@
         <v>1168</v>
       </c>
       <c r="C1016" s="20" t="s">
-        <v>2373</v>
+        <v>2369</v>
       </c>
       <c r="D1016" s="29" t="s">
         <v>2116</v>
@@ -34580,7 +34629,7 @@
         <v>1168</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2374</v>
+        <v>2370</v>
       </c>
       <c r="D1018" s="29" t="s">
         <v>2117</v>
@@ -34609,7 +34658,7 @@
         <v>1168</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2376</v>
+        <v>2372</v>
       </c>
       <c r="D1019" s="22" t="s">
         <v>2118</v>
@@ -34638,7 +34687,7 @@
         <v>1168</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2375</v>
+        <v>2371</v>
       </c>
       <c r="D1020" s="29" t="s">
         <v>2118</v>
@@ -34667,7 +34716,7 @@
         <v>1168</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2377</v>
+        <v>2373</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2118</v>
@@ -34723,7 +34772,7 @@
         <v>1168</v>
       </c>
       <c r="C1023" s="20" t="s">
-        <v>2357</v>
+        <v>2416</v>
       </c>
       <c r="D1023" s="29" t="s">
         <v>2120</v>
@@ -34775,16 +34824,16 @@
     </row>
     <row r="1025" spans="1:9" ht="60">
       <c r="A1025" s="34" t="s">
-        <v>2382</v>
+        <v>2378</v>
       </c>
       <c r="B1025" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1025" s="35" t="s">
-        <v>2379</v>
+        <v>2375</v>
       </c>
       <c r="D1025" s="34" t="s">
-        <v>2385</v>
+        <v>2381</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
@@ -34802,16 +34851,16 @@
     </row>
     <row r="1026" spans="1:9" ht="60">
       <c r="A1026" s="34" t="s">
-        <v>2383</v>
+        <v>2379</v>
       </c>
       <c r="B1026" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1026" s="35" t="s">
-        <v>2380</v>
+        <v>2376</v>
       </c>
       <c r="D1026" s="34" t="s">
-        <v>2395</v>
+        <v>2391</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34831,16 +34880,16 @@
     </row>
     <row r="1027" spans="1:9" ht="45">
       <c r="A1027" s="34" t="s">
-        <v>2384</v>
+        <v>2380</v>
       </c>
       <c r="B1027" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1027" s="35" t="s">
-        <v>2378</v>
+        <v>2374</v>
       </c>
       <c r="D1027" s="34" t="s">
-        <v>2395</v>
+        <v>2391</v>
       </c>
       <c r="E1027" s="29" t="s">
         <v>22</v>
@@ -34860,16 +34909,16 @@
     </row>
     <row r="1028" spans="1:9" ht="60">
       <c r="A1028" s="34" t="s">
-        <v>2387</v>
+        <v>2383</v>
       </c>
       <c r="B1028" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1028" s="35" t="s">
-        <v>2360</v>
+        <v>2356</v>
       </c>
       <c r="D1028" s="34" t="s">
-        <v>2394</v>
+        <v>2390</v>
       </c>
       <c r="E1028" s="29" t="s">
         <v>22</v>
@@ -34889,16 +34938,16 @@
     </row>
     <row r="1029" spans="1:9" ht="75">
       <c r="A1029" s="34" t="s">
-        <v>2386</v>
+        <v>2382</v>
       </c>
       <c r="B1029" s="36" t="s">
         <v>1168</v>
       </c>
       <c r="C1029" s="35" t="s">
-        <v>2361</v>
+        <v>2357</v>
       </c>
       <c r="D1029" s="34" t="s">
-        <v>2394</v>
+        <v>2390</v>
       </c>
       <c r="E1029" s="29" t="s">
         <v>22</v>
@@ -34924,7 +34973,7 @@
         <v>1168</v>
       </c>
       <c r="C1030" s="20" t="s">
-        <v>2381</v>
+        <v>2377</v>
       </c>
       <c r="D1030" s="29" t="s">
         <v>2121</v>
@@ -34947,7 +34996,7 @@
     </row>
     <row r="1031" spans="1:9" ht="45">
       <c r="A1031" s="22" t="s">
-        <v>2388</v>
+        <v>2384</v>
       </c>
       <c r="B1031" s="30" t="s">
         <v>1168</v>
@@ -35211,7 +35260,7 @@
         <v>1170</v>
       </c>
       <c r="C1041" s="20" t="s">
-        <v>2413</v>
+        <v>2408</v>
       </c>
       <c r="D1041" s="29"/>
       <c r="E1041" s="29" t="s">
@@ -36284,11 +36333,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36296,169 +36340,174 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A246:I246 A1033:I1083 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A521:I1031 A251:I518">
-    <cfRule type="expression" dxfId="62" priority="107">
+  <conditionalFormatting sqref="A246:I246 A1033:I1083 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1031">
+    <cfRule type="expression" dxfId="68" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="108">
+    <cfRule type="expression" dxfId="67" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="115">
+    <cfRule type="expression" dxfId="66" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A246:I246 A1033:I1083 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A521:I1031 A251:I518">
-    <cfRule type="expression" dxfId="59" priority="61">
+  <conditionalFormatting sqref="A246:I246 A1033:I1083 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1031">
+    <cfRule type="expression" dxfId="65" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="62">
+    <cfRule type="expression" dxfId="64" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="63">
+    <cfRule type="expression" dxfId="63" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F246 F1034:F1083 F20:F241 F521:F1031 F251:F518">
-    <cfRule type="expression" dxfId="56" priority="67">
+    <cfRule type="expression" dxfId="62" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="68">
+    <cfRule type="expression" dxfId="61" priority="68">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1034:I1083 I230 I233:I241">
-    <cfRule type="expression" dxfId="54" priority="58">
+    <cfRule type="expression" dxfId="60" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="53" priority="59">
+    <cfRule type="expression" dxfId="59" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="60">
+    <cfRule type="expression" dxfId="58" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1034:I1083 I230 I233:I241">
-    <cfRule type="expression" dxfId="51" priority="55">
+    <cfRule type="expression" dxfId="57" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="56">
+    <cfRule type="expression" dxfId="56" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="49" priority="57">
+    <cfRule type="expression" dxfId="55" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1033">
-    <cfRule type="expression" dxfId="48" priority="38">
+    <cfRule type="expression" dxfId="54" priority="38">
       <formula>NOT(VLOOKUP(F1033,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="39">
+    <cfRule type="expression" dxfId="53" priority="39">
       <formula>(VLOOKUP(F1033,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1033">
-    <cfRule type="expression" dxfId="46" priority="32">
+    <cfRule type="expression" dxfId="52" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="33">
+    <cfRule type="expression" dxfId="51" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="34">
+    <cfRule type="expression" dxfId="50" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1033">
-    <cfRule type="expression" dxfId="43" priority="29">
+    <cfRule type="expression" dxfId="49" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="30">
+    <cfRule type="expression" dxfId="48" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="31">
+    <cfRule type="expression" dxfId="47" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1032 C1032:I1032">
-    <cfRule type="expression" dxfId="40" priority="26">
+    <cfRule type="expression" dxfId="46" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="27">
+    <cfRule type="expression" dxfId="45" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="28">
+    <cfRule type="expression" dxfId="44" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1032 C1032:I1032">
-    <cfRule type="expression" dxfId="37" priority="21">
+    <cfRule type="expression" dxfId="43" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="22">
+    <cfRule type="expression" dxfId="42" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="23">
+    <cfRule type="expression" dxfId="41" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1032">
-    <cfRule type="expression" dxfId="34" priority="24">
+    <cfRule type="expression" dxfId="40" priority="24">
       <formula>NOT(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="25">
+    <cfRule type="expression" dxfId="39" priority="25">
       <formula>(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1032">
-    <cfRule type="expression" dxfId="32" priority="12">
+    <cfRule type="expression" dxfId="38" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="13">
+    <cfRule type="expression" dxfId="37" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="14">
+    <cfRule type="expression" dxfId="36" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1032">
-    <cfRule type="expression" dxfId="29" priority="9">
+    <cfRule type="expression" dxfId="35" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="10">
+    <cfRule type="expression" dxfId="34" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="11">
+    <cfRule type="expression" dxfId="33" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="32" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="7">
+    <cfRule type="expression" dxfId="31" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="8">
+    <cfRule type="expression" dxfId="30" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="29" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="3">
+    <cfRule type="expression" dxfId="27" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F519:F520">
-    <cfRule type="expression" dxfId="20" priority="4">
+    <cfRule type="expression" dxfId="26" priority="4">
       <formula>NOT(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[MS-OXCFOLD] Update for the review comment
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -7843,6 +7843,21 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7866,21 +7881,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8981,127 +8981,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9114,12 +9114,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9132,12 +9132,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9150,12 +9150,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9168,60 +9168,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -22042,7 +22042,7 @@
         <v>15</v>
       </c>
       <c r="H526" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I526" s="35"/>
     </row>
@@ -36274,11 +36274,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36286,6 +36281,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">

</xml_diff>

<commit_message>
[MS-OXCFOLD]: Add code for fixed TDI 75000.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -7359,9 +7359,6 @@
     <t>[In Processing a RopSetSearchCriteria ROP Request] Implementation does stop the initial population of the search folder if the STOP_SEARCH bit is set in the SearchFlags field. (Exchange 2007 and above follow this behavior).</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does not be regardless of the value of the STATIC_SEARCH bit in the RopSetSearchCriteria ROP request.(Exchange 2010 SP3 and above follow this hebavior).</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation does be regardless of the value of the STATIC_SEARCH bit in the RopSetSearchCriteria ROP request. &lt;14&gt; Section 3.2.5.4:  A content-indexed search is always static on the initial release version of Exchange 2010 and Exchange 2007 regardless of the value of the STATIC_SEARCH bit in the RopSetSearchCriteria request.</t>
   </si>
   <si>
@@ -7549,6 +7546,9 @@
   </si>
   <si>
     <t>MS-OXCFOLD_R35101</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does not be regardless of the value of the STATIC_SEARCH bit in the RopSetSearchCriteria ROP request.(Exchange 2013 and above follow this hebavior).</t>
   </si>
 </sst>
 </file>
@@ -7843,21 +7843,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7881,6 +7866,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8981,127 +8981,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9114,12 +9114,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9132,12 +9132,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9150,12 +9150,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9168,60 +9168,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -12374,7 +12374,7 @@
         <v>1080</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -13830,7 +13830,7 @@
         <v>1084</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -21643,7 +21643,7 @@
         <v>17</v>
       </c>
       <c r="I510" s="20" t="s">
-        <v>2414</v>
+        <v>2413</v>
       </c>
     </row>
     <row r="511" spans="1:9" ht="30">
@@ -21673,7 +21673,7 @@
     </row>
     <row r="512" spans="1:9">
       <c r="A512" s="22" t="s">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>1120</v>
@@ -21729,7 +21729,7 @@
         <v>1120</v>
       </c>
       <c r="C514" s="35" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="D514" s="34"/>
       <c r="E514" s="29" t="s">
@@ -27169,7 +27169,7 @@
         <v>17</v>
       </c>
       <c r="I728" s="20" t="s">
-        <v>2362</v>
+        <v>2361</v>
       </c>
     </row>
     <row r="729" spans="1:9" ht="30">
@@ -28313,7 +28313,7 @@
         <v>1156</v>
       </c>
       <c r="C774" s="20" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="D774" s="29"/>
       <c r="E774" s="29" t="s">
@@ -28529,7 +28529,7 @@
         <v>17</v>
       </c>
       <c r="I782" s="20" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
     </row>
     <row r="783" spans="1:9" ht="45">
@@ -31191,7 +31191,7 @@
         <v>1161</v>
       </c>
       <c r="C888" s="20" t="s">
-        <v>2363</v>
+        <v>2362</v>
       </c>
       <c r="D888" s="29"/>
       <c r="E888" s="29" t="s">
@@ -31218,7 +31218,7 @@
         <v>1161</v>
       </c>
       <c r="C889" s="20" t="s">
-        <v>2364</v>
+        <v>2363</v>
       </c>
       <c r="D889" s="29"/>
       <c r="E889" s="29" t="s">
@@ -33312,7 +33312,7 @@
         <v>17</v>
       </c>
       <c r="I971" s="20" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="972" spans="1:9" ht="45">
@@ -33389,7 +33389,7 @@
         <v>17</v>
       </c>
       <c r="I974" s="20" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="975" spans="1:9" ht="60">
@@ -33658,7 +33658,7 @@
         <v>1167</v>
       </c>
       <c r="C985" s="20" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="D985" s="29" t="s">
         <v>2104</v>
@@ -33687,7 +33687,7 @@
         <v>1167</v>
       </c>
       <c r="C986" s="20" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="D986" s="29" t="s">
         <v>2104</v>
@@ -33772,7 +33772,7 @@
         <v>1167</v>
       </c>
       <c r="C989" s="20" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="D989" s="29" t="s">
         <v>2105</v>
@@ -33801,7 +33801,7 @@
         <v>1167</v>
       </c>
       <c r="C990" s="20" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="D990" s="29" t="s">
         <v>2105</v>
@@ -33830,7 +33830,7 @@
         <v>1167</v>
       </c>
       <c r="C991" s="20" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D991" s="29" t="s">
         <v>2106</v>
@@ -33888,7 +33888,7 @@
         <v>1167</v>
       </c>
       <c r="C993" s="20" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D993" s="29" t="s">
         <v>2107</v>
@@ -33944,7 +33944,7 @@
         <v>1167</v>
       </c>
       <c r="C995" s="20" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="D995" s="29" t="s">
         <v>2108</v>
@@ -33998,7 +33998,7 @@
         <v>1167</v>
       </c>
       <c r="C997" s="20" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="D997" s="29" t="s">
         <v>2109</v>
@@ -34054,7 +34054,7 @@
         <v>1167</v>
       </c>
       <c r="C999" s="20" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D999" s="29" t="s">
         <v>2110</v>
@@ -34104,16 +34104,16 @@
     </row>
     <row r="1001" spans="1:9" ht="45">
       <c r="A1001" s="34" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="B1001" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1001" s="35" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D1001" s="34" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E1001" s="29" t="s">
         <v>22</v>
@@ -34131,16 +34131,16 @@
     </row>
     <row r="1002" spans="1:9" ht="45">
       <c r="A1002" s="34" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="B1002" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1002" s="35" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="D1002" s="34" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="E1002" s="29" t="s">
         <v>22</v>
@@ -34166,7 +34166,7 @@
         <v>1167</v>
       </c>
       <c r="C1003" s="20" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="D1003" s="29" t="s">
         <v>2111</v>
@@ -34224,7 +34224,7 @@
         <v>1167</v>
       </c>
       <c r="C1005" s="20" t="s">
-        <v>2356</v>
+        <v>2355</v>
       </c>
       <c r="D1005" s="29" t="s">
         <v>2112</v>
@@ -34253,7 +34253,7 @@
         <v>1167</v>
       </c>
       <c r="C1006" s="20" t="s">
-        <v>2357</v>
+        <v>2356</v>
       </c>
       <c r="D1006" s="29" t="s">
         <v>2112</v>
@@ -34276,16 +34276,16 @@
     </row>
     <row r="1007" spans="1:9" ht="45">
       <c r="A1007" s="22" t="s">
-        <v>2358</v>
+        <v>2357</v>
       </c>
       <c r="B1007" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1007" s="35" t="s">
-        <v>2360</v>
+        <v>2359</v>
       </c>
       <c r="D1007" s="34" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="E1007" s="29" t="s">
         <v>22</v>
@@ -34305,16 +34305,16 @@
     </row>
     <row r="1008" spans="1:9" ht="45">
       <c r="A1008" s="22" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="B1008" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1008" s="35" t="s">
-        <v>2361</v>
+        <v>2360</v>
       </c>
       <c r="D1008" s="34" t="s">
-        <v>2359</v>
+        <v>2358</v>
       </c>
       <c r="E1008" s="29" t="s">
         <v>22</v>
@@ -34369,7 +34369,7 @@
         <v>1167</v>
       </c>
       <c r="C1010" s="20" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="D1010" s="22" t="s">
         <v>2113</v>
@@ -34392,16 +34392,16 @@
     </row>
     <row r="1011" spans="1:9" ht="60">
       <c r="A1011" s="34" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="B1011" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1011" s="35" t="s">
-        <v>2353</v>
+        <v>2352</v>
       </c>
       <c r="D1011" s="34" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E1011" s="29" t="s">
         <v>22</v>
@@ -34421,16 +34421,16 @@
     </row>
     <row r="1012" spans="1:9" ht="45">
       <c r="A1012" s="34" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="B1012" s="36" t="s">
         <v>1167</v>
       </c>
-      <c r="C1012" s="35" t="s">
-        <v>2352</v>
+      <c r="C1012" s="20" t="s">
+        <v>2415</v>
       </c>
       <c r="D1012" s="34" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E1012" s="29" t="s">
         <v>22</v>
@@ -34456,7 +34456,7 @@
         <v>1167</v>
       </c>
       <c r="C1013" s="20" t="s">
-        <v>2365</v>
+        <v>2364</v>
       </c>
       <c r="D1013" s="29" t="s">
         <v>2114</v>
@@ -34485,7 +34485,7 @@
         <v>1167</v>
       </c>
       <c r="C1014" s="20" t="s">
-        <v>2366</v>
+        <v>2365</v>
       </c>
       <c r="D1014" s="29" t="s">
         <v>2114</v>
@@ -34514,7 +34514,7 @@
         <v>1167</v>
       </c>
       <c r="C1015" s="20" t="s">
-        <v>2367</v>
+        <v>2366</v>
       </c>
       <c r="D1015" s="29" t="s">
         <v>2114</v>
@@ -34570,7 +34570,7 @@
         <v>1167</v>
       </c>
       <c r="C1017" s="20" t="s">
-        <v>2368</v>
+        <v>2367</v>
       </c>
       <c r="D1017" s="29" t="s">
         <v>2115</v>
@@ -34599,7 +34599,7 @@
         <v>1167</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2370</v>
+        <v>2369</v>
       </c>
       <c r="D1018" s="22" t="s">
         <v>2116</v>
@@ -34628,7 +34628,7 @@
         <v>1167</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="D1019" s="29" t="s">
         <v>2116</v>
@@ -34657,7 +34657,7 @@
         <v>1167</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2371</v>
+        <v>2370</v>
       </c>
       <c r="D1020" s="29" t="s">
         <v>2116</v>
@@ -34713,7 +34713,7 @@
         <v>1167</v>
       </c>
       <c r="C1022" s="20" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="D1022" s="29" t="s">
         <v>2118</v>
@@ -34765,16 +34765,16 @@
     </row>
     <row r="1024" spans="1:9" ht="60">
       <c r="A1024" s="34" t="s">
-        <v>2376</v>
+        <v>2375</v>
       </c>
       <c r="B1024" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1024" s="35" t="s">
-        <v>2373</v>
+        <v>2372</v>
       </c>
       <c r="D1024" s="34" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="E1024" s="29" t="s">
         <v>22</v>
@@ -34792,16 +34792,16 @@
     </row>
     <row r="1025" spans="1:9" ht="60">
       <c r="A1025" s="34" t="s">
-        <v>2377</v>
+        <v>2376</v>
       </c>
       <c r="B1025" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1025" s="35" t="s">
-        <v>2374</v>
+        <v>2373</v>
       </c>
       <c r="D1025" s="34" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
@@ -34821,16 +34821,16 @@
     </row>
     <row r="1026" spans="1:9" ht="45">
       <c r="A1026" s="34" t="s">
-        <v>2378</v>
+        <v>2377</v>
       </c>
       <c r="B1026" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1026" s="35" t="s">
-        <v>2372</v>
+        <v>2371</v>
       </c>
       <c r="D1026" s="34" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34850,16 +34850,16 @@
     </row>
     <row r="1027" spans="1:9" ht="60">
       <c r="A1027" s="34" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="B1027" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1027" s="35" t="s">
-        <v>2354</v>
+        <v>2353</v>
       </c>
       <c r="D1027" s="34" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E1027" s="29" t="s">
         <v>22</v>
@@ -34879,16 +34879,16 @@
     </row>
     <row r="1028" spans="1:9" ht="75">
       <c r="A1028" s="34" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="B1028" s="36" t="s">
         <v>1167</v>
       </c>
       <c r="C1028" s="35" t="s">
-        <v>2355</v>
+        <v>2354</v>
       </c>
       <c r="D1028" s="34" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="E1028" s="29" t="s">
         <v>22</v>
@@ -34914,7 +34914,7 @@
         <v>1167</v>
       </c>
       <c r="C1029" s="20" t="s">
-        <v>2375</v>
+        <v>2374</v>
       </c>
       <c r="D1029" s="29" t="s">
         <v>2119</v>
@@ -34937,7 +34937,7 @@
     </row>
     <row r="1030" spans="1:9" ht="45">
       <c r="A1030" s="22" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="B1030" s="30" t="s">
         <v>1167</v>
@@ -35201,7 +35201,7 @@
         <v>1169</v>
       </c>
       <c r="C1040" s="20" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D1040" s="29"/>
       <c r="E1040" s="29" t="s">
@@ -36274,6 +36274,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36281,11 +36286,6 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">

</xml_diff>

<commit_message>
[MS-OXCFOLD]: Update RS for TDI 98688
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7692" uniqueCount="2414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7689" uniqueCount="2413">
   <si>
     <t>Req ID</t>
   </si>
@@ -7435,9 +7435,6 @@
   </si>
   <si>
     <t>MS-OXCFOLD_R330002</t>
-  </si>
-  <si>
-    <t>Verified by derived requirements: MS-OXCFOLD_R1177001, MS-OXCFOLD_R1177002.</t>
   </si>
   <si>
     <t>MS-OXCFOLD_R1238001</t>
@@ -7837,21 +7834,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7876,247 +7858,26 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8455,6 +8216,242 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8584,34 +8581,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1081" tableType="xml" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1081" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1081"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="60">
+    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="59">
+    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="58">
+    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="57">
+    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="56">
+    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="55">
+    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="54">
+    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="53">
+    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="52">
+    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8620,12 +8617,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="46"/>
-    <tableColumn id="2" name="Test" dataDxfId="45"/>
-    <tableColumn id="3" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8975,127 +8972,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9108,12 +9105,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9126,12 +9123,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9144,12 +9141,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9162,60 +9159,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -12368,7 +12365,7 @@
         <v>1079</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -13824,7 +13821,7 @@
         <v>1083</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -21596,7 +21593,7 @@
         <v>1118</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="D509" s="29"/>
       <c r="E509" s="29" t="s">
@@ -21612,7 +21609,7 @@
         <v>17</v>
       </c>
       <c r="I509" s="31" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
     </row>
     <row r="510" spans="1:9">
@@ -21623,7 +21620,7 @@
         <v>1118</v>
       </c>
       <c r="C510" s="20" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="D510" s="29"/>
       <c r="E510" s="29" t="s">
@@ -21667,7 +21664,7 @@
     </row>
     <row r="512" spans="1:9">
       <c r="A512" s="22" t="s">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>1119</v>
@@ -21723,7 +21720,7 @@
         <v>1119</v>
       </c>
       <c r="C514" s="35" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="D514" s="34"/>
       <c r="E514" s="29" t="s">
@@ -28307,7 +28304,7 @@
         <v>1155</v>
       </c>
       <c r="C774" s="20" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D774" s="29"/>
       <c r="E774" s="29" t="s">
@@ -28523,7 +28520,7 @@
         <v>17</v>
       </c>
       <c r="I782" s="20" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
     </row>
     <row r="783" spans="1:9" ht="45">
@@ -33353,9 +33350,7 @@
       <c r="H973" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I973" s="20" t="s">
-        <v>2378</v>
-      </c>
+      <c r="I973" s="20"/>
     </row>
     <row r="974" spans="1:9" ht="60">
       <c r="A974" s="29" t="s">
@@ -33623,7 +33618,7 @@
         <v>1166</v>
       </c>
       <c r="C984" s="20" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="D984" s="29" t="s">
         <v>2102</v>
@@ -33652,7 +33647,7 @@
         <v>1166</v>
       </c>
       <c r="C985" s="20" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D985" s="29" t="s">
         <v>2102</v>
@@ -33737,7 +33732,7 @@
         <v>1166</v>
       </c>
       <c r="C988" s="20" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="D988" s="29" t="s">
         <v>2103</v>
@@ -33766,7 +33761,7 @@
         <v>1166</v>
       </c>
       <c r="C989" s="20" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="D989" s="29" t="s">
         <v>2103</v>
@@ -33795,7 +33790,7 @@
         <v>1166</v>
       </c>
       <c r="C990" s="20" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D990" s="29" t="s">
         <v>2104</v>
@@ -33853,7 +33848,7 @@
         <v>1166</v>
       </c>
       <c r="C992" s="20" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="D992" s="29" t="s">
         <v>2105</v>
@@ -33909,7 +33904,7 @@
         <v>1166</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="D994" s="29" t="s">
         <v>2106</v>
@@ -33963,7 +33958,7 @@
         <v>1166</v>
       </c>
       <c r="C996" s="20" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="D996" s="29" t="s">
         <v>2107</v>
@@ -34019,7 +34014,7 @@
         <v>1166</v>
       </c>
       <c r="C998" s="20" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="D998" s="29" t="s">
         <v>2108</v>
@@ -34069,16 +34064,16 @@
     </row>
     <row r="1000" spans="1:9" ht="45">
       <c r="A1000" s="34" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="B1000" s="36" t="s">
         <v>1166</v>
       </c>
       <c r="C1000" s="35" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="D1000" s="34" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="E1000" s="29" t="s">
         <v>22</v>
@@ -34096,16 +34091,16 @@
     </row>
     <row r="1001" spans="1:9" ht="45">
       <c r="A1001" s="22" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="B1001" s="36" t="s">
         <v>1166</v>
       </c>
       <c r="C1001" s="20" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="D1001" s="22" t="s">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="E1001" s="29" t="s">
         <v>22</v>
@@ -34131,7 +34126,7 @@
         <v>1166</v>
       </c>
       <c r="C1002" s="20" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="D1002" s="29" t="s">
         <v>2109</v>
@@ -34270,7 +34265,7 @@
     </row>
     <row r="1007" spans="1:9" ht="45">
       <c r="A1007" s="22" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="B1007" s="36" t="s">
         <v>1166</v>
@@ -34334,7 +34329,7 @@
         <v>1166</v>
       </c>
       <c r="C1009" s="20" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D1009" s="22" t="s">
         <v>2111</v>
@@ -34357,7 +34352,7 @@
     </row>
     <row r="1010" spans="1:9" ht="60">
       <c r="A1010" s="34" t="s">
-        <v>2379</v>
+        <v>2378</v>
       </c>
       <c r="B1010" s="36" t="s">
         <v>1166</v>
@@ -34366,7 +34361,7 @@
         <v>2348</v>
       </c>
       <c r="D1010" s="34" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="E1010" s="29" t="s">
         <v>22</v>
@@ -34386,16 +34381,16 @@
     </row>
     <row r="1011" spans="1:9" ht="45">
       <c r="A1011" s="34" t="s">
-        <v>2380</v>
+        <v>2379</v>
       </c>
       <c r="B1011" s="36" t="s">
         <v>1166</v>
       </c>
       <c r="C1011" s="20" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="D1011" s="34" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="E1011" s="29" t="s">
         <v>22</v>
@@ -34678,7 +34673,7 @@
         <v>1166</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2116</v>
@@ -34766,7 +34761,7 @@
         <v>2369</v>
       </c>
       <c r="D1024" s="34" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="E1024" s="29" t="s">
         <v>22</v>
@@ -34793,7 +34788,7 @@
         <v>2367</v>
       </c>
       <c r="D1025" s="34" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
@@ -34810,7 +34805,7 @@
       <c r="I1025" s="31"/>
     </row>
     <row r="1026" spans="1:9" ht="60">
-      <c r="A1026" s="34" t="s">
+      <c r="A1026" s="22" t="s">
         <v>2376</v>
       </c>
       <c r="B1026" s="36" t="s">
@@ -34820,7 +34815,7 @@
         <v>2349</v>
       </c>
       <c r="D1026" s="34" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34832,11 +34827,9 @@
         <v>15</v>
       </c>
       <c r="H1026" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1026" s="31" t="s">
-        <v>2204</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1026" s="31"/>
     </row>
     <row r="1027" spans="1:9" ht="75">
       <c r="A1027" s="34" t="s">
@@ -34849,7 +34842,7 @@
         <v>2350</v>
       </c>
       <c r="D1027" s="34" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="E1027" s="29" t="s">
         <v>22</v>
@@ -34861,11 +34854,9 @@
         <v>15</v>
       </c>
       <c r="H1027" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1027" s="31" t="s">
-        <v>2204</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1027" s="31"/>
     </row>
     <row r="1028" spans="1:9" ht="45">
       <c r="A1028" s="22" t="s">
@@ -35162,7 +35153,7 @@
         <v>1168</v>
       </c>
       <c r="C1039" s="20" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="D1039" s="29"/>
       <c r="E1039" s="29" t="s">
@@ -36235,6 +36226,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36242,174 +36238,169 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
-    <cfRule type="expression" dxfId="43" priority="107">
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="108">
+    <cfRule type="expression" dxfId="61" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="115">
+    <cfRule type="expression" dxfId="60" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
-    <cfRule type="expression" dxfId="40" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="62">
+    <cfRule type="expression" dxfId="58" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="63">
+    <cfRule type="expression" dxfId="57" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F246 F1032:F1081 F20:F241 F251:F518 F521:F1029">
-    <cfRule type="expression" dxfId="37" priority="67">
+    <cfRule type="expression" dxfId="56" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="68">
+    <cfRule type="expression" dxfId="55" priority="68">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1032:I1081 I230 I233:I241">
-    <cfRule type="expression" dxfId="35" priority="58">
+    <cfRule type="expression" dxfId="54" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="59">
+    <cfRule type="expression" dxfId="53" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="60">
+    <cfRule type="expression" dxfId="52" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1032:I1081 I230 I233:I241">
-    <cfRule type="expression" dxfId="32" priority="55">
+    <cfRule type="expression" dxfId="51" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="56">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="57">
+    <cfRule type="expression" dxfId="49" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1031">
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="48" priority="38">
       <formula>NOT(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="47" priority="39">
       <formula>(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1031">
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="46" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="33">
+    <cfRule type="expression" dxfId="45" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1031">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="43" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="42" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="41" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1030 C1030:I1030">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="27">
+    <cfRule type="expression" dxfId="39" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="28">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1030 C1030:I1030">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1030">
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>NOT(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1030">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1030">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F519:F520">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
[MS-OXCFOLD]: Fix watchman issue
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -7443,9 +7443,6 @@
     <t>MS-OXCFOLD_R1238002</t>
   </si>
   <si>
-    <t xml:space="preserve">MS-OXCFOLD_R1238:i, MS-OXCFOLD_R113:i </t>
-  </si>
-  <si>
     <t>MS-OXCFOLD_R1177:i, MS-OXCFOLD_R113:i</t>
   </si>
   <si>
@@ -7540,6 +7537,9 @@
   </si>
   <si>
     <t>MS-OXCFOLD_R10349:i</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MS-OXCFOLD_R1238:i, MS-OXCFOLD_R114:i </t>
   </si>
 </sst>
 </file>
@@ -7834,6 +7834,21 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7857,21 +7872,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8704,6 +8704,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8739,6 +8756,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8972,127 +9006,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="39"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="46" t="s">
+      <c r="B8" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="46"/>
-      <c r="G8" s="46"/>
-      <c r="H8" s="46"/>
-      <c r="I8" s="46"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="41" t="s">
+      <c r="B9" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
+      <c r="C9" s="47"/>
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="47"/>
+      <c r="G9" s="47"/>
+      <c r="H9" s="47"/>
+      <c r="I9" s="47"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="41" t="s">
+      <c r="B10" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="47"/>
+      <c r="G10" s="47"/>
+      <c r="H10" s="47"/>
+      <c r="I10" s="47"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
-      <c r="I11" s="37"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9105,12 +9139,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="38"/>
-      <c r="G12" s="38"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="43"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9123,12 +9157,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
+      <c r="D13" s="44"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
+      <c r="H13" s="44"/>
+      <c r="I13" s="44"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9141,12 +9175,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="39"/>
-      <c r="E14" s="39"/>
-      <c r="F14" s="39"/>
-      <c r="G14" s="39"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="44"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9159,60 +9193,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
-      <c r="H15" s="40"/>
-      <c r="I15" s="40"/>
+      <c r="D15" s="45"/>
+      <c r="E15" s="45"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="37"/>
-      <c r="E16" s="37"/>
-      <c r="F16" s="37"/>
-      <c r="G16" s="37"/>
-      <c r="H16" s="37"/>
-      <c r="I16" s="37"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="42"/>
+      <c r="H16" s="42"/>
+      <c r="I16" s="42"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="44"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
+      <c r="C17" s="49"/>
+      <c r="D17" s="49"/>
+      <c r="E17" s="49"/>
+      <c r="F17" s="49"/>
+      <c r="G17" s="49"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="42"/>
+      <c r="H18" s="42"/>
+      <c r="I18" s="42"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -12365,7 +12399,7 @@
         <v>1079</v>
       </c>
       <c r="C143" s="20" t="s">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="D143" s="29"/>
       <c r="E143" s="29" t="s">
@@ -13821,7 +13855,7 @@
         <v>1083</v>
       </c>
       <c r="C201" s="20" t="s">
-        <v>2398</v>
+        <v>2397</v>
       </c>
       <c r="D201" s="29"/>
       <c r="E201" s="29" t="s">
@@ -21593,7 +21627,7 @@
         <v>1118</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="D509" s="29"/>
       <c r="E509" s="29" t="s">
@@ -21609,7 +21643,7 @@
         <v>17</v>
       </c>
       <c r="I509" s="31" t="s">
-        <v>2407</v>
+        <v>2406</v>
       </c>
     </row>
     <row r="510" spans="1:9">
@@ -21620,7 +21654,7 @@
         <v>1118</v>
       </c>
       <c r="C510" s="20" t="s">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="D510" s="29"/>
       <c r="E510" s="29" t="s">
@@ -21664,7 +21698,7 @@
     </row>
     <row r="512" spans="1:9">
       <c r="A512" s="22" t="s">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="B512" s="30" t="s">
         <v>1119</v>
@@ -21720,7 +21754,7 @@
         <v>1119</v>
       </c>
       <c r="C514" s="35" t="s">
-        <v>2401</v>
+        <v>2400</v>
       </c>
       <c r="D514" s="34"/>
       <c r="E514" s="29" t="s">
@@ -21733,7 +21767,7 @@
         <v>15</v>
       </c>
       <c r="H514" s="34" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I514" s="35"/>
     </row>
@@ -27690,7 +27724,7 @@
         <v>15</v>
       </c>
       <c r="H749" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I749" s="31"/>
     </row>
@@ -28304,7 +28338,7 @@
         <v>1155</v>
       </c>
       <c r="C774" s="20" t="s">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="D774" s="29"/>
       <c r="E774" s="29" t="s">
@@ -28520,7 +28554,7 @@
         <v>17</v>
       </c>
       <c r="I782" s="20" t="s">
-        <v>2383</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="783" spans="1:9" ht="45">
@@ -33223,7 +33257,7 @@
         <v>15</v>
       </c>
       <c r="H968" s="22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I968" s="31"/>
     </row>
@@ -33618,7 +33652,7 @@
         <v>1166</v>
       </c>
       <c r="C984" s="20" t="s">
-        <v>2402</v>
+        <v>2401</v>
       </c>
       <c r="D984" s="29" t="s">
         <v>2102</v>
@@ -33647,7 +33681,7 @@
         <v>1166</v>
       </c>
       <c r="C985" s="20" t="s">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="D985" s="29" t="s">
         <v>2102</v>
@@ -33732,7 +33766,7 @@
         <v>1166</v>
       </c>
       <c r="C988" s="20" t="s">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="D988" s="29" t="s">
         <v>2103</v>
@@ -33761,7 +33795,7 @@
         <v>1166</v>
       </c>
       <c r="C989" s="20" t="s">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="D989" s="29" t="s">
         <v>2103</v>
@@ -33790,7 +33824,7 @@
         <v>1166</v>
       </c>
       <c r="C990" s="20" t="s">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="D990" s="29" t="s">
         <v>2104</v>
@@ -33848,7 +33882,7 @@
         <v>1166</v>
       </c>
       <c r="C992" s="20" t="s">
-        <v>2389</v>
+        <v>2388</v>
       </c>
       <c r="D992" s="29" t="s">
         <v>2105</v>
@@ -33904,7 +33938,7 @@
         <v>1166</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2388</v>
+        <v>2387</v>
       </c>
       <c r="D994" s="29" t="s">
         <v>2106</v>
@@ -33958,7 +33992,7 @@
         <v>1166</v>
       </c>
       <c r="C996" s="20" t="s">
-        <v>2390</v>
+        <v>2389</v>
       </c>
       <c r="D996" s="29" t="s">
         <v>2107</v>
@@ -34014,7 +34048,7 @@
         <v>1166</v>
       </c>
       <c r="C998" s="20" t="s">
-        <v>2391</v>
+        <v>2390</v>
       </c>
       <c r="D998" s="29" t="s">
         <v>2108</v>
@@ -34064,16 +34098,16 @@
     </row>
     <row r="1000" spans="1:9" ht="45">
       <c r="A1000" s="34" t="s">
-        <v>2384</v>
+        <v>2383</v>
       </c>
       <c r="B1000" s="36" t="s">
         <v>1166</v>
       </c>
       <c r="C1000" s="35" t="s">
-        <v>2387</v>
+        <v>2386</v>
       </c>
       <c r="D1000" s="34" t="s">
-        <v>2386</v>
+        <v>2385</v>
       </c>
       <c r="E1000" s="29" t="s">
         <v>22</v>
@@ -34091,16 +34125,16 @@
     </row>
     <row r="1001" spans="1:9" ht="45">
       <c r="A1001" s="22" t="s">
-        <v>2385</v>
+        <v>2384</v>
       </c>
       <c r="B1001" s="36" t="s">
         <v>1166</v>
       </c>
       <c r="C1001" s="20" t="s">
-        <v>2403</v>
+        <v>2402</v>
       </c>
       <c r="D1001" s="22" t="s">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="E1001" s="29" t="s">
         <v>22</v>
@@ -34126,7 +34160,7 @@
         <v>1166</v>
       </c>
       <c r="C1002" s="20" t="s">
-        <v>2404</v>
+        <v>2403</v>
       </c>
       <c r="D1002" s="29" t="s">
         <v>2109</v>
@@ -34135,7 +34169,7 @@
         <v>22</v>
       </c>
       <c r="F1002" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1002" s="29" t="s">
         <v>15</v>
@@ -34164,7 +34198,7 @@
         <v>22</v>
       </c>
       <c r="F1003" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1003" s="29" t="s">
         <v>15</v>
@@ -34193,7 +34227,7 @@
         <v>22</v>
       </c>
       <c r="F1004" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1004" s="29" t="s">
         <v>15</v>
@@ -34222,7 +34256,7 @@
         <v>22</v>
       </c>
       <c r="F1005" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1005" s="29" t="s">
         <v>15</v>
@@ -34251,7 +34285,7 @@
         <v>22</v>
       </c>
       <c r="F1006" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1006" s="29" t="s">
         <v>15</v>
@@ -34265,7 +34299,7 @@
     </row>
     <row r="1007" spans="1:9" ht="45">
       <c r="A1007" s="22" t="s">
-        <v>2400</v>
+        <v>2399</v>
       </c>
       <c r="B1007" s="36" t="s">
         <v>1166</v>
@@ -34280,7 +34314,7 @@
         <v>22</v>
       </c>
       <c r="F1007" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1007" s="29" t="s">
         <v>15</v>
@@ -34309,7 +34343,7 @@
         <v>22</v>
       </c>
       <c r="F1008" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1008" s="29" t="s">
         <v>15</v>
@@ -34329,7 +34363,7 @@
         <v>1166</v>
       </c>
       <c r="C1009" s="20" t="s">
-        <v>2405</v>
+        <v>2404</v>
       </c>
       <c r="D1009" s="22" t="s">
         <v>2111</v>
@@ -34360,14 +34394,14 @@
       <c r="C1010" s="35" t="s">
         <v>2348</v>
       </c>
-      <c r="D1010" s="34" t="s">
-        <v>2380</v>
+      <c r="D1010" s="22" t="s">
+        <v>2412</v>
       </c>
       <c r="E1010" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1010" s="34" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1010" s="34" t="s">
         <v>15</v>
@@ -34387,16 +34421,16 @@
         <v>1166</v>
       </c>
       <c r="C1011" s="20" t="s">
-        <v>2409</v>
-      </c>
-      <c r="D1011" s="34" t="s">
-        <v>2380</v>
+        <v>2408</v>
+      </c>
+      <c r="D1011" s="22" t="s">
+        <v>2412</v>
       </c>
       <c r="E1011" s="29" t="s">
         <v>22</v>
       </c>
       <c r="F1011" s="34" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1011" s="34" t="s">
         <v>15</v>
@@ -34425,7 +34459,7 @@
         <v>22</v>
       </c>
       <c r="F1012" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1012" s="29" t="s">
         <v>15</v>
@@ -34454,7 +34488,7 @@
         <v>22</v>
       </c>
       <c r="F1013" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1013" s="29" t="s">
         <v>15</v>
@@ -34568,7 +34602,7 @@
         <v>22</v>
       </c>
       <c r="F1017" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1017" s="29" t="s">
         <v>15</v>
@@ -34597,7 +34631,7 @@
         <v>22</v>
       </c>
       <c r="F1018" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1018" s="29" t="s">
         <v>15</v>
@@ -34626,7 +34660,7 @@
         <v>22</v>
       </c>
       <c r="F1019" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1019" s="29" t="s">
         <v>15</v>
@@ -34653,7 +34687,7 @@
         <v>22</v>
       </c>
       <c r="F1020" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1020" s="29" t="s">
         <v>15</v>
@@ -34673,7 +34707,7 @@
         <v>1166</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2116</v>
@@ -34682,7 +34716,7 @@
         <v>22</v>
       </c>
       <c r="F1021" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1021" s="29" t="s">
         <v>15</v>
@@ -34711,7 +34745,7 @@
         <v>22</v>
       </c>
       <c r="F1022" s="22" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1022" s="29" t="s">
         <v>15</v>
@@ -34761,7 +34795,7 @@
         <v>2369</v>
       </c>
       <c r="D1024" s="34" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="E1024" s="29" t="s">
         <v>22</v>
@@ -34788,7 +34822,7 @@
         <v>2367</v>
       </c>
       <c r="D1025" s="34" t="s">
-        <v>2382</v>
+        <v>2381</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
@@ -34815,7 +34849,7 @@
         <v>2349</v>
       </c>
       <c r="D1026" s="34" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34842,7 +34876,7 @@
         <v>2350</v>
       </c>
       <c r="D1027" s="34" t="s">
-        <v>2381</v>
+        <v>2380</v>
       </c>
       <c r="E1027" s="29" t="s">
         <v>22</v>
@@ -34977,7 +35011,7 @@
       <c r="B1032" s="30" t="s">
         <v>1070</v>
       </c>
-      <c r="C1032" s="31" t="s">
+      <c r="C1032" s="20" t="s">
         <v>2047</v>
       </c>
       <c r="D1032" s="29"/>
@@ -35002,7 +35036,7 @@
       <c r="B1033" s="30" t="s">
         <v>1167</v>
       </c>
-      <c r="C1033" s="31" t="s">
+      <c r="C1033" s="20" t="s">
         <v>2048</v>
       </c>
       <c r="D1033" s="29"/>
@@ -35027,7 +35061,7 @@
       <c r="B1034" s="30" t="s">
         <v>1167</v>
       </c>
-      <c r="C1034" s="31" t="s">
+      <c r="C1034" s="20" t="s">
         <v>2049</v>
       </c>
       <c r="D1034" s="29"/>
@@ -35153,7 +35187,7 @@
         <v>1168</v>
       </c>
       <c r="C1039" s="20" t="s">
-        <v>2399</v>
+        <v>2398</v>
       </c>
       <c r="D1039" s="29"/>
       <c r="E1039" s="29" t="s">
@@ -36226,11 +36260,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36238,6 +36267,11 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">

</xml_diff>

<commit_message>
[MS-OXCFOLD] Update rs file
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17030"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
@@ -7547,14 +7547,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="165" formatCode="0.0.0"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="0.0.0"/>
   </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -7763,13 +7763,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="176" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -7802,7 +7802,7 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -7834,21 +7834,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7872,6 +7857,21 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -8956,15 +8956,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
-    <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="28.625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="12.125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="13.375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
-    <col min="9" max="9" width="28.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="28.75" style="3" customWidth="1"/>
     <col min="10" max="10" width="9" style="3" customWidth="1"/>
     <col min="11" max="16384" width="9" style="3"/>
   </cols>
@@ -9006,127 +9006,127 @@
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="40" t="s">
+      <c r="B5" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="38" t="s">
+      <c r="B7" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="46"/>
+      <c r="G7" s="46"/>
+      <c r="H7" s="46"/>
+      <c r="I7" s="46"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="38" t="s">
+      <c r="B8" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="38"/>
-      <c r="D8" s="38"/>
-      <c r="E8" s="38"/>
-      <c r="F8" s="38"/>
-      <c r="G8" s="38"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="47"/>
-      <c r="D9" s="47"/>
-      <c r="E9" s="47"/>
-      <c r="F9" s="47"/>
-      <c r="G9" s="47"/>
-      <c r="H9" s="47"/>
-      <c r="I9" s="47"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="46" t="s">
+      <c r="B10" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="47"/>
-      <c r="D10" s="47"/>
-      <c r="E10" s="47"/>
-      <c r="F10" s="47"/>
-      <c r="G10" s="47"/>
-      <c r="H10" s="47"/>
-      <c r="I10" s="47"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="37"/>
+      <c r="G11" s="37"/>
+      <c r="H11" s="37"/>
+      <c r="I11" s="37"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9139,12 +9139,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="43"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="43"/>
-      <c r="G12" s="43"/>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9157,12 +9157,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
+      <c r="D13" s="39"/>
+      <c r="E13" s="39"/>
+      <c r="F13" s="39"/>
+      <c r="G13" s="39"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9175,12 +9175,12 @@
       <c r="C14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10">
@@ -9193,60 +9193,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="45"/>
-      <c r="E15" s="45"/>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45"/>
-      <c r="H15" s="45"/>
-      <c r="I15" s="45"/>
+      <c r="D15" s="40"/>
+      <c r="E15" s="40"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="40"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="37"/>
+      <c r="F16" s="37"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="44"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="37"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -9380,7 +9380,7 @@
       </c>
       <c r="I23" s="24"/>
     </row>
-    <row r="24" spans="1:12" s="23" customFormat="1" ht="60">
+    <row r="24" spans="1:12" s="23" customFormat="1" ht="45">
       <c r="A24" s="22" t="s">
         <v>47</v>
       </c>
@@ -9430,7 +9430,7 @@
       </c>
       <c r="I25" s="24"/>
     </row>
-    <row r="26" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="26" spans="1:12" s="23" customFormat="1">
       <c r="A26" s="22" t="s">
         <v>49</v>
       </c>
@@ -9455,7 +9455,7 @@
       </c>
       <c r="I26" s="24"/>
     </row>
-    <row r="27" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="27" spans="1:12" s="23" customFormat="1">
       <c r="A27" s="22" t="s">
         <v>50</v>
       </c>
@@ -9480,7 +9480,7 @@
       </c>
       <c r="I27" s="24"/>
     </row>
-    <row r="28" spans="1:12" s="23" customFormat="1" ht="30">
+    <row r="28" spans="1:12" s="23" customFormat="1">
       <c r="A28" s="22" t="s">
         <v>51</v>
       </c>
@@ -9580,7 +9580,7 @@
       </c>
       <c r="I31" s="24"/>
     </row>
-    <row r="32" spans="1:12" s="23" customFormat="1" ht="45">
+    <row r="32" spans="1:12" s="23" customFormat="1" ht="30">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -9680,7 +9680,7 @@
       </c>
       <c r="I35" s="31"/>
     </row>
-    <row r="36" spans="1:9" ht="45">
+    <row r="36" spans="1:9" ht="30">
       <c r="A36" s="29" t="s">
         <v>59</v>
       </c>
@@ -9705,7 +9705,7 @@
       </c>
       <c r="I36" s="31"/>
     </row>
-    <row r="37" spans="1:9" ht="45">
+    <row r="37" spans="1:9" ht="30">
       <c r="A37" s="29" t="s">
         <v>60</v>
       </c>
@@ -9859,7 +9859,7 @@
         <v>2119</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9">
       <c r="A43" s="29" t="s">
         <v>66</v>
       </c>
@@ -9884,7 +9884,7 @@
       </c>
       <c r="I43" s="31"/>
     </row>
-    <row r="44" spans="1:9" ht="75">
+    <row r="44" spans="1:9" ht="60">
       <c r="A44" s="29" t="s">
         <v>67</v>
       </c>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="I46" s="31"/>
     </row>
-    <row r="47" spans="1:9" ht="120">
+    <row r="47" spans="1:9" ht="90">
       <c r="A47" s="29" t="s">
         <v>70</v>
       </c>
@@ -10038,7 +10038,7 @@
       </c>
       <c r="I49" s="31"/>
     </row>
-    <row r="50" spans="1:9" ht="45">
+    <row r="50" spans="1:9" ht="30">
       <c r="A50" s="29" t="s">
         <v>73</v>
       </c>
@@ -10065,7 +10065,7 @@
         <v>2122</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="60">
+    <row r="51" spans="1:9" ht="45">
       <c r="A51" s="29" t="s">
         <v>74</v>
       </c>
@@ -10117,7 +10117,7 @@
       </c>
       <c r="I52" s="31"/>
     </row>
-    <row r="53" spans="1:9" ht="30">
+    <row r="53" spans="1:9">
       <c r="A53" s="29" t="s">
         <v>76</v>
       </c>
@@ -10142,7 +10142,7 @@
       </c>
       <c r="I53" s="31"/>
     </row>
-    <row r="54" spans="1:9" ht="45">
+    <row r="54" spans="1:9" ht="30">
       <c r="A54" s="29" t="s">
         <v>77</v>
       </c>
@@ -10444,7 +10444,7 @@
       </c>
       <c r="I65" s="31"/>
     </row>
-    <row r="66" spans="1:9" ht="30">
+    <row r="66" spans="1:9">
       <c r="A66" s="29" t="s">
         <v>89</v>
       </c>
@@ -10469,7 +10469,7 @@
       </c>
       <c r="I66" s="31"/>
     </row>
-    <row r="67" spans="1:9" ht="30">
+    <row r="67" spans="1:9">
       <c r="A67" s="29" t="s">
         <v>90</v>
       </c>
@@ -10494,7 +10494,7 @@
       </c>
       <c r="I67" s="31"/>
     </row>
-    <row r="68" spans="1:9" ht="30">
+    <row r="68" spans="1:9">
       <c r="A68" s="29" t="s">
         <v>91</v>
       </c>
@@ -10594,7 +10594,7 @@
       </c>
       <c r="I71" s="31"/>
     </row>
-    <row r="72" spans="1:9" ht="45">
+    <row r="72" spans="1:9" ht="30">
       <c r="A72" s="29" t="s">
         <v>95</v>
       </c>
@@ -10644,7 +10644,7 @@
       </c>
       <c r="I73" s="31"/>
     </row>
-    <row r="74" spans="1:9" ht="45">
+    <row r="74" spans="1:9" ht="30">
       <c r="A74" s="29" t="s">
         <v>97</v>
       </c>
@@ -10794,7 +10794,7 @@
       </c>
       <c r="I79" s="31"/>
     </row>
-    <row r="80" spans="1:9" ht="45">
+    <row r="80" spans="1:9" ht="30">
       <c r="A80" s="29" t="s">
         <v>103</v>
       </c>
@@ -10819,7 +10819,7 @@
       </c>
       <c r="I80" s="31"/>
     </row>
-    <row r="81" spans="1:9" ht="45">
+    <row r="81" spans="1:9" ht="30">
       <c r="A81" s="29" t="s">
         <v>104</v>
       </c>
@@ -10844,7 +10844,7 @@
       </c>
       <c r="I81" s="31"/>
     </row>
-    <row r="82" spans="1:9" ht="45">
+    <row r="82" spans="1:9" ht="30">
       <c r="A82" s="29" t="s">
         <v>105</v>
       </c>
@@ -11069,7 +11069,7 @@
       </c>
       <c r="I90" s="31"/>
     </row>
-    <row r="91" spans="1:9" ht="210">
+    <row r="91" spans="1:9" ht="165">
       <c r="A91" s="29" t="s">
         <v>114</v>
       </c>
@@ -11173,7 +11173,7 @@
         <v>2118</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="60">
+    <row r="95" spans="1:9" ht="45">
       <c r="A95" s="29" t="s">
         <v>118</v>
       </c>
@@ -11277,7 +11277,7 @@
       </c>
       <c r="I98" s="31"/>
     </row>
-    <row r="99" spans="1:9" ht="45">
+    <row r="99" spans="1:9" ht="30">
       <c r="A99" s="29" t="s">
         <v>122</v>
       </c>
@@ -11404,7 +11404,7 @@
       </c>
       <c r="I103" s="31"/>
     </row>
-    <row r="104" spans="1:9" ht="45">
+    <row r="104" spans="1:9" ht="30">
       <c r="A104" s="29" t="s">
         <v>127</v>
       </c>
@@ -11431,7 +11431,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="30">
+    <row r="105" spans="1:9">
       <c r="A105" s="29" t="s">
         <v>128</v>
       </c>
@@ -11506,7 +11506,7 @@
       </c>
       <c r="I107" s="31"/>
     </row>
-    <row r="108" spans="1:9" ht="45">
+    <row r="108" spans="1:9" ht="30">
       <c r="A108" s="29" t="s">
         <v>131</v>
       </c>
@@ -11781,7 +11781,7 @@
       </c>
       <c r="I118" s="31"/>
     </row>
-    <row r="119" spans="1:9" ht="30">
+    <row r="119" spans="1:9">
       <c r="A119" s="29" t="s">
         <v>142</v>
       </c>
@@ -11806,7 +11806,7 @@
       </c>
       <c r="I119" s="31"/>
     </row>
-    <row r="120" spans="1:9" ht="30">
+    <row r="120" spans="1:9">
       <c r="A120" s="29" t="s">
         <v>143</v>
       </c>
@@ -11831,7 +11831,7 @@
       </c>
       <c r="I120" s="31"/>
     </row>
-    <row r="121" spans="1:9" ht="30">
+    <row r="121" spans="1:9">
       <c r="A121" s="29" t="s">
         <v>144</v>
       </c>
@@ -11856,7 +11856,7 @@
       </c>
       <c r="I121" s="31"/>
     </row>
-    <row r="122" spans="1:9" ht="30">
+    <row r="122" spans="1:9">
       <c r="A122" s="29" t="s">
         <v>145</v>
       </c>
@@ -11931,7 +11931,7 @@
       </c>
       <c r="I124" s="31"/>
     </row>
-    <row r="125" spans="1:9" ht="45">
+    <row r="125" spans="1:9" ht="30">
       <c r="A125" s="29" t="s">
         <v>148</v>
       </c>
@@ -11956,7 +11956,7 @@
       </c>
       <c r="I125" s="31"/>
     </row>
-    <row r="126" spans="1:9" ht="45">
+    <row r="126" spans="1:9" ht="30">
       <c r="A126" s="29" t="s">
         <v>149</v>
       </c>
@@ -11981,7 +11981,7 @@
       </c>
       <c r="I126" s="31"/>
     </row>
-    <row r="127" spans="1:9" ht="105">
+    <row r="127" spans="1:9" ht="75">
       <c r="A127" s="29" t="s">
         <v>150</v>
       </c>
@@ -12008,7 +12008,7 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="60">
+    <row r="128" spans="1:9" ht="45">
       <c r="A128" s="29" t="s">
         <v>151</v>
       </c>
@@ -12237,7 +12237,7 @@
       </c>
       <c r="I136" s="31"/>
     </row>
-    <row r="137" spans="1:9" ht="165">
+    <row r="137" spans="1:9" ht="120">
       <c r="A137" s="29" t="s">
         <v>160</v>
       </c>
@@ -12314,7 +12314,7 @@
       </c>
       <c r="I139" s="31"/>
     </row>
-    <row r="140" spans="1:9" ht="45">
+    <row r="140" spans="1:9" ht="30">
       <c r="A140" s="29" t="s">
         <v>163</v>
       </c>
@@ -12491,7 +12491,7 @@
       </c>
       <c r="I146" s="31"/>
     </row>
-    <row r="147" spans="1:9" ht="45">
+    <row r="147" spans="1:9" ht="30">
       <c r="A147" s="29" t="s">
         <v>170</v>
       </c>
@@ -12891,7 +12891,7 @@
       </c>
       <c r="I162" s="31"/>
     </row>
-    <row r="163" spans="1:9" ht="30">
+    <row r="163" spans="1:9">
       <c r="A163" s="29" t="s">
         <v>186</v>
       </c>
@@ -12991,7 +12991,7 @@
       </c>
       <c r="I166" s="20"/>
     </row>
-    <row r="167" spans="1:9" ht="45">
+    <row r="167" spans="1:9" ht="30">
       <c r="A167" s="29" t="s">
         <v>190</v>
       </c>
@@ -13066,7 +13066,7 @@
       </c>
       <c r="I169" s="31"/>
     </row>
-    <row r="170" spans="1:9" ht="45">
+    <row r="170" spans="1:9" ht="30">
       <c r="A170" s="29" t="s">
         <v>193</v>
       </c>
@@ -13118,7 +13118,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="172" spans="1:9" ht="45">
+    <row r="172" spans="1:9" ht="30">
       <c r="A172" s="29" t="s">
         <v>195</v>
       </c>
@@ -13143,7 +13143,7 @@
       </c>
       <c r="I172" s="31"/>
     </row>
-    <row r="173" spans="1:9" ht="45">
+    <row r="173" spans="1:9" ht="30">
       <c r="A173" s="29" t="s">
         <v>196</v>
       </c>
@@ -13193,7 +13193,7 @@
       </c>
       <c r="I174" s="31"/>
     </row>
-    <row r="175" spans="1:9" ht="45">
+    <row r="175" spans="1:9" ht="30">
       <c r="A175" s="29" t="s">
         <v>198</v>
       </c>
@@ -13218,7 +13218,7 @@
       </c>
       <c r="I175" s="31"/>
     </row>
-    <row r="176" spans="1:9" ht="45">
+    <row r="176" spans="1:9" ht="30">
       <c r="A176" s="29" t="s">
         <v>199</v>
       </c>
@@ -13270,7 +13270,7 @@
         <v>2134</v>
       </c>
     </row>
-    <row r="178" spans="1:9" ht="45">
+    <row r="178" spans="1:9" ht="30">
       <c r="A178" s="29" t="s">
         <v>201</v>
       </c>
@@ -13295,7 +13295,7 @@
       </c>
       <c r="I178" s="31"/>
     </row>
-    <row r="179" spans="1:9" ht="45">
+    <row r="179" spans="1:9" ht="30">
       <c r="A179" s="29" t="s">
         <v>202</v>
       </c>
@@ -13370,7 +13370,7 @@
       </c>
       <c r="I181" s="31"/>
     </row>
-    <row r="182" spans="1:9" ht="45">
+    <row r="182" spans="1:9" ht="30">
       <c r="A182" s="29" t="s">
         <v>205</v>
       </c>
@@ -13545,7 +13545,7 @@
       </c>
       <c r="I188" s="31"/>
     </row>
-    <row r="189" spans="1:9" ht="195">
+    <row r="189" spans="1:9" ht="165">
       <c r="A189" s="29" t="s">
         <v>212</v>
       </c>
@@ -13647,7 +13647,7 @@
       </c>
       <c r="I192" s="31"/>
     </row>
-    <row r="193" spans="1:9" ht="30">
+    <row r="193" spans="1:9">
       <c r="A193" s="29" t="s">
         <v>216</v>
       </c>
@@ -13747,7 +13747,7 @@
       </c>
       <c r="I196" s="31"/>
     </row>
-    <row r="197" spans="1:9" ht="45">
+    <row r="197" spans="1:9" ht="30">
       <c r="A197" s="29" t="s">
         <v>220</v>
       </c>
@@ -13797,7 +13797,7 @@
       </c>
       <c r="I198" s="31"/>
     </row>
-    <row r="199" spans="1:9" ht="45">
+    <row r="199" spans="1:9" ht="30">
       <c r="A199" s="29" t="s">
         <v>222</v>
       </c>
@@ -13822,7 +13822,7 @@
       </c>
       <c r="I199" s="31"/>
     </row>
-    <row r="200" spans="1:9" ht="45">
+    <row r="200" spans="1:9" ht="30">
       <c r="A200" s="29" t="s">
         <v>223</v>
       </c>
@@ -13922,7 +13922,7 @@
       </c>
       <c r="I203" s="31"/>
     </row>
-    <row r="204" spans="1:9" ht="45">
+    <row r="204" spans="1:9" ht="30">
       <c r="A204" s="29" t="s">
         <v>227</v>
       </c>
@@ -13972,7 +13972,7 @@
       </c>
       <c r="I205" s="31"/>
     </row>
-    <row r="206" spans="1:9" ht="90">
+    <row r="206" spans="1:9" ht="60">
       <c r="A206" s="29" t="s">
         <v>229</v>
       </c>
@@ -14099,7 +14099,7 @@
       </c>
       <c r="I210" s="31"/>
     </row>
-    <row r="211" spans="1:9" ht="45">
+    <row r="211" spans="1:9" ht="30">
       <c r="A211" s="29" t="s">
         <v>234</v>
       </c>
@@ -14226,7 +14226,7 @@
       </c>
       <c r="I215" s="31"/>
     </row>
-    <row r="216" spans="1:9" ht="45">
+    <row r="216" spans="1:9" ht="30">
       <c r="A216" s="29" t="s">
         <v>239</v>
       </c>
@@ -14251,7 +14251,7 @@
       </c>
       <c r="I216" s="31"/>
     </row>
-    <row r="217" spans="1:9" ht="45">
+    <row r="217" spans="1:9" ht="30">
       <c r="A217" s="29" t="s">
         <v>240</v>
       </c>
@@ -14326,7 +14326,7 @@
       </c>
       <c r="I219" s="31"/>
     </row>
-    <row r="220" spans="1:9" ht="180">
+    <row r="220" spans="1:9" ht="135">
       <c r="A220" s="29" t="s">
         <v>243</v>
       </c>
@@ -14353,7 +14353,7 @@
         <v>2138</v>
       </c>
     </row>
-    <row r="221" spans="1:9" ht="60">
+    <row r="221" spans="1:9" ht="45">
       <c r="A221" s="29" t="s">
         <v>244</v>
       </c>
@@ -14403,7 +14403,7 @@
       </c>
       <c r="I222" s="31"/>
     </row>
-    <row r="223" spans="1:9" ht="45">
+    <row r="223" spans="1:9" ht="30">
       <c r="A223" s="29" t="s">
         <v>246</v>
       </c>
@@ -14703,7 +14703,7 @@
       </c>
       <c r="I234" s="31"/>
     </row>
-    <row r="235" spans="1:9" ht="30">
+    <row r="235" spans="1:9">
       <c r="A235" s="29" t="s">
         <v>258</v>
       </c>
@@ -14728,7 +14728,7 @@
       </c>
       <c r="I235" s="31"/>
     </row>
-    <row r="236" spans="1:9" ht="30">
+    <row r="236" spans="1:9">
       <c r="A236" s="29" t="s">
         <v>259</v>
       </c>
@@ -14753,7 +14753,7 @@
       </c>
       <c r="I236" s="31"/>
     </row>
-    <row r="237" spans="1:9" ht="30">
+    <row r="237" spans="1:9">
       <c r="A237" s="29" t="s">
         <v>260</v>
       </c>
@@ -14853,7 +14853,7 @@
       </c>
       <c r="I240" s="31"/>
     </row>
-    <row r="241" spans="1:10" ht="45">
+    <row r="241" spans="1:10" ht="30">
       <c r="A241" s="29" t="s">
         <v>264</v>
       </c>
@@ -14930,7 +14930,7 @@
       <c r="I243" s="20"/>
       <c r="J243" s="20"/>
     </row>
-    <row r="244" spans="1:10" ht="60">
+    <row r="244" spans="1:10" ht="45">
       <c r="A244" s="22" t="s">
         <v>2216</v>
       </c>
@@ -14956,7 +14956,7 @@
       <c r="I244" s="20"/>
       <c r="J244" s="20"/>
     </row>
-    <row r="245" spans="1:10" ht="60">
+    <row r="245" spans="1:10" ht="45">
       <c r="A245" s="22" t="s">
         <v>2217</v>
       </c>
@@ -14982,7 +14982,7 @@
       <c r="I245" s="20"/>
       <c r="J245" s="20"/>
     </row>
-    <row r="246" spans="1:10" ht="45">
+    <row r="246" spans="1:10" ht="30">
       <c r="A246" s="29" t="s">
         <v>265</v>
       </c>
@@ -15059,7 +15059,7 @@
       <c r="I248" s="20"/>
       <c r="J248" s="20"/>
     </row>
-    <row r="249" spans="1:10" ht="60">
+    <row r="249" spans="1:10" ht="45">
       <c r="A249" s="22" t="s">
         <v>2253</v>
       </c>
@@ -15085,7 +15085,7 @@
       <c r="I249" s="20"/>
       <c r="J249" s="20"/>
     </row>
-    <row r="250" spans="1:10" ht="60">
+    <row r="250" spans="1:10" ht="45">
       <c r="A250" s="22" t="s">
         <v>2218</v>
       </c>
@@ -15136,7 +15136,7 @@
       </c>
       <c r="I251" s="31"/>
     </row>
-    <row r="252" spans="1:10" ht="45">
+    <row r="252" spans="1:10" ht="30">
       <c r="A252" s="29" t="s">
         <v>267</v>
       </c>
@@ -15311,7 +15311,7 @@
       </c>
       <c r="I258" s="31"/>
     </row>
-    <row r="259" spans="1:9" ht="45">
+    <row r="259" spans="1:9" ht="30">
       <c r="A259" s="29" t="s">
         <v>274</v>
       </c>
@@ -15336,7 +15336,7 @@
       </c>
       <c r="I259" s="31"/>
     </row>
-    <row r="260" spans="1:9" ht="90">
+    <row r="260" spans="1:9" ht="75">
       <c r="A260" s="29" t="s">
         <v>275</v>
       </c>
@@ -15690,7 +15690,7 @@
       </c>
       <c r="I273" s="31"/>
     </row>
-    <row r="274" spans="1:9" ht="45">
+    <row r="274" spans="1:9" ht="30">
       <c r="A274" s="29" t="s">
         <v>289</v>
       </c>
@@ -15740,7 +15740,7 @@
       </c>
       <c r="I275" s="31"/>
     </row>
-    <row r="276" spans="1:9" ht="45">
+    <row r="276" spans="1:9" ht="30">
       <c r="A276" s="29" t="s">
         <v>291</v>
       </c>
@@ -15990,7 +15990,7 @@
       </c>
       <c r="I285" s="31"/>
     </row>
-    <row r="286" spans="1:9" ht="90">
+    <row r="286" spans="1:9" ht="60">
       <c r="A286" s="29" t="s">
         <v>301</v>
       </c>
@@ -16119,7 +16119,7 @@
       </c>
       <c r="I290" s="31"/>
     </row>
-    <row r="291" spans="1:9" ht="45">
+    <row r="291" spans="1:9" ht="30">
       <c r="A291" s="29" t="s">
         <v>306</v>
       </c>
@@ -16219,7 +16219,7 @@
       </c>
       <c r="I294" s="31"/>
     </row>
-    <row r="295" spans="1:9" ht="45">
+    <row r="295" spans="1:9" ht="30">
       <c r="A295" s="29" t="s">
         <v>310</v>
       </c>
@@ -16348,7 +16348,7 @@
       </c>
       <c r="I299" s="31"/>
     </row>
-    <row r="300" spans="1:9" ht="45">
+    <row r="300" spans="1:9" ht="30">
       <c r="A300" s="29" t="s">
         <v>315</v>
       </c>
@@ -16398,7 +16398,7 @@
       </c>
       <c r="I301" s="31"/>
     </row>
-    <row r="302" spans="1:9" ht="45">
+    <row r="302" spans="1:9" ht="30">
       <c r="A302" s="29" t="s">
         <v>317</v>
       </c>
@@ -16523,7 +16523,7 @@
       </c>
       <c r="I306" s="31"/>
     </row>
-    <row r="307" spans="1:9" ht="60">
+    <row r="307" spans="1:9" ht="45">
       <c r="A307" s="29" t="s">
         <v>322</v>
       </c>
@@ -16548,7 +16548,7 @@
       </c>
       <c r="I307" s="31"/>
     </row>
-    <row r="308" spans="1:9" ht="60">
+    <row r="308" spans="1:9" ht="45">
       <c r="A308" s="29" t="s">
         <v>323</v>
       </c>
@@ -16700,7 +16700,7 @@
       </c>
       <c r="I313" s="31"/>
     </row>
-    <row r="314" spans="1:9" ht="90">
+    <row r="314" spans="1:9" ht="60">
       <c r="A314" s="29" t="s">
         <v>329</v>
       </c>
@@ -16906,7 +16906,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="322" spans="1:9" ht="45">
+    <row r="322" spans="1:9" ht="30">
       <c r="A322" s="29" t="s">
         <v>337</v>
       </c>
@@ -16933,7 +16933,7 @@
         <v>2148</v>
       </c>
     </row>
-    <row r="323" spans="1:9" ht="30">
+    <row r="323" spans="1:9">
       <c r="A323" s="29" t="s">
         <v>338</v>
       </c>
@@ -17033,7 +17033,7 @@
       </c>
       <c r="I326" s="31"/>
     </row>
-    <row r="327" spans="1:9" ht="30">
+    <row r="327" spans="1:9">
       <c r="A327" s="29" t="s">
         <v>342</v>
       </c>
@@ -17058,7 +17058,7 @@
       </c>
       <c r="I327" s="31"/>
     </row>
-    <row r="328" spans="1:9" ht="45">
+    <row r="328" spans="1:9" ht="30">
       <c r="A328" s="29" t="s">
         <v>343</v>
       </c>
@@ -17158,7 +17158,7 @@
       </c>
       <c r="I331" s="31"/>
     </row>
-    <row r="332" spans="1:9" ht="45">
+    <row r="332" spans="1:9" ht="30">
       <c r="A332" s="29" t="s">
         <v>347</v>
       </c>
@@ -17183,7 +17183,7 @@
       </c>
       <c r="I332" s="31"/>
     </row>
-    <row r="333" spans="1:9" ht="45">
+    <row r="333" spans="1:9" ht="30">
       <c r="A333" s="29" t="s">
         <v>348</v>
       </c>
@@ -17233,7 +17233,7 @@
       </c>
       <c r="I334" s="31"/>
     </row>
-    <row r="335" spans="1:9" ht="75">
+    <row r="335" spans="1:9" ht="60">
       <c r="A335" s="29" t="s">
         <v>350</v>
       </c>
@@ -17310,7 +17310,7 @@
       </c>
       <c r="I337" s="31"/>
     </row>
-    <row r="338" spans="1:9" ht="45">
+    <row r="338" spans="1:9" ht="30">
       <c r="A338" s="29" t="s">
         <v>353</v>
       </c>
@@ -17412,7 +17412,7 @@
       </c>
       <c r="I341" s="31"/>
     </row>
-    <row r="342" spans="1:9" ht="45">
+    <row r="342" spans="1:9" ht="30">
       <c r="A342" s="29" t="s">
         <v>357</v>
       </c>
@@ -17439,7 +17439,7 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="343" spans="1:9" ht="45">
+    <row r="343" spans="1:9" ht="30">
       <c r="A343" s="29" t="s">
         <v>358</v>
       </c>
@@ -17464,7 +17464,7 @@
       </c>
       <c r="I343" s="31"/>
     </row>
-    <row r="344" spans="1:9" ht="30">
+    <row r="344" spans="1:9">
       <c r="A344" s="29" t="s">
         <v>359</v>
       </c>
@@ -17489,7 +17489,7 @@
       </c>
       <c r="I344" s="31"/>
     </row>
-    <row r="345" spans="1:9" ht="30">
+    <row r="345" spans="1:9">
       <c r="A345" s="29" t="s">
         <v>360</v>
       </c>
@@ -17514,7 +17514,7 @@
       </c>
       <c r="I345" s="31"/>
     </row>
-    <row r="346" spans="1:9" ht="45">
+    <row r="346" spans="1:9" ht="30">
       <c r="A346" s="29" t="s">
         <v>361</v>
       </c>
@@ -17564,7 +17564,7 @@
       </c>
       <c r="I347" s="31"/>
     </row>
-    <row r="348" spans="1:9" ht="60">
+    <row r="348" spans="1:9" ht="45">
       <c r="A348" s="29" t="s">
         <v>363</v>
       </c>
@@ -17639,7 +17639,7 @@
       </c>
       <c r="I350" s="31"/>
     </row>
-    <row r="351" spans="1:9" ht="45">
+    <row r="351" spans="1:9" ht="30">
       <c r="A351" s="29" t="s">
         <v>366</v>
       </c>
@@ -17664,7 +17664,7 @@
       </c>
       <c r="I351" s="31"/>
     </row>
-    <row r="352" spans="1:9" ht="45">
+    <row r="352" spans="1:9" ht="30">
       <c r="A352" s="29" t="s">
         <v>367</v>
       </c>
@@ -17714,7 +17714,7 @@
       </c>
       <c r="I353" s="31"/>
     </row>
-    <row r="354" spans="1:9" ht="75">
+    <row r="354" spans="1:9" ht="60">
       <c r="A354" s="29" t="s">
         <v>369</v>
       </c>
@@ -17845,7 +17845,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="359" spans="1:9" ht="45">
+    <row r="359" spans="1:9" ht="30">
       <c r="A359" s="29" t="s">
         <v>374</v>
       </c>
@@ -17970,7 +17970,7 @@
       </c>
       <c r="I363" s="31"/>
     </row>
-    <row r="364" spans="1:9" ht="30">
+    <row r="364" spans="1:9">
       <c r="A364" s="22" t="s">
         <v>2260</v>
       </c>
@@ -18095,7 +18095,7 @@
       </c>
       <c r="I368" s="31"/>
     </row>
-    <row r="369" spans="1:9" ht="45">
+    <row r="369" spans="1:9" ht="30">
       <c r="A369" s="29" t="s">
         <v>382</v>
       </c>
@@ -18245,7 +18245,7 @@
       </c>
       <c r="I374" s="31"/>
     </row>
-    <row r="375" spans="1:9" ht="45">
+    <row r="375" spans="1:9" ht="30">
       <c r="A375" s="29" t="s">
         <v>388</v>
       </c>
@@ -18370,7 +18370,7 @@
       </c>
       <c r="I379" s="31"/>
     </row>
-    <row r="380" spans="1:9" ht="60">
+    <row r="380" spans="1:9" ht="45">
       <c r="A380" s="29" t="s">
         <v>393</v>
       </c>
@@ -18447,7 +18447,7 @@
       </c>
       <c r="I382" s="31"/>
     </row>
-    <row r="383" spans="1:9" ht="45">
+    <row r="383" spans="1:9" ht="30">
       <c r="A383" s="29" t="s">
         <v>396</v>
       </c>
@@ -18649,7 +18649,7 @@
       </c>
       <c r="I390" s="31"/>
     </row>
-    <row r="391" spans="1:9" ht="45">
+    <row r="391" spans="1:9" ht="30">
       <c r="A391" s="29" t="s">
         <v>404</v>
       </c>
@@ -18674,7 +18674,7 @@
       </c>
       <c r="I391" s="31"/>
     </row>
-    <row r="392" spans="1:9" ht="45">
+    <row r="392" spans="1:9" ht="30">
       <c r="A392" s="29" t="s">
         <v>405</v>
       </c>
@@ -18899,7 +18899,7 @@
       </c>
       <c r="I400" s="31"/>
     </row>
-    <row r="401" spans="1:9" ht="45">
+    <row r="401" spans="1:9" ht="30">
       <c r="A401" s="29" t="s">
         <v>414</v>
       </c>
@@ -18924,7 +18924,7 @@
       </c>
       <c r="I401" s="31"/>
     </row>
-    <row r="402" spans="1:9" ht="60">
+    <row r="402" spans="1:9" ht="45">
       <c r="A402" s="29" t="s">
         <v>415</v>
       </c>
@@ -19001,7 +19001,7 @@
       </c>
       <c r="I404" s="31"/>
     </row>
-    <row r="405" spans="1:9" ht="45">
+    <row r="405" spans="1:9" ht="30">
       <c r="A405" s="29" t="s">
         <v>418</v>
       </c>
@@ -19053,7 +19053,7 @@
       </c>
       <c r="I406" s="31"/>
     </row>
-    <row r="407" spans="1:9" ht="45">
+    <row r="407" spans="1:9" ht="30">
       <c r="A407" s="29" t="s">
         <v>420</v>
       </c>
@@ -19103,7 +19103,7 @@
       </c>
       <c r="I408" s="31"/>
     </row>
-    <row r="409" spans="1:9" ht="30">
+    <row r="409" spans="1:9">
       <c r="A409" s="29" t="s">
         <v>422</v>
       </c>
@@ -19128,7 +19128,7 @@
       </c>
       <c r="I409" s="31"/>
     </row>
-    <row r="410" spans="1:9" ht="30">
+    <row r="410" spans="1:9">
       <c r="A410" s="29" t="s">
         <v>423</v>
       </c>
@@ -19178,7 +19178,7 @@
       </c>
       <c r="I411" s="31"/>
     </row>
-    <row r="412" spans="1:9" ht="30">
+    <row r="412" spans="1:9">
       <c r="A412" s="29" t="s">
         <v>425</v>
       </c>
@@ -19278,7 +19278,7 @@
       </c>
       <c r="I415" s="31"/>
     </row>
-    <row r="416" spans="1:9" ht="45">
+    <row r="416" spans="1:9" ht="30">
       <c r="A416" s="29" t="s">
         <v>429</v>
       </c>
@@ -19328,7 +19328,7 @@
       </c>
       <c r="I417" s="31"/>
     </row>
-    <row r="418" spans="1:9" ht="45">
+    <row r="418" spans="1:9" ht="30">
       <c r="A418" s="29" t="s">
         <v>431</v>
       </c>
@@ -19353,7 +19353,7 @@
       </c>
       <c r="I418" s="31"/>
     </row>
-    <row r="419" spans="1:9" ht="45">
+    <row r="419" spans="1:9" ht="30">
       <c r="A419" s="29" t="s">
         <v>432</v>
       </c>
@@ -19453,7 +19453,7 @@
       </c>
       <c r="I422" s="31"/>
     </row>
-    <row r="423" spans="1:9" ht="30">
+    <row r="423" spans="1:9">
       <c r="A423" s="29" t="s">
         <v>436</v>
       </c>
@@ -19528,7 +19528,7 @@
       </c>
       <c r="I425" s="31"/>
     </row>
-    <row r="426" spans="1:9" ht="60">
+    <row r="426" spans="1:9" ht="45">
       <c r="A426" s="29" t="s">
         <v>439</v>
       </c>
@@ -19630,7 +19630,7 @@
       </c>
       <c r="I429" s="31"/>
     </row>
-    <row r="430" spans="1:9" ht="45">
+    <row r="430" spans="1:9" ht="30">
       <c r="A430" s="29" t="s">
         <v>443</v>
       </c>
@@ -19730,7 +19730,7 @@
       </c>
       <c r="I433" s="31"/>
     </row>
-    <row r="434" spans="1:9" ht="45">
+    <row r="434" spans="1:9" ht="30">
       <c r="A434" s="29" t="s">
         <v>447</v>
       </c>
@@ -19755,7 +19755,7 @@
       </c>
       <c r="I434" s="31"/>
     </row>
-    <row r="435" spans="1:9" ht="45">
+    <row r="435" spans="1:9" ht="30">
       <c r="A435" s="29" t="s">
         <v>448</v>
       </c>
@@ -19780,7 +19780,7 @@
       </c>
       <c r="I435" s="31"/>
     </row>
-    <row r="436" spans="1:9" ht="60">
+    <row r="436" spans="1:9" ht="45">
       <c r="A436" s="29" t="s">
         <v>449</v>
       </c>
@@ -19909,7 +19909,7 @@
       </c>
       <c r="I440" s="31"/>
     </row>
-    <row r="441" spans="1:9" ht="45">
+    <row r="441" spans="1:9" ht="30">
       <c r="A441" s="29" t="s">
         <v>454</v>
       </c>
@@ -20059,7 +20059,7 @@
       </c>
       <c r="I446" s="31"/>
     </row>
-    <row r="447" spans="1:9" ht="30">
+    <row r="447" spans="1:9">
       <c r="A447" s="29" t="s">
         <v>460</v>
       </c>
@@ -20159,7 +20159,7 @@
       </c>
       <c r="I450" s="31"/>
     </row>
-    <row r="451" spans="1:9" ht="45">
+    <row r="451" spans="1:9" ht="30">
       <c r="A451" s="29" t="s">
         <v>464</v>
       </c>
@@ -20184,7 +20184,7 @@
       </c>
       <c r="I451" s="31"/>
     </row>
-    <row r="452" spans="1:9" ht="45">
+    <row r="452" spans="1:9" ht="30">
       <c r="A452" s="29" t="s">
         <v>465</v>
       </c>
@@ -20209,7 +20209,7 @@
       </c>
       <c r="I452" s="31"/>
     </row>
-    <row r="453" spans="1:9" ht="45">
+    <row r="453" spans="1:9" ht="30">
       <c r="A453" s="29" t="s">
         <v>466</v>
       </c>
@@ -20234,7 +20234,7 @@
       </c>
       <c r="I453" s="31"/>
     </row>
-    <row r="454" spans="1:9" ht="45">
+    <row r="454" spans="1:9" ht="30">
       <c r="A454" s="29" t="s">
         <v>467</v>
       </c>
@@ -20309,7 +20309,7 @@
       </c>
       <c r="I456" s="31"/>
     </row>
-    <row r="457" spans="1:9" ht="45">
+    <row r="457" spans="1:9" ht="30">
       <c r="A457" s="22" t="s">
         <v>470</v>
       </c>
@@ -20334,7 +20334,7 @@
       </c>
       <c r="I457" s="31"/>
     </row>
-    <row r="458" spans="1:9" ht="30">
+    <row r="458" spans="1:9">
       <c r="A458" s="29" t="s">
         <v>471</v>
       </c>
@@ -20459,7 +20459,7 @@
       </c>
       <c r="I462" s="31"/>
     </row>
-    <row r="463" spans="1:9" ht="30">
+    <row r="463" spans="1:9">
       <c r="A463" s="29" t="s">
         <v>476</v>
       </c>
@@ -20534,7 +20534,7 @@
       </c>
       <c r="I465" s="31"/>
     </row>
-    <row r="466" spans="1:9" ht="30">
+    <row r="466" spans="1:9">
       <c r="A466" s="29" t="s">
         <v>479</v>
       </c>
@@ -20686,7 +20686,7 @@
       </c>
       <c r="I471" s="31"/>
     </row>
-    <row r="472" spans="1:9" ht="45">
+    <row r="472" spans="1:9" ht="30">
       <c r="A472" s="29" t="s">
         <v>485</v>
       </c>
@@ -20811,7 +20811,7 @@
       </c>
       <c r="I476" s="31"/>
     </row>
-    <row r="477" spans="1:9" ht="30">
+    <row r="477" spans="1:9">
       <c r="A477" s="29" t="s">
         <v>490</v>
       </c>
@@ -20992,7 +20992,7 @@
       </c>
       <c r="I483" s="31"/>
     </row>
-    <row r="484" spans="1:9" ht="90">
+    <row r="484" spans="1:9" ht="75">
       <c r="A484" s="29" t="s">
         <v>497</v>
       </c>
@@ -21094,7 +21094,7 @@
       </c>
       <c r="I487" s="31"/>
     </row>
-    <row r="488" spans="1:9" ht="45">
+    <row r="488" spans="1:9" ht="30">
       <c r="A488" s="29" t="s">
         <v>501</v>
       </c>
@@ -21119,7 +21119,7 @@
       </c>
       <c r="I488" s="31"/>
     </row>
-    <row r="489" spans="1:9" ht="30">
+    <row r="489" spans="1:9">
       <c r="A489" s="29" t="s">
         <v>502</v>
       </c>
@@ -21144,7 +21144,7 @@
       </c>
       <c r="I489" s="31"/>
     </row>
-    <row r="490" spans="1:9" ht="45">
+    <row r="490" spans="1:9" ht="30">
       <c r="A490" s="29" t="s">
         <v>503</v>
       </c>
@@ -21294,7 +21294,7 @@
       </c>
       <c r="I495" s="31"/>
     </row>
-    <row r="496" spans="1:9" ht="45">
+    <row r="496" spans="1:9" ht="30">
       <c r="A496" s="29" t="s">
         <v>509</v>
       </c>
@@ -21444,7 +21444,7 @@
       </c>
       <c r="I501" s="31"/>
     </row>
-    <row r="502" spans="1:9" ht="45">
+    <row r="502" spans="1:9" ht="30">
       <c r="A502" s="29" t="s">
         <v>515</v>
       </c>
@@ -21494,7 +21494,7 @@
       </c>
       <c r="I503" s="31"/>
     </row>
-    <row r="504" spans="1:9" ht="30">
+    <row r="504" spans="1:9">
       <c r="A504" s="29" t="s">
         <v>517</v>
       </c>
@@ -21519,7 +21519,7 @@
       </c>
       <c r="I504" s="31"/>
     </row>
-    <row r="505" spans="1:9" ht="45">
+    <row r="505" spans="1:9" ht="30">
       <c r="A505" s="29" t="s">
         <v>518</v>
       </c>
@@ -21619,7 +21619,7 @@
       </c>
       <c r="I508" s="31"/>
     </row>
-    <row r="509" spans="1:9" ht="60">
+    <row r="509" spans="1:9" ht="45">
       <c r="A509" s="22" t="s">
         <v>522</v>
       </c>
@@ -21671,7 +21671,7 @@
       </c>
       <c r="I510" s="20"/>
     </row>
-    <row r="511" spans="1:9" ht="30">
+    <row r="511" spans="1:9">
       <c r="A511" s="29" t="s">
         <v>524</v>
       </c>
@@ -21816,8 +21816,8 @@
       <c r="G516" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H516" s="34" t="s">
-        <v>20</v>
+      <c r="H516" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="I516" s="35"/>
     </row>
@@ -21866,8 +21866,8 @@
       <c r="G518" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="H518" s="34" t="s">
-        <v>20</v>
+      <c r="H518" s="29" t="s">
+        <v>18</v>
       </c>
       <c r="I518" s="35"/>
     </row>
@@ -21971,7 +21971,7 @@
       </c>
       <c r="I522" s="31"/>
     </row>
-    <row r="523" spans="1:9" ht="30">
+    <row r="523" spans="1:9">
       <c r="A523" s="29" t="s">
         <v>528</v>
       </c>
@@ -22021,7 +22021,7 @@
       </c>
       <c r="I524" s="31"/>
     </row>
-    <row r="525" spans="1:9" ht="45">
+    <row r="525" spans="1:9" ht="30">
       <c r="A525" s="22" t="s">
         <v>530</v>
       </c>
@@ -22071,7 +22071,7 @@
       </c>
       <c r="I526" s="35"/>
     </row>
-    <row r="527" spans="1:9" ht="45">
+    <row r="527" spans="1:9" ht="30">
       <c r="A527" s="34" t="s">
         <v>2280</v>
       </c>
@@ -22146,7 +22146,7 @@
       </c>
       <c r="I529" s="31"/>
     </row>
-    <row r="530" spans="1:9" ht="30">
+    <row r="530" spans="1:9">
       <c r="A530" s="29" t="s">
         <v>533</v>
       </c>
@@ -22171,7 +22171,7 @@
       </c>
       <c r="I530" s="31"/>
     </row>
-    <row r="531" spans="1:9" ht="45">
+    <row r="531" spans="1:9" ht="30">
       <c r="A531" s="29" t="s">
         <v>534</v>
       </c>
@@ -22271,7 +22271,7 @@
       </c>
       <c r="I534" s="31"/>
     </row>
-    <row r="535" spans="1:9" ht="30">
+    <row r="535" spans="1:9">
       <c r="A535" s="29" t="s">
         <v>538</v>
       </c>
@@ -22321,7 +22321,7 @@
       </c>
       <c r="I536" s="31"/>
     </row>
-    <row r="537" spans="1:9" ht="45">
+    <row r="537" spans="1:9" ht="30">
       <c r="A537" s="29" t="s">
         <v>540</v>
       </c>
@@ -22371,7 +22371,7 @@
       </c>
       <c r="I538" s="31"/>
     </row>
-    <row r="539" spans="1:9" ht="45">
+    <row r="539" spans="1:9" ht="30">
       <c r="A539" s="29" t="s">
         <v>542</v>
       </c>
@@ -22546,7 +22546,7 @@
       </c>
       <c r="I545" s="31"/>
     </row>
-    <row r="546" spans="1:9" ht="30">
+    <row r="546" spans="1:9">
       <c r="A546" s="29" t="s">
         <v>549</v>
       </c>
@@ -22721,7 +22721,7 @@
       </c>
       <c r="I552" s="31"/>
     </row>
-    <row r="553" spans="1:9" ht="30">
+    <row r="553" spans="1:9">
       <c r="A553" s="29" t="s">
         <v>556</v>
       </c>
@@ -22771,7 +22771,7 @@
       </c>
       <c r="I554" s="20"/>
     </row>
-    <row r="555" spans="1:9" ht="45">
+    <row r="555" spans="1:9" ht="30">
       <c r="A555" s="29" t="s">
         <v>558</v>
       </c>
@@ -22898,7 +22898,7 @@
       </c>
       <c r="I559" s="31"/>
     </row>
-    <row r="560" spans="1:9" ht="30">
+    <row r="560" spans="1:9">
       <c r="A560" s="29" t="s">
         <v>563</v>
       </c>
@@ -22923,7 +22923,7 @@
       </c>
       <c r="I560" s="31"/>
     </row>
-    <row r="561" spans="1:9" ht="45">
+    <row r="561" spans="1:9" ht="30">
       <c r="A561" s="29" t="s">
         <v>564</v>
       </c>
@@ -22948,7 +22948,7 @@
       </c>
       <c r="I561" s="31"/>
     </row>
-    <row r="562" spans="1:9" ht="45">
+    <row r="562" spans="1:9" ht="30">
       <c r="A562" s="29" t="s">
         <v>565</v>
       </c>
@@ -22998,7 +22998,7 @@
       </c>
       <c r="I563" s="31"/>
     </row>
-    <row r="564" spans="1:9" ht="60">
+    <row r="564" spans="1:9" ht="45">
       <c r="A564" s="29" t="s">
         <v>567</v>
       </c>
@@ -23350,7 +23350,7 @@
       </c>
       <c r="I577" s="31"/>
     </row>
-    <row r="578" spans="1:9" ht="75">
+    <row r="578" spans="1:9" ht="60">
       <c r="A578" s="29" t="s">
         <v>581</v>
       </c>
@@ -23377,7 +23377,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="579" spans="1:9" ht="75">
+    <row r="579" spans="1:9" ht="60">
       <c r="A579" s="29" t="s">
         <v>582</v>
       </c>
@@ -23404,7 +23404,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="580" spans="1:9" ht="75">
+    <row r="580" spans="1:9" ht="60">
       <c r="A580" s="29" t="s">
         <v>583</v>
       </c>
@@ -23431,7 +23431,7 @@
         <v>2164</v>
       </c>
     </row>
-    <row r="581" spans="1:9" ht="30">
+    <row r="581" spans="1:9">
       <c r="A581" s="29" t="s">
         <v>584</v>
       </c>
@@ -23456,7 +23456,7 @@
       </c>
       <c r="I581" s="31"/>
     </row>
-    <row r="582" spans="1:9" ht="75">
+    <row r="582" spans="1:9" ht="60">
       <c r="A582" s="29" t="s">
         <v>585</v>
       </c>
@@ -23535,7 +23535,7 @@
       </c>
       <c r="I584" s="31"/>
     </row>
-    <row r="585" spans="1:9" ht="105">
+    <row r="585" spans="1:9" ht="90">
       <c r="A585" s="29" t="s">
         <v>588</v>
       </c>
@@ -23562,7 +23562,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="586" spans="1:9" ht="105">
+    <row r="586" spans="1:9" ht="90">
       <c r="A586" s="29" t="s">
         <v>589</v>
       </c>
@@ -23589,7 +23589,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="587" spans="1:9" ht="105">
+    <row r="587" spans="1:9" ht="90">
       <c r="A587" s="29" t="s">
         <v>590</v>
       </c>
@@ -23695,7 +23695,7 @@
         <v>2168</v>
       </c>
     </row>
-    <row r="591" spans="1:9" ht="30">
+    <row r="591" spans="1:9">
       <c r="A591" s="29" t="s">
         <v>594</v>
       </c>
@@ -23772,7 +23772,7 @@
       </c>
       <c r="I593" s="31"/>
     </row>
-    <row r="594" spans="1:9" ht="30">
+    <row r="594" spans="1:9">
       <c r="A594" s="29" t="s">
         <v>597</v>
       </c>
@@ -23797,7 +23797,7 @@
       </c>
       <c r="I594" s="31"/>
     </row>
-    <row r="595" spans="1:9" ht="30">
+    <row r="595" spans="1:9">
       <c r="A595" s="29" t="s">
         <v>598</v>
       </c>
@@ -23897,7 +23897,7 @@
       </c>
       <c r="I598" s="31"/>
     </row>
-    <row r="599" spans="1:9" ht="30">
+    <row r="599" spans="1:9">
       <c r="A599" s="29" t="s">
         <v>602</v>
       </c>
@@ -24097,7 +24097,7 @@
       </c>
       <c r="I606" s="31"/>
     </row>
-    <row r="607" spans="1:9" ht="30">
+    <row r="607" spans="1:9">
       <c r="A607" s="29" t="s">
         <v>610</v>
       </c>
@@ -24228,7 +24228,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="612" spans="1:9" ht="45">
+    <row r="612" spans="1:9" ht="30">
       <c r="A612" s="29" t="s">
         <v>615</v>
       </c>
@@ -24328,7 +24328,7 @@
       </c>
       <c r="I615" s="31"/>
     </row>
-    <row r="616" spans="1:9" ht="60">
+    <row r="616" spans="1:9" ht="45">
       <c r="A616" s="29" t="s">
         <v>619</v>
       </c>
@@ -24453,7 +24453,7 @@
       </c>
       <c r="I620" s="31"/>
     </row>
-    <row r="621" spans="1:9" ht="60">
+    <row r="621" spans="1:9" ht="45">
       <c r="A621" s="29" t="s">
         <v>624</v>
       </c>
@@ -24503,7 +24503,7 @@
       </c>
       <c r="I622" s="31"/>
     </row>
-    <row r="623" spans="1:9" ht="30">
+    <row r="623" spans="1:9">
       <c r="A623" s="29" t="s">
         <v>626</v>
       </c>
@@ -24553,7 +24553,7 @@
       </c>
       <c r="I624" s="31"/>
     </row>
-    <row r="625" spans="1:9" ht="75">
+    <row r="625" spans="1:9" ht="60">
       <c r="A625" s="29" t="s">
         <v>628</v>
       </c>
@@ -24580,7 +24580,7 @@
         <v>2172</v>
       </c>
     </row>
-    <row r="626" spans="1:9" ht="225">
+    <row r="626" spans="1:9" ht="210">
       <c r="A626" s="29" t="s">
         <v>629</v>
       </c>
@@ -24736,7 +24736,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="632" spans="1:9" ht="60">
+    <row r="632" spans="1:9" ht="45">
       <c r="A632" s="29" t="s">
         <v>635</v>
       </c>
@@ -24761,7 +24761,7 @@
       </c>
       <c r="I632" s="31"/>
     </row>
-    <row r="633" spans="1:9" ht="30">
+    <row r="633" spans="1:9">
       <c r="A633" s="29" t="s">
         <v>636</v>
       </c>
@@ -24890,7 +24890,7 @@
         <v>2176</v>
       </c>
     </row>
-    <row r="638" spans="1:9" ht="45">
+    <row r="638" spans="1:9" ht="30">
       <c r="A638" s="29" t="s">
         <v>641</v>
       </c>
@@ -24915,7 +24915,7 @@
       </c>
       <c r="I638" s="31"/>
     </row>
-    <row r="639" spans="1:9" ht="60">
+    <row r="639" spans="1:9" ht="45">
       <c r="A639" s="29" t="s">
         <v>642</v>
       </c>
@@ -24940,7 +24940,7 @@
       </c>
       <c r="I639" s="31"/>
     </row>
-    <row r="640" spans="1:9" ht="30">
+    <row r="640" spans="1:9">
       <c r="A640" s="29" t="s">
         <v>643</v>
       </c>
@@ -24965,7 +24965,7 @@
       </c>
       <c r="I640" s="31"/>
     </row>
-    <row r="641" spans="1:9" ht="60">
+    <row r="641" spans="1:9" ht="45">
       <c r="A641" s="29" t="s">
         <v>644</v>
       </c>
@@ -24990,7 +24990,7 @@
       </c>
       <c r="I641" s="31"/>
     </row>
-    <row r="642" spans="1:9" ht="60">
+    <row r="642" spans="1:9" ht="45">
       <c r="A642" s="29" t="s">
         <v>645</v>
       </c>
@@ -25069,7 +25069,7 @@
         <v>2147</v>
       </c>
     </row>
-    <row r="645" spans="1:9" ht="45">
+    <row r="645" spans="1:9" ht="30">
       <c r="A645" s="29" t="s">
         <v>648</v>
       </c>
@@ -25194,7 +25194,7 @@
       </c>
       <c r="I649" s="31"/>
     </row>
-    <row r="650" spans="1:9" ht="30">
+    <row r="650" spans="1:9">
       <c r="A650" s="29" t="s">
         <v>652</v>
       </c>
@@ -25569,7 +25569,7 @@
       </c>
       <c r="I664" s="31"/>
     </row>
-    <row r="665" spans="1:9" ht="75">
+    <row r="665" spans="1:9" ht="60">
       <c r="A665" s="29" t="s">
         <v>667</v>
       </c>
@@ -25669,7 +25669,7 @@
       </c>
       <c r="I668" s="31"/>
     </row>
-    <row r="669" spans="1:9" ht="150">
+    <row r="669" spans="1:9" ht="135">
       <c r="A669" s="29" t="s">
         <v>671</v>
       </c>
@@ -25694,7 +25694,7 @@
       </c>
       <c r="I669" s="31"/>
     </row>
-    <row r="670" spans="1:9" ht="45">
+    <row r="670" spans="1:9" ht="30">
       <c r="A670" s="29" t="s">
         <v>672</v>
       </c>
@@ -25869,7 +25869,7 @@
       </c>
       <c r="I676" s="31"/>
     </row>
-    <row r="677" spans="1:9" ht="30">
+    <row r="677" spans="1:9">
       <c r="A677" s="29" t="s">
         <v>679</v>
       </c>
@@ -25944,7 +25944,7 @@
       </c>
       <c r="I679" s="31"/>
     </row>
-    <row r="680" spans="1:9" ht="45">
+    <row r="680" spans="1:9" ht="30">
       <c r="A680" s="29" t="s">
         <v>682</v>
       </c>
@@ -26044,7 +26044,7 @@
       </c>
       <c r="I683" s="31"/>
     </row>
-    <row r="684" spans="1:9" ht="45">
+    <row r="684" spans="1:9" ht="30">
       <c r="A684" s="29" t="s">
         <v>686</v>
       </c>
@@ -26069,7 +26069,7 @@
       </c>
       <c r="I684" s="31"/>
     </row>
-    <row r="685" spans="1:9" ht="60">
+    <row r="685" spans="1:9" ht="45">
       <c r="A685" s="29" t="s">
         <v>687</v>
       </c>
@@ -26096,7 +26096,7 @@
         <v>2178</v>
       </c>
     </row>
-    <row r="686" spans="1:9" ht="45">
+    <row r="686" spans="1:9" ht="30">
       <c r="A686" s="29" t="s">
         <v>688</v>
       </c>
@@ -26123,7 +26123,7 @@
       </c>
       <c r="I686" s="31"/>
     </row>
-    <row r="687" spans="1:9" ht="45">
+    <row r="687" spans="1:9" ht="30">
       <c r="A687" s="29" t="s">
         <v>689</v>
       </c>
@@ -26364,7 +26364,7 @@
       </c>
       <c r="I695" s="31"/>
     </row>
-    <row r="696" spans="1:9" ht="105">
+    <row r="696" spans="1:9" ht="75">
       <c r="A696" s="29" t="s">
         <v>698</v>
       </c>
@@ -26416,7 +26416,7 @@
       </c>
       <c r="I697" s="31"/>
     </row>
-    <row r="698" spans="1:9" ht="30">
+    <row r="698" spans="1:9">
       <c r="A698" s="29" t="s">
         <v>700</v>
       </c>
@@ -26441,7 +26441,7 @@
       </c>
       <c r="I698" s="31"/>
     </row>
-    <row r="699" spans="1:9" ht="45">
+    <row r="699" spans="1:9" ht="30">
       <c r="A699" s="29" t="s">
         <v>701</v>
       </c>
@@ -26491,7 +26491,7 @@
       </c>
       <c r="I700" s="31"/>
     </row>
-    <row r="701" spans="1:9" ht="45">
+    <row r="701" spans="1:9" ht="30">
       <c r="A701" s="29" t="s">
         <v>703</v>
       </c>
@@ -26516,7 +26516,7 @@
       </c>
       <c r="I701" s="31"/>
     </row>
-    <row r="702" spans="1:9" ht="30">
+    <row r="702" spans="1:9">
       <c r="A702" s="29" t="s">
         <v>704</v>
       </c>
@@ -26541,7 +26541,7 @@
       </c>
       <c r="I702" s="31"/>
     </row>
-    <row r="703" spans="1:9" ht="45">
+    <row r="703" spans="1:9" ht="30">
       <c r="A703" s="29" t="s">
         <v>705</v>
       </c>
@@ -26566,7 +26566,7 @@
       </c>
       <c r="I703" s="31"/>
     </row>
-    <row r="704" spans="1:9" ht="45">
+    <row r="704" spans="1:9" ht="30">
       <c r="A704" s="29" t="s">
         <v>706</v>
       </c>
@@ -26666,7 +26666,7 @@
       </c>
       <c r="I707" s="31"/>
     </row>
-    <row r="708" spans="1:9" ht="45">
+    <row r="708" spans="1:9" ht="30">
       <c r="A708" s="29" t="s">
         <v>710</v>
       </c>
@@ -26716,7 +26716,7 @@
       </c>
       <c r="I709" s="31"/>
     </row>
-    <row r="710" spans="1:9" ht="30">
+    <row r="710" spans="1:9">
       <c r="A710" s="29" t="s">
         <v>712</v>
       </c>
@@ -26741,7 +26741,7 @@
       </c>
       <c r="I710" s="31"/>
     </row>
-    <row r="711" spans="1:9" ht="30">
+    <row r="711" spans="1:9">
       <c r="A711" s="29" t="s">
         <v>713</v>
       </c>
@@ -26791,7 +26791,7 @@
       </c>
       <c r="I712" s="31"/>
     </row>
-    <row r="713" spans="1:9" ht="60">
+    <row r="713" spans="1:9" ht="45">
       <c r="A713" s="29" t="s">
         <v>715</v>
       </c>
@@ -26841,7 +26841,7 @@
       </c>
       <c r="I714" s="31"/>
     </row>
-    <row r="715" spans="1:9" ht="60">
+    <row r="715" spans="1:9" ht="45">
       <c r="A715" s="29" t="s">
         <v>717</v>
       </c>
@@ -26868,7 +26868,7 @@
         <v>2181</v>
       </c>
     </row>
-    <row r="716" spans="1:9" ht="240">
+    <row r="716" spans="1:9" ht="195">
       <c r="A716" s="29" t="s">
         <v>718</v>
       </c>
@@ -26920,7 +26920,7 @@
       </c>
       <c r="I717" s="31"/>
     </row>
-    <row r="718" spans="1:9" ht="30">
+    <row r="718" spans="1:9">
       <c r="A718" s="29" t="s">
         <v>720</v>
       </c>
@@ -26970,7 +26970,7 @@
       </c>
       <c r="I719" s="31"/>
     </row>
-    <row r="720" spans="1:9" ht="30">
+    <row r="720" spans="1:9">
       <c r="A720" s="29" t="s">
         <v>722</v>
       </c>
@@ -27020,7 +27020,7 @@
       </c>
       <c r="I721" s="31"/>
     </row>
-    <row r="722" spans="1:9" ht="30">
+    <row r="722" spans="1:9">
       <c r="A722" s="29" t="s">
         <v>724</v>
       </c>
@@ -27070,7 +27070,7 @@
       </c>
       <c r="I723" s="31"/>
     </row>
-    <row r="724" spans="1:9" ht="30">
+    <row r="724" spans="1:9">
       <c r="A724" s="29" t="s">
         <v>726</v>
       </c>
@@ -27095,7 +27095,7 @@
       </c>
       <c r="I724" s="31"/>
     </row>
-    <row r="725" spans="1:9" ht="45">
+    <row r="725" spans="1:9" ht="30">
       <c r="A725" s="29" t="s">
         <v>727</v>
       </c>
@@ -27120,7 +27120,7 @@
       </c>
       <c r="I725" s="31"/>
     </row>
-    <row r="726" spans="1:9" ht="30">
+    <row r="726" spans="1:9">
       <c r="A726" s="29" t="s">
         <v>728</v>
       </c>
@@ -27145,7 +27145,7 @@
       </c>
       <c r="I726" s="31"/>
     </row>
-    <row r="727" spans="1:9" ht="45">
+    <row r="727" spans="1:9" ht="30">
       <c r="A727" s="22" t="s">
         <v>729</v>
       </c>
@@ -27170,7 +27170,7 @@
       </c>
       <c r="I727" s="31"/>
     </row>
-    <row r="728" spans="1:9" ht="60">
+    <row r="728" spans="1:9" ht="45">
       <c r="A728" s="22" t="s">
         <v>730</v>
       </c>
@@ -27197,7 +27197,7 @@
         <v>2357</v>
       </c>
     </row>
-    <row r="729" spans="1:9" ht="30">
+    <row r="729" spans="1:9">
       <c r="A729" s="29" t="s">
         <v>731</v>
       </c>
@@ -27274,7 +27274,7 @@
       </c>
       <c r="I731" s="31"/>
     </row>
-    <row r="732" spans="1:9" ht="45">
+    <row r="732" spans="1:9" ht="30">
       <c r="A732" s="29" t="s">
         <v>734</v>
       </c>
@@ -27299,7 +27299,7 @@
       </c>
       <c r="I732" s="31"/>
     </row>
-    <row r="733" spans="1:9" ht="45">
+    <row r="733" spans="1:9" ht="30">
       <c r="A733" s="29" t="s">
         <v>735</v>
       </c>
@@ -27449,7 +27449,7 @@
       </c>
       <c r="I738" s="31"/>
     </row>
-    <row r="739" spans="1:9" ht="45">
+    <row r="739" spans="1:9" ht="30">
       <c r="A739" s="29" t="s">
         <v>741</v>
       </c>
@@ -27499,7 +27499,7 @@
       </c>
       <c r="I740" s="31"/>
     </row>
-    <row r="741" spans="1:9" ht="60">
+    <row r="741" spans="1:9" ht="45">
       <c r="A741" s="29" t="s">
         <v>743</v>
       </c>
@@ -27549,7 +27549,7 @@
       </c>
       <c r="I742" s="31"/>
     </row>
-    <row r="743" spans="1:9" ht="60">
+    <row r="743" spans="1:9" ht="45">
       <c r="A743" s="29" t="s">
         <v>745</v>
       </c>
@@ -27599,7 +27599,7 @@
       </c>
       <c r="I744" s="31"/>
     </row>
-    <row r="745" spans="1:9" ht="60">
+    <row r="745" spans="1:9" ht="45">
       <c r="A745" s="29" t="s">
         <v>747</v>
       </c>
@@ -27626,7 +27626,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="746" spans="1:9" ht="180">
+    <row r="746" spans="1:9" ht="135">
       <c r="A746" s="29" t="s">
         <v>748</v>
       </c>
@@ -27678,7 +27678,7 @@
       </c>
       <c r="I747" s="31"/>
     </row>
-    <row r="748" spans="1:9" ht="30">
+    <row r="748" spans="1:9">
       <c r="A748" s="29" t="s">
         <v>750</v>
       </c>
@@ -27755,7 +27755,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="751" spans="1:9" ht="30">
+    <row r="751" spans="1:9">
       <c r="A751" s="29" t="s">
         <v>753</v>
       </c>
@@ -27805,7 +27805,7 @@
       </c>
       <c r="I752" s="31"/>
     </row>
-    <row r="753" spans="1:9" ht="30">
+    <row r="753" spans="1:9">
       <c r="A753" s="29" t="s">
         <v>755</v>
       </c>
@@ -27880,7 +27880,7 @@
       </c>
       <c r="I755" s="31"/>
     </row>
-    <row r="756" spans="1:9" ht="30">
+    <row r="756" spans="1:9">
       <c r="A756" s="29" t="s">
         <v>758</v>
       </c>
@@ -27905,7 +27905,7 @@
       </c>
       <c r="I756" s="31"/>
     </row>
-    <row r="757" spans="1:9" ht="45">
+    <row r="757" spans="1:9" ht="30">
       <c r="A757" s="29" t="s">
         <v>759</v>
       </c>
@@ -27930,7 +27930,7 @@
       </c>
       <c r="I757" s="31"/>
     </row>
-    <row r="758" spans="1:9" ht="45">
+    <row r="758" spans="1:9" ht="30">
       <c r="A758" s="29" t="s">
         <v>760</v>
       </c>
@@ -27955,7 +27955,7 @@
       </c>
       <c r="I758" s="31"/>
     </row>
-    <row r="759" spans="1:9" ht="45">
+    <row r="759" spans="1:9" ht="30">
       <c r="A759" s="29" t="s">
         <v>761</v>
       </c>
@@ -28055,7 +28055,7 @@
       </c>
       <c r="I762" s="31"/>
     </row>
-    <row r="763" spans="1:9" ht="45">
+    <row r="763" spans="1:9" ht="30">
       <c r="A763" s="29" t="s">
         <v>765</v>
       </c>
@@ -28105,7 +28105,7 @@
       </c>
       <c r="I764" s="31"/>
     </row>
-    <row r="765" spans="1:9" ht="45">
+    <row r="765" spans="1:9" ht="30">
       <c r="A765" s="29" t="s">
         <v>767</v>
       </c>
@@ -28180,7 +28180,7 @@
       </c>
       <c r="I767" s="31"/>
     </row>
-    <row r="768" spans="1:9" ht="45">
+    <row r="768" spans="1:9" ht="30">
       <c r="A768" s="29" t="s">
         <v>770</v>
       </c>
@@ -28205,7 +28205,7 @@
       </c>
       <c r="I768" s="31"/>
     </row>
-    <row r="769" spans="1:9" ht="45">
+    <row r="769" spans="1:9" ht="30">
       <c r="A769" s="29" t="s">
         <v>771</v>
       </c>
@@ -28255,7 +28255,7 @@
       </c>
       <c r="I770" s="31"/>
     </row>
-    <row r="771" spans="1:9" ht="45">
+    <row r="771" spans="1:9" ht="30">
       <c r="A771" s="29" t="s">
         <v>773</v>
       </c>
@@ -28280,7 +28280,7 @@
       </c>
       <c r="I771" s="31"/>
     </row>
-    <row r="772" spans="1:9" ht="45">
+    <row r="772" spans="1:9" ht="30">
       <c r="A772" s="29" t="s">
         <v>774</v>
       </c>
@@ -28405,7 +28405,7 @@
       </c>
       <c r="I776" s="31"/>
     </row>
-    <row r="777" spans="1:9" ht="45">
+    <row r="777" spans="1:9" ht="30">
       <c r="A777" s="29" t="s">
         <v>779</v>
       </c>
@@ -28505,7 +28505,7 @@
       </c>
       <c r="I780" s="31"/>
     </row>
-    <row r="781" spans="1:9" ht="45">
+    <row r="781" spans="1:9" ht="30">
       <c r="A781" s="29" t="s">
         <v>783</v>
       </c>
@@ -28530,7 +28530,7 @@
       </c>
       <c r="I781" s="31"/>
     </row>
-    <row r="782" spans="1:9" ht="60">
+    <row r="782" spans="1:9" ht="45">
       <c r="A782" s="22" t="s">
         <v>784</v>
       </c>
@@ -28557,7 +28557,7 @@
         <v>2382</v>
       </c>
     </row>
-    <row r="783" spans="1:9" ht="45">
+    <row r="783" spans="1:9" ht="30">
       <c r="A783" s="29" t="s">
         <v>785</v>
       </c>
@@ -28607,7 +28607,7 @@
       </c>
       <c r="I784" s="31"/>
     </row>
-    <row r="785" spans="1:9" ht="60">
+    <row r="785" spans="1:9" ht="45">
       <c r="A785" s="29" t="s">
         <v>787</v>
       </c>
@@ -28632,7 +28632,7 @@
       </c>
       <c r="I785" s="31"/>
     </row>
-    <row r="786" spans="1:9" ht="60">
+    <row r="786" spans="1:9" ht="45">
       <c r="A786" s="29" t="s">
         <v>788</v>
       </c>
@@ -28657,7 +28657,7 @@
       </c>
       <c r="I786" s="31"/>
     </row>
-    <row r="787" spans="1:9" ht="60">
+    <row r="787" spans="1:9" ht="45">
       <c r="A787" s="29" t="s">
         <v>789</v>
       </c>
@@ -28707,7 +28707,7 @@
       </c>
       <c r="I788" s="31"/>
     </row>
-    <row r="789" spans="1:9" ht="60">
+    <row r="789" spans="1:9" ht="45">
       <c r="A789" s="22" t="s">
         <v>791</v>
       </c>
@@ -28732,7 +28732,7 @@
       </c>
       <c r="I789" s="31"/>
     </row>
-    <row r="790" spans="1:9" ht="45">
+    <row r="790" spans="1:9" ht="30">
       <c r="A790" s="29" t="s">
         <v>792</v>
       </c>
@@ -28759,7 +28759,7 @@
         <v>2185</v>
       </c>
     </row>
-    <row r="791" spans="1:9" ht="45">
+    <row r="791" spans="1:9" ht="30">
       <c r="A791" s="29" t="s">
         <v>793</v>
       </c>
@@ -28859,7 +28859,7 @@
       </c>
       <c r="I794" s="31"/>
     </row>
-    <row r="795" spans="1:9" ht="45">
+    <row r="795" spans="1:9" ht="30">
       <c r="A795" s="29" t="s">
         <v>797</v>
       </c>
@@ -28884,7 +28884,7 @@
       </c>
       <c r="I795" s="31"/>
     </row>
-    <row r="796" spans="1:9" ht="60">
+    <row r="796" spans="1:9" ht="45">
       <c r="A796" s="22" t="s">
         <v>798</v>
       </c>
@@ -28911,7 +28911,7 @@
         <v>2186</v>
       </c>
     </row>
-    <row r="797" spans="1:9" ht="60">
+    <row r="797" spans="1:9" ht="45">
       <c r="A797" s="29" t="s">
         <v>799</v>
       </c>
@@ -28938,7 +28938,7 @@
         <v>2187</v>
       </c>
     </row>
-    <row r="798" spans="1:9" ht="210">
+    <row r="798" spans="1:9" ht="180">
       <c r="A798" s="29" t="s">
         <v>800</v>
       </c>
@@ -28990,7 +28990,7 @@
       </c>
       <c r="I799" s="31"/>
     </row>
-    <row r="800" spans="1:9" ht="30">
+    <row r="800" spans="1:9">
       <c r="A800" s="29" t="s">
         <v>802</v>
       </c>
@@ -29040,7 +29040,7 @@
       </c>
       <c r="I801" s="31"/>
     </row>
-    <row r="802" spans="1:9" ht="30">
+    <row r="802" spans="1:9">
       <c r="A802" s="29" t="s">
         <v>804</v>
       </c>
@@ -29090,7 +29090,7 @@
       </c>
       <c r="I803" s="31"/>
     </row>
-    <row r="804" spans="1:9" ht="30">
+    <row r="804" spans="1:9">
       <c r="A804" s="29" t="s">
         <v>806</v>
       </c>
@@ -29165,7 +29165,7 @@
       </c>
       <c r="I806" s="31"/>
     </row>
-    <row r="807" spans="1:9" ht="45">
+    <row r="807" spans="1:9" ht="30">
       <c r="A807" s="29" t="s">
         <v>809</v>
       </c>
@@ -29190,7 +29190,7 @@
       </c>
       <c r="I807" s="31"/>
     </row>
-    <row r="808" spans="1:9" ht="30">
+    <row r="808" spans="1:9">
       <c r="A808" s="29" t="s">
         <v>810</v>
       </c>
@@ -29240,7 +29240,7 @@
       </c>
       <c r="I809" s="31"/>
     </row>
-    <row r="810" spans="1:9" ht="30">
+    <row r="810" spans="1:9">
       <c r="A810" s="29" t="s">
         <v>812</v>
       </c>
@@ -29265,7 +29265,7 @@
       </c>
       <c r="I810" s="31"/>
     </row>
-    <row r="811" spans="1:9" ht="45">
+    <row r="811" spans="1:9" ht="30">
       <c r="A811" s="29" t="s">
         <v>813</v>
       </c>
@@ -29315,7 +29315,7 @@
       </c>
       <c r="I812" s="20"/>
     </row>
-    <row r="813" spans="1:9" ht="45">
+    <row r="813" spans="1:9" ht="30">
       <c r="A813" s="29" t="s">
         <v>815</v>
       </c>
@@ -29465,7 +29465,7 @@
       </c>
       <c r="I818" s="31"/>
     </row>
-    <row r="819" spans="1:9" ht="75">
+    <row r="819" spans="1:9" ht="60">
       <c r="A819" s="29" t="s">
         <v>821</v>
       </c>
@@ -29567,7 +29567,7 @@
       </c>
       <c r="I822" s="31"/>
     </row>
-    <row r="823" spans="1:9" ht="30">
+    <row r="823" spans="1:9">
       <c r="A823" s="29" t="s">
         <v>825</v>
       </c>
@@ -29592,7 +29592,7 @@
       </c>
       <c r="I823" s="31"/>
     </row>
-    <row r="824" spans="1:9" ht="45">
+    <row r="824" spans="1:9" ht="30">
       <c r="A824" s="29" t="s">
         <v>826</v>
       </c>
@@ -29617,7 +29617,7 @@
       </c>
       <c r="I824" s="31"/>
     </row>
-    <row r="825" spans="1:9" ht="45">
+    <row r="825" spans="1:9" ht="30">
       <c r="A825" s="29" t="s">
         <v>827</v>
       </c>
@@ -29794,7 +29794,7 @@
       </c>
       <c r="I831" s="31"/>
     </row>
-    <row r="832" spans="1:9" ht="45">
+    <row r="832" spans="1:9" ht="30">
       <c r="A832" s="29" t="s">
         <v>834</v>
       </c>
@@ -29869,7 +29869,7 @@
       </c>
       <c r="I834" s="31"/>
     </row>
-    <row r="835" spans="1:9" ht="75">
+    <row r="835" spans="1:9" ht="60">
       <c r="A835" s="29" t="s">
         <v>837</v>
       </c>
@@ -29946,7 +29946,7 @@
       </c>
       <c r="I837" s="31"/>
     </row>
-    <row r="838" spans="1:9" ht="45">
+    <row r="838" spans="1:9" ht="30">
       <c r="A838" s="29" t="s">
         <v>840</v>
       </c>
@@ -29971,7 +29971,7 @@
       </c>
       <c r="I838" s="31"/>
     </row>
-    <row r="839" spans="1:9" ht="30">
+    <row r="839" spans="1:9">
       <c r="A839" s="29" t="s">
         <v>841</v>
       </c>
@@ -30023,7 +30023,7 @@
         <v>2226</v>
       </c>
     </row>
-    <row r="841" spans="1:9" ht="45">
+    <row r="841" spans="1:9" ht="30">
       <c r="A841" s="29" t="s">
         <v>843</v>
       </c>
@@ -30175,7 +30175,7 @@
       </c>
       <c r="I846" s="31"/>
     </row>
-    <row r="847" spans="1:9" ht="45">
+    <row r="847" spans="1:9" ht="30">
       <c r="A847" s="29" t="s">
         <v>849</v>
       </c>
@@ -30275,7 +30275,7 @@
       </c>
       <c r="I850" s="31"/>
     </row>
-    <row r="851" spans="1:9" ht="75">
+    <row r="851" spans="1:9" ht="60">
       <c r="A851" s="29" t="s">
         <v>853</v>
       </c>
@@ -30327,7 +30327,7 @@
       </c>
       <c r="I852" s="31"/>
     </row>
-    <row r="853" spans="1:9" ht="30">
+    <row r="853" spans="1:9">
       <c r="A853" s="29" t="s">
         <v>855</v>
       </c>
@@ -30377,7 +30377,7 @@
       </c>
       <c r="I854" s="31"/>
     </row>
-    <row r="855" spans="1:9" ht="30">
+    <row r="855" spans="1:9">
       <c r="A855" s="29" t="s">
         <v>857</v>
       </c>
@@ -30427,7 +30427,7 @@
       </c>
       <c r="I856" s="31"/>
     </row>
-    <row r="857" spans="1:9" ht="45">
+    <row r="857" spans="1:9" ht="30">
       <c r="A857" s="29" t="s">
         <v>859</v>
       </c>
@@ -30577,7 +30577,7 @@
       </c>
       <c r="I862" s="31"/>
     </row>
-    <row r="863" spans="1:9" ht="60">
+    <row r="863" spans="1:9" ht="45">
       <c r="A863" s="29" t="s">
         <v>865</v>
       </c>
@@ -30627,7 +30627,7 @@
       </c>
       <c r="I864" s="31"/>
     </row>
-    <row r="865" spans="1:9" ht="45">
+    <row r="865" spans="1:9" ht="30">
       <c r="A865" s="29" t="s">
         <v>867</v>
       </c>
@@ -30727,7 +30727,7 @@
       </c>
       <c r="I868" s="31"/>
     </row>
-    <row r="869" spans="1:9" ht="75">
+    <row r="869" spans="1:9" ht="60">
       <c r="A869" s="29" t="s">
         <v>871</v>
       </c>
@@ -30779,7 +30779,7 @@
       </c>
       <c r="I870" s="31"/>
     </row>
-    <row r="871" spans="1:9" ht="30">
+    <row r="871" spans="1:9">
       <c r="A871" s="29" t="s">
         <v>873</v>
       </c>
@@ -30829,7 +30829,7 @@
       </c>
       <c r="I872" s="31"/>
     </row>
-    <row r="873" spans="1:9" ht="30">
+    <row r="873" spans="1:9">
       <c r="A873" s="29" t="s">
         <v>875</v>
       </c>
@@ -30879,7 +30879,7 @@
       </c>
       <c r="I874" s="31"/>
     </row>
-    <row r="875" spans="1:9" ht="45">
+    <row r="875" spans="1:9" ht="30">
       <c r="A875" s="29" t="s">
         <v>877</v>
       </c>
@@ -31108,7 +31108,7 @@
       </c>
       <c r="I883" s="31"/>
     </row>
-    <row r="884" spans="1:9" ht="45">
+    <row r="884" spans="1:9" ht="30">
       <c r="A884" s="29" t="s">
         <v>886</v>
       </c>
@@ -31208,7 +31208,7 @@
       </c>
       <c r="I887" s="31"/>
     </row>
-    <row r="888" spans="1:9" ht="60">
+    <row r="888" spans="1:9" ht="45">
       <c r="A888" s="22" t="s">
         <v>890</v>
       </c>
@@ -31262,7 +31262,7 @@
         <v>2194</v>
       </c>
     </row>
-    <row r="890" spans="1:9" ht="45">
+    <row r="890" spans="1:9" ht="30">
       <c r="A890" s="29" t="s">
         <v>892</v>
       </c>
@@ -31314,7 +31314,7 @@
       </c>
       <c r="I891" s="31"/>
     </row>
-    <row r="892" spans="1:9" ht="30">
+    <row r="892" spans="1:9">
       <c r="A892" s="29" t="s">
         <v>894</v>
       </c>
@@ -31339,7 +31339,7 @@
       </c>
       <c r="I892" s="31"/>
     </row>
-    <row r="893" spans="1:9" ht="45">
+    <row r="893" spans="1:9" ht="30">
       <c r="A893" s="29" t="s">
         <v>895</v>
       </c>
@@ -31364,7 +31364,7 @@
       </c>
       <c r="I893" s="31"/>
     </row>
-    <row r="894" spans="1:9" ht="45">
+    <row r="894" spans="1:9" ht="30">
       <c r="A894" s="29" t="s">
         <v>896</v>
       </c>
@@ -31514,7 +31514,7 @@
       </c>
       <c r="I899" s="31"/>
     </row>
-    <row r="900" spans="1:9" ht="45">
+    <row r="900" spans="1:9" ht="30">
       <c r="A900" s="29" t="s">
         <v>902</v>
       </c>
@@ -31595,7 +31595,7 @@
       </c>
       <c r="I902" s="31"/>
     </row>
-    <row r="903" spans="1:9" ht="45">
+    <row r="903" spans="1:9" ht="30">
       <c r="A903" s="29" t="s">
         <v>905</v>
       </c>
@@ -31697,7 +31697,7 @@
       </c>
       <c r="I906" s="31"/>
     </row>
-    <row r="907" spans="1:9" ht="60">
+    <row r="907" spans="1:9" ht="45">
       <c r="A907" s="29" t="s">
         <v>909</v>
       </c>
@@ -31747,7 +31747,7 @@
       </c>
       <c r="I908" s="31"/>
     </row>
-    <row r="909" spans="1:9" ht="45">
+    <row r="909" spans="1:9" ht="30">
       <c r="A909" s="29" t="s">
         <v>911</v>
       </c>
@@ -31849,7 +31849,7 @@
       </c>
       <c r="I912" s="31"/>
     </row>
-    <row r="913" spans="1:9" ht="45">
+    <row r="913" spans="1:9" ht="30">
       <c r="A913" s="29" t="s">
         <v>915</v>
       </c>
@@ -32001,7 +32001,7 @@
       </c>
       <c r="I918" s="31"/>
     </row>
-    <row r="919" spans="1:9" ht="60">
+    <row r="919" spans="1:9" ht="45">
       <c r="A919" s="29" t="s">
         <v>921</v>
       </c>
@@ -32076,7 +32076,7 @@
       </c>
       <c r="I921" s="31"/>
     </row>
-    <row r="922" spans="1:9" ht="45">
+    <row r="922" spans="1:9" ht="30">
       <c r="A922" s="29" t="s">
         <v>924</v>
       </c>
@@ -32176,7 +32176,7 @@
       </c>
       <c r="I925" s="31"/>
     </row>
-    <row r="926" spans="1:9" ht="45">
+    <row r="926" spans="1:9" ht="30">
       <c r="A926" s="29" t="s">
         <v>928</v>
       </c>
@@ -32228,7 +32228,7 @@
       </c>
       <c r="I927" s="31"/>
     </row>
-    <row r="928" spans="1:9" ht="30">
+    <row r="928" spans="1:9">
       <c r="A928" s="29" t="s">
         <v>930</v>
       </c>
@@ -32253,7 +32253,7 @@
       </c>
       <c r="I928" s="31"/>
     </row>
-    <row r="929" spans="1:9" ht="45">
+    <row r="929" spans="1:9" ht="30">
       <c r="A929" s="29" t="s">
         <v>931</v>
       </c>
@@ -32278,7 +32278,7 @@
       </c>
       <c r="I929" s="31"/>
     </row>
-    <row r="930" spans="1:9" ht="45">
+    <row r="930" spans="1:9" ht="30">
       <c r="A930" s="29" t="s">
         <v>932</v>
       </c>
@@ -32430,7 +32430,7 @@
       </c>
       <c r="I935" s="31"/>
     </row>
-    <row r="936" spans="1:9" ht="60">
+    <row r="936" spans="1:9" ht="45">
       <c r="A936" s="29" t="s">
         <v>938</v>
       </c>
@@ -32480,7 +32480,7 @@
       </c>
       <c r="I937" s="31"/>
     </row>
-    <row r="938" spans="1:9" ht="45">
+    <row r="938" spans="1:9" ht="30">
       <c r="A938" s="29" t="s">
         <v>940</v>
       </c>
@@ -32580,7 +32580,7 @@
       </c>
       <c r="I941" s="31"/>
     </row>
-    <row r="942" spans="1:9" ht="45">
+    <row r="942" spans="1:9" ht="30">
       <c r="A942" s="29" t="s">
         <v>944</v>
       </c>
@@ -32657,7 +32657,7 @@
       </c>
       <c r="I944" s="31"/>
     </row>
-    <row r="945" spans="1:9" ht="45">
+    <row r="945" spans="1:9" ht="30">
       <c r="A945" s="29" t="s">
         <v>947</v>
       </c>
@@ -32682,7 +32682,7 @@
       </c>
       <c r="I945" s="31"/>
     </row>
-    <row r="946" spans="1:9" ht="45">
+    <row r="946" spans="1:9" ht="30">
       <c r="A946" s="29" t="s">
         <v>948</v>
       </c>
@@ -32832,7 +32832,7 @@
       </c>
       <c r="I951" s="31"/>
     </row>
-    <row r="952" spans="1:9" ht="45">
+    <row r="952" spans="1:9" ht="30">
       <c r="A952" s="29" t="s">
         <v>954</v>
       </c>
@@ -32932,7 +32932,7 @@
       </c>
       <c r="I955" s="31"/>
     </row>
-    <row r="956" spans="1:9" ht="60">
+    <row r="956" spans="1:9" ht="45">
       <c r="A956" s="29" t="s">
         <v>958</v>
       </c>
@@ -32959,7 +32959,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="957" spans="1:9" ht="45">
+    <row r="957" spans="1:9" ht="30">
       <c r="A957" s="29" t="s">
         <v>959</v>
       </c>
@@ -33011,7 +33011,7 @@
       </c>
       <c r="I958" s="31"/>
     </row>
-    <row r="959" spans="1:9" ht="30">
+    <row r="959" spans="1:9">
       <c r="A959" s="29" t="s">
         <v>961</v>
       </c>
@@ -33036,7 +33036,7 @@
       </c>
       <c r="I959" s="31"/>
     </row>
-    <row r="960" spans="1:9" ht="45">
+    <row r="960" spans="1:9" ht="30">
       <c r="A960" s="29" t="s">
         <v>962</v>
       </c>
@@ -33061,7 +33061,7 @@
       </c>
       <c r="I960" s="31"/>
     </row>
-    <row r="961" spans="1:9" ht="45">
+    <row r="961" spans="1:9" ht="30">
       <c r="A961" s="29" t="s">
         <v>963</v>
       </c>
@@ -33361,7 +33361,7 @@
       </c>
       <c r="I972" s="31"/>
     </row>
-    <row r="973" spans="1:9" ht="60">
+    <row r="973" spans="1:9" ht="45">
       <c r="A973" s="22" t="s">
         <v>975</v>
       </c>
@@ -33386,7 +33386,7 @@
       </c>
       <c r="I973" s="20"/>
     </row>
-    <row r="974" spans="1:9" ht="60">
+    <row r="974" spans="1:9" ht="45">
       <c r="A974" s="29" t="s">
         <v>976</v>
       </c>
@@ -33413,7 +33413,7 @@
         <v>2202</v>
       </c>
     </row>
-    <row r="975" spans="1:9" ht="75">
+    <row r="975" spans="1:9" ht="60">
       <c r="A975" s="29" t="s">
         <v>977</v>
       </c>
@@ -33465,7 +33465,7 @@
       </c>
       <c r="I976" s="31"/>
     </row>
-    <row r="977" spans="1:9" ht="30">
+    <row r="977" spans="1:9">
       <c r="A977" s="29" t="s">
         <v>979</v>
       </c>
@@ -33490,7 +33490,7 @@
       </c>
       <c r="I977" s="31"/>
     </row>
-    <row r="978" spans="1:9" ht="45">
+    <row r="978" spans="1:9" ht="30">
       <c r="A978" s="29" t="s">
         <v>980</v>
       </c>
@@ -33515,7 +33515,7 @@
       </c>
       <c r="I978" s="31"/>
     </row>
-    <row r="979" spans="1:9" ht="30">
+    <row r="979" spans="1:9">
       <c r="A979" s="29" t="s">
         <v>981</v>
       </c>
@@ -33700,7 +33700,7 @@
       </c>
       <c r="I985" s="31"/>
     </row>
-    <row r="986" spans="1:9" ht="60">
+    <row r="986" spans="1:9" ht="45">
       <c r="A986" s="29" t="s">
         <v>988</v>
       </c>
@@ -33758,7 +33758,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="988" spans="1:9" ht="60">
+    <row r="988" spans="1:9" ht="45">
       <c r="A988" s="29" t="s">
         <v>990</v>
       </c>
@@ -33845,7 +33845,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="991" spans="1:9" ht="60">
+    <row r="991" spans="1:9" ht="45">
       <c r="A991" s="29" t="s">
         <v>993</v>
       </c>
@@ -33874,7 +33874,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="992" spans="1:9" ht="60">
+    <row r="992" spans="1:9" ht="45">
       <c r="A992" s="29" t="s">
         <v>994</v>
       </c>
@@ -33930,7 +33930,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="994" spans="1:9" ht="60">
+    <row r="994" spans="1:9" ht="45">
       <c r="A994" s="29" t="s">
         <v>996</v>
       </c>
@@ -33984,7 +33984,7 @@
       </c>
       <c r="I995" s="31"/>
     </row>
-    <row r="996" spans="1:9" ht="60">
+    <row r="996" spans="1:9" ht="45">
       <c r="A996" s="29" t="s">
         <v>998</v>
       </c>
@@ -34040,7 +34040,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="998" spans="1:9" ht="75">
+    <row r="998" spans="1:9" ht="60">
       <c r="A998" s="29" t="s">
         <v>1000</v>
       </c>
@@ -34067,7 +34067,7 @@
       </c>
       <c r="I998" s="31"/>
     </row>
-    <row r="999" spans="1:9" ht="60">
+    <row r="999" spans="1:9" ht="45">
       <c r="A999" s="29" t="s">
         <v>1001</v>
       </c>
@@ -34152,7 +34152,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1002" spans="1:9" ht="75">
+    <row r="1002" spans="1:9" ht="60">
       <c r="A1002" s="29" t="s">
         <v>1002</v>
       </c>
@@ -34471,7 +34471,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1013" spans="1:9" ht="60">
+    <row r="1013" spans="1:9" ht="45">
       <c r="A1013" s="29" t="s">
         <v>1008</v>
       </c>
@@ -34500,7 +34500,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1014" spans="1:9" ht="60">
+    <row r="1014" spans="1:9" ht="45">
       <c r="A1014" s="22" t="s">
         <v>1009</v>
       </c>
@@ -34556,7 +34556,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1016" spans="1:9" ht="60">
+    <row r="1016" spans="1:9" ht="45">
       <c r="A1016" s="29" t="s">
         <v>1011</v>
       </c>
@@ -34757,7 +34757,7 @@
         <v>2204</v>
       </c>
     </row>
-    <row r="1023" spans="1:9" ht="60">
+    <row r="1023" spans="1:9" ht="45">
       <c r="A1023" s="34" t="s">
         <v>2371</v>
       </c>
@@ -34784,7 +34784,7 @@
       </c>
       <c r="I1023" s="31"/>
     </row>
-    <row r="1024" spans="1:9" ht="60">
+    <row r="1024" spans="1:9" ht="45">
       <c r="A1024" s="34" t="s">
         <v>2372</v>
       </c>
@@ -34865,7 +34865,7 @@
       </c>
       <c r="I1026" s="31"/>
     </row>
-    <row r="1027" spans="1:9" ht="75">
+    <row r="1027" spans="1:9" ht="60">
       <c r="A1027" s="34" t="s">
         <v>2375</v>
       </c>
@@ -35154,7 +35154,7 @@
       </c>
       <c r="I1037" s="31"/>
     </row>
-    <row r="1038" spans="1:9" ht="60">
+    <row r="1038" spans="1:9" ht="45">
       <c r="A1038" s="29" t="s">
         <v>1024</v>
       </c>
@@ -36260,6 +36260,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36267,14 +36272,9 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
+  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A521:I1029 A251:I518">
     <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36285,7 +36285,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
+  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A521:I1029 A251:I518">
     <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>

</xml_diff>

<commit_message>
Task 1887607 and 1887609.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7675" uniqueCount="2418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7677" uniqueCount="2420">
   <si>
     <t>Req ID</t>
   </si>
@@ -7580,6 +7580,14 @@
   </si>
   <si>
     <t>Test Case</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Verified by derived requirements: MS-OXCFOLD_R271501, MS-OXCFOLD_R271502.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19.2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -7920,242 +7928,6 @@
   </cellStyles>
   <dxfs count="63">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -8493,6 +8265,242 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8622,34 +8630,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1079" tableType="xml" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1079" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1079" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="59">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="58">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="57">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="52">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8658,12 +8666,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8993,8 +9001,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1080"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A973" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C995" sqref="C995"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9037,14 +9045,14 @@
       <c r="B3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="33">
-        <v>14.1</v>
+      <c r="C3" s="33" t="s">
+        <v>2419</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>42261</v>
+        <v>42997</v>
       </c>
       <c r="J3" s="5"/>
     </row>
@@ -16847,7 +16855,7 @@
         <v>2136</v>
       </c>
     </row>
-    <row r="318" spans="1:9" ht="30">
+    <row r="318" spans="1:9" ht="45">
       <c r="A318" s="22" t="s">
         <v>2394</v>
       </c>
@@ -16870,7 +16878,9 @@
       <c r="H318" s="22" t="s">
         <v>2401</v>
       </c>
-      <c r="I318" s="31"/>
+      <c r="I318" s="20" t="s">
+        <v>2418</v>
+      </c>
     </row>
     <row r="319" spans="1:9" ht="30">
       <c r="A319" s="29" t="s">
@@ -36272,166 +36282,166 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1029:I1079 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1027">
-    <cfRule type="expression" dxfId="43" priority="107">
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="108">
+    <cfRule type="expression" dxfId="61" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="115">
+    <cfRule type="expression" dxfId="60" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246:I246 A1029:I1079 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1027">
-    <cfRule type="expression" dxfId="40" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="62">
+    <cfRule type="expression" dxfId="58" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="63">
+    <cfRule type="expression" dxfId="57" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F246 F1030:F1079 F20:F241 F521:F1027 F251:F518">
-    <cfRule type="expression" dxfId="37" priority="67">
+    <cfRule type="expression" dxfId="56" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="68">
+    <cfRule type="expression" dxfId="55" priority="68">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1030:I1079 I230 I233:I241">
-    <cfRule type="expression" dxfId="35" priority="58">
+    <cfRule type="expression" dxfId="54" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="59">
+    <cfRule type="expression" dxfId="53" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="60">
+    <cfRule type="expression" dxfId="52" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1030:I1079 I230 I233:I241">
-    <cfRule type="expression" dxfId="32" priority="55">
+    <cfRule type="expression" dxfId="51" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="56">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="57">
+    <cfRule type="expression" dxfId="49" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1029">
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="48" priority="38">
       <formula>NOT(VLOOKUP(F1029,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="47" priority="39">
       <formula>(VLOOKUP(F1029,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1029">
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="46" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="33">
+    <cfRule type="expression" dxfId="45" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1029">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="43" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="42" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="41" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1028 C1028:I1028">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="27">
+    <cfRule type="expression" dxfId="39" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="28">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1028 C1028:I1028">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1028">
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>NOT(VLOOKUP(F1028,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>(VLOOKUP(F1028,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1028">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1028">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F519:F520">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -36462,7 +36472,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="C3 B996:B1080 B19:B993" numberStoredAsText="1"/>
+    <ignoredError sqref="B996:B1080 B19:B993" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
[MAPI package] fomart the Requirement Specification.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4237CC5-E74B-476D-ACD3-9FFFFAFFE23A}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570"/>
+    <workbookView xWindow="-15" yWindow="60" windowWidth="15405" windowHeight="6900" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -20,8 +21,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="tmpF9CB" type="4" refreshedVersion="0" background="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="tmpF9CB" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\v-xiaoyj\AppData\Local\Temp\tmpF9CB.tmp" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
@@ -7614,7 +7615,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="0.0.0"/>
@@ -7962,242 +7963,6 @@
   </cellStyles>
   <dxfs count="63">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -8535,6 +8300,242 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8664,34 +8665,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Requirement" displayName="Requirement" ref="A19:I1082" tableType="xml" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" connectionId="1">
-  <autoFilter ref="A19:I1082"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1082" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1082" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="59">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" uniqueName="ns1:Description" name="Description" dataDxfId="58">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" uniqueName="ns1:Derived" name="Derived" dataDxfId="57">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" uniqueName="ns1:Scope" name="Scope" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" uniqueName="ns1:Verification" name="Verification" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="52">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8700,12 +8701,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
-  <autoFilter ref="A12:C15"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
+  <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Scope" dataDxfId="46"/>
-    <tableColumn id="2" name="Test" dataDxfId="45"/>
-    <tableColumn id="3" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8787,6 +8788,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -8822,6 +8840,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -8997,18 +9032,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1083"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A981" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C983" sqref="C983"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="11" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="11" customWidth="1"/>
+    <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="85" style="3" customWidth="1"/>
     <col min="4" max="4" width="28.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
@@ -36369,187 +36402,187 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">
-    <cfRule type="expression" dxfId="43" priority="107">
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="108">
+    <cfRule type="expression" dxfId="61" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="115">
+    <cfRule type="expression" dxfId="60" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">
-    <cfRule type="expression" dxfId="40" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="62">
+    <cfRule type="expression" dxfId="58" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="63">
+    <cfRule type="expression" dxfId="57" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F246 F1033:F1082 F20:F241 F251:F518 F521:F1030">
-    <cfRule type="expression" dxfId="37" priority="67">
+    <cfRule type="expression" dxfId="56" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="68">
+    <cfRule type="expression" dxfId="55" priority="68">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1033:I1082 I230 I233:I241">
-    <cfRule type="expression" dxfId="35" priority="58">
+    <cfRule type="expression" dxfId="54" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="59">
+    <cfRule type="expression" dxfId="53" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="60">
+    <cfRule type="expression" dxfId="52" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1033:I1082 I230 I233:I241">
-    <cfRule type="expression" dxfId="32" priority="55">
+    <cfRule type="expression" dxfId="51" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="56">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="57">
+    <cfRule type="expression" dxfId="49" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1032">
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="48" priority="38">
       <formula>NOT(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="47" priority="39">
       <formula>(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1032">
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="46" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="33">
+    <cfRule type="expression" dxfId="45" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1032">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="43" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="42" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="41" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1031 C1031:I1031">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="27">
+    <cfRule type="expression" dxfId="39" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="28">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1031 C1031:I1031">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1031">
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>NOT(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1031">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1031">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F519:F520">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1082">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1082" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1082">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1082" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1082">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1082" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H246 H1033:H1082 H20:H241 H251:H1030">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H246 H1033:H1082 H20:H241 H251:H1030" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H247:H250 H242:H245 H1031:H1032">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H247:H250 H242:H245 H1031:H1032" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case, Deleted"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36559,7 +36592,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1019:B1040 B992:B995 B19:B989 B1083 B998:B1017" numberStoredAsText="1"/>
+    <ignoredError sqref="B1018:B1082 B991:B997 B19:B990 B1083 B998:B1017 C3" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Updated RS and ptfconfig for MS-OXCFOLD. Updated S01 and S02 for MS-OXCFOLD. In the SHOULDMAY file, R106601Enabled and R106602Enabled should be set according to the actual situation since TDI is set to 'false' first.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ECF757B-1FAC-4ECF-A9F0-D8DEFE17E5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436B72D9-A79D-434F-8B2B-08BC25E1A5AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1082</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Requirements!$A$19:$G$1081</definedName>
     <definedName name="ExtensionList">Requirements!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Requirements!$A:$A,Requirements!$19:$19</definedName>
     <definedName name="ScopeList">Requirements!#REF!</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7704" uniqueCount="2430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7695" uniqueCount="2428">
   <si>
     <t>Req ID</t>
   </si>
@@ -7296,15 +7296,6 @@
     <t>Verified by derived requirements: MS-OXCFOLD_R764001, MS-OXCFOLD_R764002.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] If this bit [DELETE_HARD_DELETE] is set, implement does not hard delete the folder. (Microsoft Exchange server 2013 and above follow this behavior).</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] If this bit [DELETE_HARD_DELETE] is set, implement does hard delete the folder. &lt;4&gt; Section 2.2.1.3.1:  For Exchange 2003, Exchange 2007 and Exchange 2010, if DELETE_HARD_DELETE is set, the folder is hard deleted.</t>
-  </si>
-  <si>
-    <t>MS-OXCFOLD_R764001</t>
-  </si>
-  <si>
     <t>MS-OXCFOLD_R764002</t>
   </si>
   <si>
@@ -7506,21 +7497,12 @@
     <t>[In Appendix A: Product Behavior] Implementation does not support the RopHardDeleteMessagesAndSubfolders ROP ([MS-OXCROPS] section 2.2.4.10) for public folders. &lt;8&gt; Section 2.2.1.10: Exchange 2013, Exchange 2016 and Exchange 2019 do not support the RopHardDeleteMessagesAndSubfolders ROP ([MS-OXCROPS] section 2.2.4.10) for public folders.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] The implementation does not support the PidTagAddressBookEntryId property. &lt;10&gt; Section 2.2.2.2.1.4:  Exchange 2013, Exchange 2016 and Exchange 2019 do not support the PidTagAddressBookEntryId property.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] Implementation returns ecAccessdenied if the client does not have permissions to create the folder. &lt;13&gt; Section 3.2.5.2: Exchange 2007, Exchange 2013, Exchange 2016 and Exchange 2019 return ecAccessdenied.</t>
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] If the ROP was called to create a search folder on a public folders message store, the implemetation does return ecNotSupported. &lt;14&gt; Exchange 2007, Exchange 2013, Exchange 2016 and Exchange 2019 return ecNotSupported.</t>
   </si>
   <si>
-    <t>[In Appendix A: Product Behavior] Implementation does ignore invalid bits instead of failing the ROP [RopDeleteFolder], if the client sets an invalid bit in the DeleteFolderFlags field of the ROP request buffer. &lt;15&gt; Section 3.2.5.3:  Exchange 2010, Exchange 2013, Exchange 2016 and Exchange 2019 ignore invalid bits instead of failing the ROP.</t>
-  </si>
-  <si>
-    <t>[In Appendix A: Product Behavior] Implementation does return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder. &lt;20&gt; Section 3.2.5.9: Update Rollup 4 for Exchange Server 2010 Service Pack 2 (SP2), Exchange 2013, Exchange 2016 and Exchange 2019 return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder.</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] If the client sets an invalid bit in the SearchFlags field, implementation does fail the RopSetSearchCriteria ROP operation with ecInvalidParam (0x80070057). (Microsoft Exchange 2010, Microsoft Exchange 2013 and Microsoft Exchange 2016 follow this behavior.)</t>
   </si>
   <si>
@@ -7533,83 +7515,94 @@
     <t>[In Appendix A: Product Behavior] If rules are associated with the folder, implementation does set a zero value to HasRules field. &lt;2&gt; Section 2.2.1.1.2: Exchange 2003 and Exchange 2007, Exchange 2016 and Exchange 2019 return zero (FALSE) in the HasRules field, even when there are rules on the Inbox folder.</t>
   </si>
   <si>
+    <t>[In PidTagContentCount Property] The PidTagContentCount property ([MS-OXPROPS] section 2.646) specifies the number of messages in a folder, as computed by the message store.</t>
+  </si>
+  <si>
+    <t>[In PidTagContentUnreadCount Property] The PidTagContentUnreadCount property ([MS-OXPROPS] section 2.648) specifies the number of unread messages in a folder, as computed by the message store.</t>
+  </si>
+  <si>
+    <t>[In PidTagDeletedOn Property] The PidTagDeletedOn property ([MS-OXPROPS] section 2.670) specifies the time when the folder was soft deleted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[In PidTagAddressBookEntryId Property] The PidTagAddressBookEntryId property ([MS-OXPROPS] section 2.521) contains an Address Book EntryID structure, as specified in [MS-OXCDATA] section 2.2.5.2, that specifies the name-service entry ID of a directory object that refers to a public folder. &lt;10&gt; </t>
+  </si>
+  <si>
+    <t>[In PidTagFolderFlags Property] The PidTagFolderId property ([MS-OXPROPS] section 2.701) contains a computed value that specifies the type or state of a folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagFolderId Property] The PidTagFolderId property ([MS-OXPROPS] section 2.700) contains a FID structure ([MS-OXCDATA] section 2.2.1.1) that uniquely identifies a folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagParentEntryId Property] The PidTagParentEntryId property ([MS-OXPROPS] section 2.858) contains a Folder EntryID structure, as specified in [MS-OXCDATA] section 2.2.4.1, that specifies the entry ID of the folder that contains the message or subfolder.</t>
+  </si>
+  <si>
+    <t>[In PidTagHierarchyChangeNumber Property] The PidTagHierarchyChangeNumber property ([MS-OXPROPS] section 2.720) specifies the number of subfolders in the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagMessageSize Property] The PidTagMessageSize property ([MS-OXPROPS] section 2.796) specifies the aggregate size of messages in the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagHierRev Property] The PidTagHierRev property ([MS-OXPROPS] section 2.721) specifies the time, in Coordinated Universal Time (UTC), to trigger the client in cached mode to synchronize the folder hierarchy.</t>
+  </si>
+  <si>
+    <t>[In PidTagMessageSizeExtended Property] The PidTagMessageSizeExtended property ([MS-OXPROPS] section 2.797) specifies the 64-bit version of the PidTagMessageSize property (section 2.2.2.2.1.7).</t>
+  </si>
+  <si>
+    <t>[In PidTagSubfolders Property] The PidTagSubfolders property ([MS-OXPROPS] section 2.1032) specifies whether the folder has any subfolders.</t>
+  </si>
+  <si>
+    <t>[In PidTagLocalCommitTime Property] The PidTagLocalCommitTime property ([MS-OXPROPS] section 2.772) specifies the time, in Coordinated Universal Time (UTC), that the folder was last changed.</t>
+  </si>
+  <si>
+    <t>[In PidTagLocalCommitTimeMax Property] The PidTagLocalCommitTimeMax property ([MS-OXPROPS] section 2.773) specifies the most recent time that a top level object within a folder was changed.</t>
+  </si>
+  <si>
+    <t>[In PidTagDeletedCountTotal Property] The PidTagDeletedCountTotal property ([MS-OXPROPS] section 2.669) specifies the total number of messages that have been deleted from a folder, excluding messages that have been deleted from the folder's subfolders.</t>
+  </si>
+  <si>
+    <t>[In PidTagAttributeHidden Property] The PidTagAttributeHidden property ([MS-OXPROPS] section 2.611) specifies whether the folder is hidden.</t>
+  </si>
+  <si>
+    <t>[In PidTagComment Property] The PidTagComment property ([MS-OXPROPS] section 2.637) contains a comment about the purpose or content of the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagContainerClass Property] The PidTagContainerClass property ([MS-OXPROPS] section 2.642) specifies the type of Message object that the folder contains.</t>
+  </si>
+  <si>
+    <t>[PidTagContainerHierarchy Property] The PidTagContainerHierarchy property ([MS-OXPROPS] section 2.645) contains identifiers of the subfolders that are contained in the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagDisplayName Property] The PidTagDisplayName property ([MS-OXPROPS] section 2.676) specifies the display name of the folder.</t>
+  </si>
+  <si>
+    <t>[PidTagFolderAssociatedContents Property] The PidTagFolderAssociatedContents property ([MS-OXPROPS] section 2.699) contains identifiers of the FAI messages that are contained in the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagFolderType Property] The PidTagFolderType property ([MS-OXPROPS] section 2.702) specifies the type of the folder.</t>
+  </si>
+  <si>
+    <t>[In PidTagRights Property] The PidTagRights property ([MS-OXPROPS] section 2.935) specifies the client's folder permissions.</t>
+  </si>
+  <si>
+    <t>MS-OXCFOLD</t>
+  </si>
+  <si>
     <t>MS-OXCFOLD_R114:I,MS-OXCFOLD_R764:i</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[In PidTagContentCount Property] The PidTagContentCount property ([MS-OXPROPS] section 2.646) specifies the number of messages in a folder, as computed by the message store.</t>
-  </si>
-  <si>
-    <t>[In PidTagContentUnreadCount Property] The PidTagContentUnreadCount property ([MS-OXPROPS] section 2.648) specifies the number of unread messages in a folder, as computed by the message store.</t>
-  </si>
-  <si>
-    <t>[In PidTagDeletedOn Property] The PidTagDeletedOn property ([MS-OXPROPS] section 2.670) specifies the time when the folder was soft deleted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[In PidTagAddressBookEntryId Property] The PidTagAddressBookEntryId property ([MS-OXPROPS] section 2.521) contains an Address Book EntryID structure, as specified in [MS-OXCDATA] section 2.2.5.2, that specifies the name-service entry ID of a directory object that refers to a public folder. &lt;10&gt; </t>
-  </si>
-  <si>
-    <t>[In PidTagFolderFlags Property] The PidTagFolderId property ([MS-OXPROPS] section 2.701) contains a computed value that specifies the type or state of a folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagFolderId Property] The PidTagFolderId property ([MS-OXPROPS] section 2.700) contains a FID structure ([MS-OXCDATA] section 2.2.1.1) that uniquely identifies a folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagParentEntryId Property] The PidTagParentEntryId property ([MS-OXPROPS] section 2.858) contains a Folder EntryID structure, as specified in [MS-OXCDATA] section 2.2.4.1, that specifies the entry ID of the folder that contains the message or subfolder.</t>
-  </si>
-  <si>
-    <t>[In PidTagHierarchyChangeNumber Property] The PidTagHierarchyChangeNumber property ([MS-OXPROPS] section 2.720) specifies the number of subfolders in the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagMessageSize Property] The PidTagMessageSize property ([MS-OXPROPS] section 2.796) specifies the aggregate size of messages in the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagHierRev Property] The PidTagHierRev property ([MS-OXPROPS] section 2.721) specifies the time, in Coordinated Universal Time (UTC), to trigger the client in cached mode to synchronize the folder hierarchy.</t>
-  </si>
-  <si>
-    <t>[In PidTagMessageSizeExtended Property] The PidTagMessageSizeExtended property ([MS-OXPROPS] section 2.797) specifies the 64-bit version of the PidTagMessageSize property (section 2.2.2.2.1.7).</t>
-  </si>
-  <si>
-    <t>[In PidTagSubfolders Property] The PidTagSubfolders property ([MS-OXPROPS] section 2.1032) specifies whether the folder has any subfolders.</t>
-  </si>
-  <si>
-    <t>[In PidTagLocalCommitTime Property] The PidTagLocalCommitTime property ([MS-OXPROPS] section 2.772) specifies the time, in Coordinated Universal Time (UTC), that the folder was last changed.</t>
-  </si>
-  <si>
-    <t>[In PidTagLocalCommitTimeMax Property] The PidTagLocalCommitTimeMax property ([MS-OXPROPS] section 2.773) specifies the most recent time that a top level object within a folder was changed.</t>
-  </si>
-  <si>
-    <t>[In PidTagDeletedCountTotal Property] The PidTagDeletedCountTotal property ([MS-OXPROPS] section 2.669) specifies the total number of messages that have been deleted from a folder, excluding messages that have been deleted from the folder's subfolders.</t>
-  </si>
-  <si>
-    <t>[In PidTagAttributeHidden Property] The PidTagAttributeHidden property ([MS-OXPROPS] section 2.611) specifies whether the folder is hidden.</t>
-  </si>
-  <si>
-    <t>[In PidTagComment Property] The PidTagComment property ([MS-OXPROPS] section 2.637) contains a comment about the purpose or content of the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagContainerClass Property] The PidTagContainerClass property ([MS-OXPROPS] section 2.642) specifies the type of Message object that the folder contains.</t>
-  </si>
-  <si>
-    <t>[PidTagContainerHierarchy Property] The PidTagContainerHierarchy property ([MS-OXPROPS] section 2.645) contains identifiers of the subfolders that are contained in the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagDisplayName Property] The PidTagDisplayName property ([MS-OXPROPS] section 2.676) specifies the display name of the folder.</t>
-  </si>
-  <si>
-    <t>[PidTagFolderAssociatedContents Property] The PidTagFolderAssociatedContents property ([MS-OXPROPS] section 2.699) contains identifiers of the FAI messages that are contained in the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagFolderType Property] The PidTagFolderType property ([MS-OXPROPS] section 2.702) specifies the type of the folder.</t>
-  </si>
-  <si>
-    <t>[In PidTagRights Property] The PidTagRights property ([MS-OXPROPS] section 2.935) specifies the client's folder permissions.</t>
-  </si>
-  <si>
-    <t>MS-OXCFOLD</t>
-  </si>
-  <si>
-    <t>22.0</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] If this bit [DELETE_HARD_DELETE] is set, implement does hard delete the folder. &lt;4&gt; Section 2.2.1.3.1:  For Exchange 2003 and later, if DELETE_HARD_DELETE is set, the folder is hard deleted.</t>
+  </si>
+  <si>
+    <t>23.0</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] The implementation does not support the PidTagAddressBookEntryId property. &lt;10&gt; Section 2.2.2.2.1.4:  Exchange 2013 and later do not support the PidTagAddressBookEntryId property.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does ignore invalid bits instead of failing the ROP [RopDeleteFolder], if the client sets an invalid bit in the DeleteFolderFlags field of the ROP request buffer. &lt;15&gt; Section 3.2.5.3:  Exchange 2010 and later ignore invalid bits instead of failing the ROP.</t>
+  </si>
+  <si>
+    <t>[In Appendix A: Product Behavior] Implementation does return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder. &lt;20&gt; Section 3.2.5.9: Update Rollup 4 for Exchange Server 2010 Service Pack 2 (SP2) and later return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder.</t>
   </si>
 </sst>
 </file>
@@ -7830,7 +7823,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -7914,9 +7907,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -8669,8 +8659,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1082" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
-  <autoFilter ref="A19:I1082" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1081" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
+  <autoFilter ref="A19:I1081" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
@@ -9038,18 +9028,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:L1083"/>
+  <dimension ref="A1:L1082"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A1016" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1020" sqref="C1020"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="11" customWidth="1"/>
+    <col min="1" max="1" width="41.42578125" style="11" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
     <col min="3" max="3" width="67.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17" style="3" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" style="3" customWidth="1"/>
     <col min="6" max="6" width="12.140625" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" style="3" customWidth="1"/>
@@ -9061,7 +9051,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>2428</v>
+        <v>2421</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>27</v>
@@ -9085,138 +9075,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2429</v>
+        <v>2424</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="12">
-        <v>44308</v>
+        <v>44425</v>
       </c>
       <c r="J3" s="5"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="48" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="49"/>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
+      <c r="B4" s="48"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="48"/>
+      <c r="F4" s="48"/>
+      <c r="G4" s="48"/>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="52" t="s">
+      <c r="B5" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="53"/>
-      <c r="D5" s="53"/>
-      <c r="E5" s="53"/>
-      <c r="F5" s="53"/>
-      <c r="G5" s="53"/>
-      <c r="H5" s="53"/>
-      <c r="I5" s="53"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>2307</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="50"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="50"/>
-      <c r="D7" s="50"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="G7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="I7" s="50"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="45" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="46"/>
-      <c r="D9" s="46"/>
-      <c r="E9" s="46"/>
-      <c r="F9" s="46"/>
-      <c r="G9" s="46"/>
-      <c r="H9" s="46"/>
-      <c r="I9" s="46"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="45" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
-      <c r="I10" s="46"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="41" t="s">
+      <c r="B11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10">
@@ -9229,12 +9219,12 @@
       <c r="C12" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="42"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9247,12 +9237,12 @@
       <c r="C13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="43"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="43"/>
-      <c r="G13" s="43"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -9265,12 +9255,12 @@
       <c r="C14" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="43"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -9283,60 +9273,60 @@
       <c r="C15" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="44"/>
-      <c r="G15" s="44"/>
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:12" ht="64.5" customHeight="1">
       <c r="A17" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="46" t="s">
         <v>2305</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="48"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:12" ht="30" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="41"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="5"/>
       <c r="L18" s="4"/>
     </row>
@@ -16319,7 +16309,7 @@
         <v>1084</v>
       </c>
       <c r="C295" s="20" t="s">
-        <v>2329</v>
+        <v>2326</v>
       </c>
       <c r="D295" s="29"/>
       <c r="E295" s="29" t="s">
@@ -16346,7 +16336,7 @@
         <v>1084</v>
       </c>
       <c r="C296" s="20" t="s">
-        <v>2330</v>
+        <v>2327</v>
       </c>
       <c r="D296" s="29"/>
       <c r="E296" s="29" t="s">
@@ -16904,7 +16894,7 @@
         <v>1086</v>
       </c>
       <c r="C318" s="20" t="s">
-        <v>2331</v>
+        <v>2328</v>
       </c>
       <c r="D318" s="29"/>
       <c r="E318" s="29" t="s">
@@ -17008,7 +16998,7 @@
         <v>1087</v>
       </c>
       <c r="C322" s="20" t="s">
-        <v>2332</v>
+        <v>2329</v>
       </c>
       <c r="D322" s="29"/>
       <c r="E322" s="29" t="s">
@@ -17514,7 +17504,7 @@
         <v>1090</v>
       </c>
       <c r="C342" s="20" t="s">
-        <v>2333</v>
+        <v>2330</v>
       </c>
       <c r="D342" s="29"/>
       <c r="E342" s="29" t="s">
@@ -20411,7 +20401,7 @@
         <v>1103</v>
       </c>
       <c r="C457" s="20" t="s">
-        <v>2334</v>
+        <v>2331</v>
       </c>
       <c r="D457" s="29"/>
       <c r="E457" s="29" t="s">
@@ -21546,7 +21536,7 @@
         <v>1108</v>
       </c>
       <c r="C502" s="20" t="s">
-        <v>2405</v>
+        <v>2398</v>
       </c>
       <c r="D502" s="29"/>
       <c r="E502" s="29" t="s">
@@ -21621,7 +21611,7 @@
         <v>1109</v>
       </c>
       <c r="C505" s="20" t="s">
-        <v>2406</v>
+        <v>2399</v>
       </c>
       <c r="D505" s="29"/>
       <c r="E505" s="29" t="s">
@@ -21671,7 +21661,7 @@
         <v>1110</v>
       </c>
       <c r="C507" s="20" t="s">
-        <v>2407</v>
+        <v>2400</v>
       </c>
       <c r="D507" s="29"/>
       <c r="E507" s="29" t="s">
@@ -21721,7 +21711,7 @@
         <v>1111</v>
       </c>
       <c r="C509" s="20" t="s">
-        <v>2408</v>
+        <v>2401</v>
       </c>
       <c r="D509" s="29"/>
       <c r="E509" s="29" t="s">
@@ -21736,7 +21726,7 @@
       <c r="H509" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="I509" s="31" t="s">
+      <c r="I509" s="20" t="s">
         <v>2295</v>
       </c>
     </row>
@@ -21823,7 +21813,7 @@
         <v>1112</v>
       </c>
       <c r="C513" s="20" t="s">
-        <v>2409</v>
+        <v>2402</v>
       </c>
       <c r="D513" s="29"/>
       <c r="E513" s="29" t="s">
@@ -21998,7 +21988,7 @@
         <v>1113</v>
       </c>
       <c r="C520" s="20" t="s">
-        <v>2410</v>
+        <v>2403</v>
       </c>
       <c r="D520" s="22"/>
       <c r="E520" s="22" t="s">
@@ -22048,7 +22038,7 @@
         <v>1114</v>
       </c>
       <c r="C522" s="20" t="s">
-        <v>2411</v>
+        <v>2404</v>
       </c>
       <c r="D522" s="29"/>
       <c r="E522" s="29" t="s">
@@ -22098,7 +22088,7 @@
         <v>1115</v>
       </c>
       <c r="C524" s="20" t="s">
-        <v>2412</v>
+        <v>2405</v>
       </c>
       <c r="D524" s="29"/>
       <c r="E524" s="29" t="s">
@@ -22173,7 +22163,7 @@
         <v>1116</v>
       </c>
       <c r="C527" s="20" t="s">
-        <v>2414</v>
+        <v>2407</v>
       </c>
       <c r="D527" s="34"/>
       <c r="E527" s="34" t="s">
@@ -22223,7 +22213,7 @@
         <v>1117</v>
       </c>
       <c r="C529" s="20" t="s">
-        <v>2413</v>
+        <v>2406</v>
       </c>
       <c r="D529" s="29"/>
       <c r="E529" s="29" t="s">
@@ -22273,7 +22263,7 @@
         <v>1118</v>
       </c>
       <c r="C531" s="20" t="s">
-        <v>2415</v>
+        <v>2408</v>
       </c>
       <c r="D531" s="29"/>
       <c r="E531" s="29" t="s">
@@ -22323,7 +22313,7 @@
         <v>1119</v>
       </c>
       <c r="C533" s="20" t="s">
-        <v>2416</v>
+        <v>2409</v>
       </c>
       <c r="D533" s="29"/>
       <c r="E533" s="29" t="s">
@@ -22423,7 +22413,7 @@
         <v>1120</v>
       </c>
       <c r="C537" s="20" t="s">
-        <v>2417</v>
+        <v>2410</v>
       </c>
       <c r="D537" s="29"/>
       <c r="E537" s="29" t="s">
@@ -22473,7 +22463,7 @@
         <v>2224</v>
       </c>
       <c r="C539" s="20" t="s">
-        <v>2418</v>
+        <v>2411</v>
       </c>
       <c r="D539" s="29"/>
       <c r="E539" s="29" t="s">
@@ -22548,7 +22538,7 @@
         <v>2225</v>
       </c>
       <c r="C542" s="20" t="s">
-        <v>2419</v>
+        <v>2412</v>
       </c>
       <c r="D542" s="29"/>
       <c r="E542" s="29" t="s">
@@ -22598,7 +22588,7 @@
         <v>1121</v>
       </c>
       <c r="C544" s="20" t="s">
-        <v>2420</v>
+        <v>2413</v>
       </c>
       <c r="D544" s="29"/>
       <c r="E544" s="29" t="s">
@@ -22698,7 +22688,7 @@
         <v>1122</v>
       </c>
       <c r="C548" s="20" t="s">
-        <v>2421</v>
+        <v>2414</v>
       </c>
       <c r="D548" s="29"/>
       <c r="E548" s="29" t="s">
@@ -22798,7 +22788,7 @@
         <v>1123</v>
       </c>
       <c r="C552" s="20" t="s">
-        <v>2422</v>
+        <v>2415</v>
       </c>
       <c r="D552" s="29"/>
       <c r="E552" s="29" t="s">
@@ -22873,7 +22863,7 @@
         <v>1124</v>
       </c>
       <c r="C555" s="20" t="s">
-        <v>2423</v>
+        <v>2416</v>
       </c>
       <c r="D555" s="29"/>
       <c r="E555" s="29" t="s">
@@ -22948,7 +22938,7 @@
         <v>1125</v>
       </c>
       <c r="C558" s="20" t="s">
-        <v>2424</v>
+        <v>2417</v>
       </c>
       <c r="D558" s="29"/>
       <c r="E558" s="29" t="s">
@@ -23025,7 +23015,7 @@
         <v>1126</v>
       </c>
       <c r="C561" s="20" t="s">
-        <v>2425</v>
+        <v>2418</v>
       </c>
       <c r="D561" s="29"/>
       <c r="E561" s="29" t="s">
@@ -23100,7 +23090,7 @@
         <v>1127</v>
       </c>
       <c r="C564" s="20" t="s">
-        <v>2426</v>
+        <v>2419</v>
       </c>
       <c r="D564" s="29"/>
       <c r="E564" s="29" t="s">
@@ -23277,7 +23267,7 @@
         <v>1128</v>
       </c>
       <c r="C571" s="20" t="s">
-        <v>2427</v>
+        <v>2420</v>
       </c>
       <c r="D571" s="29"/>
       <c r="E571" s="29" t="s">
@@ -23352,7 +23342,7 @@
         <v>1129</v>
       </c>
       <c r="C574" s="20" t="s">
-        <v>2335</v>
+        <v>2332</v>
       </c>
       <c r="D574" s="29"/>
       <c r="E574" s="29" t="s">
@@ -26171,7 +26161,7 @@
         <v>1145</v>
       </c>
       <c r="C685" s="20" t="s">
-        <v>2336</v>
+        <v>2333</v>
       </c>
       <c r="D685" s="29"/>
       <c r="E685" s="29" t="s">
@@ -26943,7 +26933,7 @@
         <v>1146</v>
       </c>
       <c r="C715" s="20" t="s">
-        <v>2338</v>
+        <v>2335</v>
       </c>
       <c r="D715" s="29"/>
       <c r="E715" s="29" t="s">
@@ -27272,7 +27262,7 @@
         <v>1146</v>
       </c>
       <c r="C728" s="20" t="s">
-        <v>2339</v>
+        <v>2336</v>
       </c>
       <c r="D728" s="29"/>
       <c r="E728" s="29" t="s">
@@ -28607,7 +28597,7 @@
         <v>1148</v>
       </c>
       <c r="C781" s="20" t="s">
-        <v>2340</v>
+        <v>2337</v>
       </c>
       <c r="D781" s="29"/>
       <c r="E781" s="29" t="s">
@@ -28784,7 +28774,7 @@
         <v>1148</v>
       </c>
       <c r="C788" s="20" t="s">
-        <v>2341</v>
+        <v>2338</v>
       </c>
       <c r="D788" s="29"/>
       <c r="E788" s="29" t="s">
@@ -28961,7 +28951,7 @@
         <v>1148</v>
       </c>
       <c r="C795" s="20" t="s">
-        <v>2342</v>
+        <v>2339</v>
       </c>
       <c r="D795" s="29"/>
       <c r="E795" s="29" t="s">
@@ -28988,7 +28978,7 @@
         <v>1148</v>
       </c>
       <c r="C796" s="20" t="s">
-        <v>2343</v>
+        <v>2340</v>
       </c>
       <c r="D796" s="29"/>
       <c r="E796" s="29" t="s">
@@ -31312,7 +31302,7 @@
         <v>1153</v>
       </c>
       <c r="C888" s="20" t="s">
-        <v>2344</v>
+        <v>2341</v>
       </c>
       <c r="D888" s="29"/>
       <c r="E888" s="29" t="s">
@@ -33009,7 +32999,7 @@
         <v>1157</v>
       </c>
       <c r="C955" s="20" t="s">
-        <v>2345</v>
+        <v>2342</v>
       </c>
       <c r="D955" s="29"/>
       <c r="E955" s="29" t="s">
@@ -33363,7 +33353,7 @@
         <v>1158</v>
       </c>
       <c r="C969" s="20" t="s">
-        <v>2346</v>
+        <v>2343</v>
       </c>
       <c r="D969" s="29"/>
       <c r="E969" s="29" t="s">
@@ -33438,7 +33428,7 @@
         <v>1158</v>
       </c>
       <c r="C972" s="20" t="s">
-        <v>2347</v>
+        <v>2344</v>
       </c>
       <c r="D972" s="29"/>
       <c r="E972" s="29" t="s">
@@ -33725,7 +33715,7 @@
         <v>1159</v>
       </c>
       <c r="C983" s="20" t="s">
-        <v>2388</v>
+        <v>2385</v>
       </c>
       <c r="D983" s="29" t="s">
         <v>2053</v>
@@ -33810,7 +33800,7 @@
         <v>1159</v>
       </c>
       <c r="C986" s="20" t="s">
-        <v>2403</v>
+        <v>2397</v>
       </c>
       <c r="D986" s="29" t="s">
         <v>2054</v>
@@ -33839,7 +33829,7 @@
         <v>1159</v>
       </c>
       <c r="C987" s="20" t="s">
-        <v>2348</v>
+        <v>2345</v>
       </c>
       <c r="D987" s="29" t="s">
         <v>2054</v>
@@ -33868,7 +33858,7 @@
         <v>1159</v>
       </c>
       <c r="C988" s="20" t="s">
-        <v>2389</v>
+        <v>2386</v>
       </c>
       <c r="D988" s="29" t="s">
         <v>2055</v>
@@ -33916,18 +33906,18 @@
       </c>
       <c r="I989" s="31"/>
     </row>
-    <row r="990" spans="1:9" ht="45">
+    <row r="990" spans="1:9" ht="60">
       <c r="A990" s="37" t="s">
-        <v>2327</v>
+        <v>2325</v>
       </c>
       <c r="B990" s="38" t="s">
         <v>1159</v>
       </c>
-      <c r="C990" s="39" t="s">
-        <v>2325</v>
+      <c r="C990" s="20" t="s">
+        <v>2423</v>
       </c>
       <c r="D990" s="22" t="s">
-        <v>2404</v>
+        <v>2422</v>
       </c>
       <c r="E990" s="29" t="s">
         <v>22</v>
@@ -33945,18 +33935,18 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="991" spans="1:9" ht="60">
-      <c r="A991" s="37" t="s">
-        <v>2328</v>
-      </c>
-      <c r="B991" s="38" t="s">
+    <row r="991" spans="1:9" ht="75">
+      <c r="A991" s="22" t="s">
+        <v>988</v>
+      </c>
+      <c r="B991" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C991" s="39" t="s">
-        <v>2326</v>
-      </c>
-      <c r="D991" s="22" t="s">
-        <v>2404</v>
+      <c r="C991" s="20" t="s">
+        <v>2387</v>
+      </c>
+      <c r="D991" s="29" t="s">
+        <v>2056</v>
       </c>
       <c r="E991" s="29" t="s">
         <v>22</v>
@@ -33968,21 +33958,19 @@
         <v>15</v>
       </c>
       <c r="H991" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I991" s="31" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="992" spans="1:9" ht="75">
+        <v>18</v>
+      </c>
+      <c r="I991" s="31"/>
+    </row>
+    <row r="992" spans="1:9" ht="60">
       <c r="A992" s="22" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="B992" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C992" s="20" t="s">
-        <v>2390</v>
+        <v>1992</v>
       </c>
       <c r="D992" s="29" t="s">
         <v>2056</v>
@@ -33997,22 +33985,24 @@
         <v>15</v>
       </c>
       <c r="H992" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I992" s="31"/>
-    </row>
-    <row r="993" spans="1:9" ht="60">
+        <v>20</v>
+      </c>
+      <c r="I992" s="31" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="993" spans="1:9" ht="75">
       <c r="A993" s="22" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="B993" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C993" s="20" t="s">
-        <v>1992</v>
+        <v>2388</v>
       </c>
       <c r="D993" s="29" t="s">
-        <v>2056</v>
+        <v>2057</v>
       </c>
       <c r="E993" s="29" t="s">
         <v>22</v>
@@ -34030,21 +34020,21 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="994" spans="1:9" ht="75">
+    <row r="994" spans="1:9" ht="60">
       <c r="A994" s="22" t="s">
-        <v>990</v>
+        <v>2318</v>
       </c>
       <c r="B994" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C994" s="20" t="s">
-        <v>2391</v>
-      </c>
-      <c r="D994" s="29" t="s">
-        <v>2057</v>
-      </c>
-      <c r="E994" s="29" t="s">
-        <v>22</v>
+        <v>2309</v>
+      </c>
+      <c r="D994" s="22" t="s">
+        <v>2310</v>
+      </c>
+      <c r="E994" s="22" t="s">
+        <v>2312</v>
       </c>
       <c r="F994" s="29" t="s">
         <v>6</v>
@@ -34053,54 +34043,54 @@
         <v>15</v>
       </c>
       <c r="H994" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I994" s="31" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="995" spans="1:9" ht="60">
+        <v>18</v>
+      </c>
+      <c r="I994" s="31"/>
+    </row>
+    <row r="995" spans="1:9" ht="45">
       <c r="A995" s="22" t="s">
-        <v>2318</v>
-      </c>
-      <c r="B995" s="30" t="s">
-        <v>1159</v>
+        <v>2319</v>
+      </c>
+      <c r="B995" s="24">
+        <v>6</v>
       </c>
       <c r="C995" s="20" t="s">
-        <v>2309</v>
+        <v>2317</v>
       </c>
       <c r="D995" s="22" t="s">
-        <v>2310</v>
+        <v>2320</v>
       </c>
       <c r="E995" s="22" t="s">
-        <v>2312</v>
-      </c>
-      <c r="F995" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G995" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H995" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I995" s="31"/>
+        <v>2313</v>
+      </c>
+      <c r="F995" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G995" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H995" s="22" t="s">
+        <v>2321</v>
+      </c>
+      <c r="I995" s="20" t="s">
+        <v>2315</v>
+      </c>
     </row>
     <row r="996" spans="1:9" ht="45">
       <c r="A996" s="22" t="s">
-        <v>2319</v>
+        <v>2308</v>
       </c>
       <c r="B996" s="24">
         <v>6</v>
       </c>
       <c r="C996" s="20" t="s">
-        <v>2317</v>
+        <v>2389</v>
       </c>
       <c r="D996" s="22" t="s">
-        <v>2320</v>
+        <v>2311</v>
       </c>
       <c r="E996" s="22" t="s">
-        <v>2313</v>
+        <v>2314</v>
       </c>
       <c r="F996" s="22" t="s">
         <v>6</v>
@@ -34109,50 +34099,48 @@
         <v>15</v>
       </c>
       <c r="H996" s="22" t="s">
-        <v>2321</v>
+        <v>20</v>
       </c>
       <c r="I996" s="20" t="s">
-        <v>2315</v>
-      </c>
-    </row>
-    <row r="997" spans="1:9" ht="45">
-      <c r="A997" s="22" t="s">
-        <v>2308</v>
-      </c>
-      <c r="B997" s="24">
-        <v>6</v>
+        <v>2316</v>
+      </c>
+    </row>
+    <row r="997" spans="1:9" ht="75">
+      <c r="A997" s="29" t="s">
+        <v>991</v>
+      </c>
+      <c r="B997" s="30" t="s">
+        <v>1159</v>
       </c>
       <c r="C997" s="20" t="s">
-        <v>2392</v>
-      </c>
-      <c r="D997" s="22" t="s">
-        <v>2311</v>
-      </c>
-      <c r="E997" s="22" t="s">
-        <v>2314</v>
-      </c>
-      <c r="F997" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G997" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H997" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="I997" s="20" t="s">
-        <v>2316</v>
-      </c>
-    </row>
-    <row r="998" spans="1:9" ht="75">
+        <v>2390</v>
+      </c>
+      <c r="D997" s="29" t="s">
+        <v>2058</v>
+      </c>
+      <c r="E997" s="29" t="s">
+        <v>22</v>
+      </c>
+      <c r="F997" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G997" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H997" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="I997" s="31"/>
+    </row>
+    <row r="998" spans="1:9" ht="60">
       <c r="A998" s="29" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="B998" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C998" s="20" t="s">
-        <v>2393</v>
+      <c r="C998" s="31" t="s">
+        <v>1993</v>
       </c>
       <c r="D998" s="29" t="s">
         <v>2058</v>
@@ -34167,22 +34155,24 @@
         <v>15</v>
       </c>
       <c r="H998" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I998" s="31"/>
-    </row>
-    <row r="999" spans="1:9" ht="60">
+        <v>20</v>
+      </c>
+      <c r="I998" s="20" t="s">
+        <v>2315</v>
+      </c>
+    </row>
+    <row r="999" spans="1:9" ht="90">
       <c r="A999" s="29" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="B999" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C999" s="31" t="s">
-        <v>1993</v>
+      <c r="C999" s="20" t="s">
+        <v>2391</v>
       </c>
       <c r="D999" s="29" t="s">
-        <v>2058</v>
+        <v>2059</v>
       </c>
       <c r="E999" s="29" t="s">
         <v>22</v>
@@ -34194,21 +34184,19 @@
         <v>15</v>
       </c>
       <c r="H999" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I999" s="20" t="s">
-        <v>2315</v>
-      </c>
-    </row>
-    <row r="1000" spans="1:9" ht="90">
+        <v>18</v>
+      </c>
+      <c r="I999" s="31"/>
+    </row>
+    <row r="1000" spans="1:9" ht="60">
       <c r="A1000" s="29" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="B1000" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C1000" s="20" t="s">
-        <v>2394</v>
+      <c r="C1000" s="31" t="s">
+        <v>1994</v>
       </c>
       <c r="D1000" s="29" t="s">
         <v>2059</v>
@@ -34223,51 +34211,51 @@
         <v>15</v>
       </c>
       <c r="H1000" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1000" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I1000" s="31" t="s">
+        <v>2155</v>
+      </c>
     </row>
     <row r="1001" spans="1:9" ht="60">
-      <c r="A1001" s="29" t="s">
-        <v>994</v>
-      </c>
-      <c r="B1001" s="30" t="s">
+      <c r="A1001" s="34" t="s">
+        <v>2286</v>
+      </c>
+      <c r="B1001" s="36" t="s">
         <v>1159</v>
       </c>
-      <c r="C1001" s="31" t="s">
-        <v>1994</v>
-      </c>
-      <c r="D1001" s="29" t="s">
-        <v>2059</v>
+      <c r="C1001" s="20" t="s">
+        <v>2425</v>
+      </c>
+      <c r="D1001" s="34" t="s">
+        <v>2288</v>
       </c>
       <c r="E1001" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1001" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1001" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1001" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1001" s="31" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="1002" spans="1:9" ht="60">
-      <c r="A1002" s="34" t="s">
-        <v>2286</v>
+      <c r="F1001" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1001" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1001" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1001" s="35"/>
+    </row>
+    <row r="1002" spans="1:9" ht="45">
+      <c r="A1002" s="22" t="s">
+        <v>2287</v>
       </c>
       <c r="B1002" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1002" s="20" t="s">
-        <v>2395</v>
-      </c>
-      <c r="D1002" s="34" t="s">
-        <v>2288</v>
+        <v>2294</v>
+      </c>
+      <c r="D1002" s="22" t="s">
+        <v>2299</v>
       </c>
       <c r="E1002" s="29" t="s">
         <v>22</v>
@@ -34279,48 +34267,50 @@
         <v>15</v>
       </c>
       <c r="H1002" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1002" s="35"/>
-    </row>
-    <row r="1003" spans="1:9" ht="45">
-      <c r="A1003" s="22" t="s">
-        <v>2287</v>
-      </c>
-      <c r="B1003" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1002" s="31" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:9" ht="90">
+      <c r="A1003" s="29" t="s">
+        <v>995</v>
+      </c>
+      <c r="B1003" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1003" s="20" t="s">
-        <v>2294</v>
-      </c>
-      <c r="D1003" s="22" t="s">
-        <v>2299</v>
+        <v>2334</v>
+      </c>
+      <c r="D1003" s="29" t="s">
+        <v>2060</v>
       </c>
       <c r="E1003" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1003" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1003" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1003" s="34" t="s">
+      <c r="F1003" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1003" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1003" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1003" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1004" spans="1:9" ht="90">
+    <row r="1004" spans="1:9" ht="60">
       <c r="A1004" s="29" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="B1004" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1004" s="20" t="s">
-        <v>2337</v>
+        <v>1995</v>
       </c>
       <c r="D1004" s="29" t="s">
         <v>2060</v>
@@ -34343,16 +34333,16 @@
     </row>
     <row r="1005" spans="1:9" ht="60">
       <c r="A1005" s="29" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="B1005" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1005" s="20" t="s">
-        <v>1995</v>
+        <v>2392</v>
       </c>
       <c r="D1005" s="29" t="s">
-        <v>2060</v>
+        <v>2061</v>
       </c>
       <c r="E1005" s="29" t="s">
         <v>22</v>
@@ -34372,13 +34362,13 @@
     </row>
     <row r="1006" spans="1:9" ht="60">
       <c r="A1006" s="29" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="B1006" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1006" s="20" t="s">
-        <v>2396</v>
+        <v>2346</v>
       </c>
       <c r="D1006" s="29" t="s">
         <v>2061</v>
@@ -34399,18 +34389,18 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="1007" spans="1:9" ht="60">
-      <c r="A1007" s="29" t="s">
-        <v>998</v>
-      </c>
-      <c r="B1007" s="30" t="s">
+    <row r="1007" spans="1:9" ht="45">
+      <c r="A1007" s="22" t="s">
+        <v>2303</v>
+      </c>
+      <c r="B1007" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1007" s="20" t="s">
-        <v>2349</v>
-      </c>
-      <c r="D1007" s="29" t="s">
-        <v>2061</v>
+        <v>2347</v>
+      </c>
+      <c r="D1007" s="34" t="s">
+        <v>2270</v>
       </c>
       <c r="E1007" s="29" t="s">
         <v>22</v>
@@ -34421,22 +34411,22 @@
       <c r="G1007" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1007" s="29" t="s">
+      <c r="H1007" s="34" t="s">
         <v>20</v>
       </c>
       <c r="I1007" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1008" spans="1:9" ht="45">
+    <row r="1008" spans="1:9" ht="60">
       <c r="A1008" s="22" t="s">
-        <v>2303</v>
+        <v>2304</v>
       </c>
       <c r="B1008" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1008" s="20" t="s">
-        <v>2350</v>
+        <v>2393</v>
       </c>
       <c r="D1008" s="34" t="s">
         <v>2270</v>
@@ -34458,17 +34448,17 @@
       </c>
     </row>
     <row r="1009" spans="1:9" ht="60">
-      <c r="A1009" s="22" t="s">
-        <v>2304</v>
-      </c>
-      <c r="B1009" s="36" t="s">
+      <c r="A1009" s="29" t="s">
+        <v>999</v>
+      </c>
+      <c r="B1009" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1009" s="20" t="s">
-        <v>2397</v>
-      </c>
-      <c r="D1009" s="34" t="s">
-        <v>2270</v>
+        <v>2172</v>
+      </c>
+      <c r="D1009" s="29" t="s">
+        <v>2062</v>
       </c>
       <c r="E1009" s="29" t="s">
         <v>22</v>
@@ -34479,30 +34469,30 @@
       <c r="G1009" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="H1009" s="34" t="s">
+      <c r="H1009" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1009" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1010" spans="1:9" ht="60">
+    <row r="1010" spans="1:9" ht="75">
       <c r="A1010" s="29" t="s">
-        <v>999</v>
-      </c>
-      <c r="B1010" s="30" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B1010" s="24" t="s">
         <v>1159</v>
       </c>
       <c r="C1010" s="20" t="s">
-        <v>2172</v>
-      </c>
-      <c r="D1010" s="29" t="s">
+        <v>2426</v>
+      </c>
+      <c r="D1010" s="22" t="s">
         <v>2062</v>
       </c>
       <c r="E1010" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1010" s="22" t="s">
+      <c r="F1010" s="29" t="s">
         <v>6</v>
       </c>
       <c r="G1010" s="29" t="s">
@@ -34515,44 +34505,44 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="1011" spans="1:9" ht="75">
-      <c r="A1011" s="29" t="s">
-        <v>1000</v>
-      </c>
-      <c r="B1011" s="24" t="s">
+    <row r="1011" spans="1:9" ht="90">
+      <c r="A1011" s="34" t="s">
+        <v>2282</v>
+      </c>
+      <c r="B1011" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1011" s="20" t="s">
-        <v>2398</v>
+        <v>2348</v>
       </c>
       <c r="D1011" s="22" t="s">
-        <v>2062</v>
+        <v>2300</v>
       </c>
       <c r="E1011" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1011" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1011" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1011" s="29" t="s">
+      <c r="F1011" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1011" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1011" s="34" t="s">
         <v>20</v>
       </c>
       <c r="I1011" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1012" spans="1:9" ht="90">
+    <row r="1012" spans="1:9" ht="60">
       <c r="A1012" s="34" t="s">
-        <v>2282</v>
+        <v>2283</v>
       </c>
       <c r="B1012" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1012" s="20" t="s">
-        <v>2351</v>
+        <v>2297</v>
       </c>
       <c r="D1012" s="22" t="s">
         <v>2300</v>
@@ -34574,43 +34564,43 @@
       </c>
     </row>
     <row r="1013" spans="1:9" ht="60">
-      <c r="A1013" s="34" t="s">
-        <v>2283</v>
-      </c>
-      <c r="B1013" s="36" t="s">
+      <c r="A1013" s="22" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B1013" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1013" s="20" t="s">
-        <v>2297</v>
-      </c>
-      <c r="D1013" s="22" t="s">
-        <v>2300</v>
+        <v>2273</v>
+      </c>
+      <c r="D1013" s="29" t="s">
+        <v>2063</v>
       </c>
       <c r="E1013" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1013" s="34" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1013" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1013" s="34" t="s">
+      <c r="F1013" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1013" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1013" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1013" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1014" spans="1:9" ht="60">
-      <c r="A1014" s="22" t="s">
-        <v>2177</v>
+    <row r="1014" spans="1:9" ht="75">
+      <c r="A1014" s="29" t="s">
+        <v>1001</v>
       </c>
       <c r="B1014" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1014" s="20" t="s">
-        <v>2273</v>
+        <v>2349</v>
       </c>
       <c r="D1014" s="29" t="s">
         <v>2063</v>
@@ -34632,14 +34622,14 @@
       </c>
     </row>
     <row r="1015" spans="1:9" ht="75">
-      <c r="A1015" s="29" t="s">
-        <v>1001</v>
+      <c r="A1015" s="22" t="s">
+        <v>1002</v>
       </c>
       <c r="B1015" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1015" s="20" t="s">
-        <v>2352</v>
+        <v>2350</v>
       </c>
       <c r="D1015" s="29" t="s">
         <v>2063</v>
@@ -34647,31 +34637,29 @@
       <c r="E1015" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1015" s="22" t="s">
+      <c r="F1015" s="29" t="s">
         <v>6</v>
       </c>
       <c r="G1015" s="29" t="s">
         <v>15</v>
       </c>
       <c r="H1015" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1015" s="31" t="s">
-        <v>2155</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I1015" s="31"/>
     </row>
     <row r="1016" spans="1:9" ht="75">
-      <c r="A1016" s="22" t="s">
-        <v>1002</v>
+      <c r="A1016" s="29" t="s">
+        <v>1003</v>
       </c>
       <c r="B1016" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1016" s="20" t="s">
-        <v>2353</v>
+        <v>2394</v>
       </c>
       <c r="D1016" s="29" t="s">
-        <v>2063</v>
+        <v>2064</v>
       </c>
       <c r="E1016" s="29" t="s">
         <v>22</v>
@@ -34683,19 +34671,21 @@
         <v>15</v>
       </c>
       <c r="H1016" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1016" s="31"/>
-    </row>
-    <row r="1017" spans="1:9" ht="75">
-      <c r="A1017" s="29" t="s">
-        <v>1003</v>
-      </c>
-      <c r="B1017" s="30" t="s">
-        <v>1159</v>
+        <v>20</v>
+      </c>
+      <c r="I1016" s="31" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:9" ht="60">
+      <c r="A1017" s="22" t="s">
+        <v>2396</v>
+      </c>
+      <c r="B1017" s="39">
+        <v>6</v>
       </c>
       <c r="C1017" s="20" t="s">
-        <v>2400</v>
+        <v>2395</v>
       </c>
       <c r="D1017" s="29" t="s">
         <v>2064</v>
@@ -34706,25 +34696,25 @@
       <c r="F1017" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G1017" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1017" s="29" t="s">
+      <c r="G1017" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1017" s="37" t="s">
         <v>20</v>
       </c>
       <c r="I1017" s="31" t="s">
         <v>2155</v>
       </c>
     </row>
-    <row r="1018" spans="1:9" ht="60">
-      <c r="A1018" s="22" t="s">
-        <v>2402</v>
-      </c>
-      <c r="B1018" s="40">
-        <v>6</v>
+    <row r="1018" spans="1:9" ht="75">
+      <c r="A1018" s="29" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B1018" s="30" t="s">
+        <v>1159</v>
       </c>
       <c r="C1018" s="20" t="s">
-        <v>2401</v>
+        <v>2351</v>
       </c>
       <c r="D1018" s="29" t="s">
         <v>2064</v>
@@ -34735,10 +34725,10 @@
       <c r="F1018" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="G1018" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1018" s="37" t="s">
+      <c r="G1018" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1018" s="29" t="s">
         <v>20</v>
       </c>
       <c r="I1018" s="31" t="s">
@@ -34747,21 +34737,21 @@
     </row>
     <row r="1019" spans="1:9" ht="75">
       <c r="A1019" s="29" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
       <c r="B1019" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1019" s="20" t="s">
-        <v>2354</v>
-      </c>
-      <c r="D1019" s="29" t="s">
-        <v>2064</v>
+        <v>2274</v>
+      </c>
+      <c r="D1019" s="22" t="s">
+        <v>2065</v>
       </c>
       <c r="E1019" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1019" s="29" t="s">
+      <c r="F1019" s="22" t="s">
         <v>6</v>
       </c>
       <c r="G1019" s="29" t="s">
@@ -34776,13 +34766,13 @@
     </row>
     <row r="1020" spans="1:9" ht="75">
       <c r="A1020" s="29" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
       <c r="B1020" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2274</v>
+        <v>2427</v>
       </c>
       <c r="D1020" s="22" t="s">
         <v>2065</v>
@@ -34804,14 +34794,14 @@
       </c>
     </row>
     <row r="1021" spans="1:9" ht="90">
-      <c r="A1021" s="29" t="s">
-        <v>1006</v>
+      <c r="A1021" s="22" t="s">
+        <v>1007</v>
       </c>
       <c r="B1021" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1021" s="20" t="s">
-        <v>2399</v>
+        <v>2352</v>
       </c>
       <c r="D1021" s="29" t="s">
         <v>2065</v>
@@ -34826,24 +34816,22 @@
         <v>15</v>
       </c>
       <c r="H1021" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1021" s="31" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="1022" spans="1:9" ht="90">
-      <c r="A1022" s="22" t="s">
-        <v>1007</v>
+        <v>18</v>
+      </c>
+      <c r="I1021" s="31"/>
+    </row>
+    <row r="1022" spans="1:9" ht="60">
+      <c r="A1022" s="29" t="s">
+        <v>1008</v>
       </c>
       <c r="B1022" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C1022" s="20" t="s">
-        <v>2355</v>
+      <c r="C1022" s="31" t="s">
+        <v>1996</v>
       </c>
       <c r="D1022" s="29" t="s">
-        <v>2065</v>
+        <v>2066</v>
       </c>
       <c r="E1022" s="29" t="s">
         <v>22</v>
@@ -34855,22 +34843,24 @@
         <v>15</v>
       </c>
       <c r="H1022" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1022" s="31"/>
+        <v>20</v>
+      </c>
+      <c r="I1022" s="20" t="s">
+        <v>2175</v>
+      </c>
     </row>
     <row r="1023" spans="1:9" ht="60">
       <c r="A1023" s="29" t="s">
-        <v>1008</v>
+        <v>1009</v>
       </c>
       <c r="B1023" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C1023" s="31" t="s">
-        <v>1996</v>
+      <c r="C1023" s="20" t="s">
+        <v>2353</v>
       </c>
       <c r="D1023" s="29" t="s">
-        <v>2066</v>
+        <v>2067</v>
       </c>
       <c r="E1023" s="29" t="s">
         <v>22</v>
@@ -34884,19 +34874,19 @@
       <c r="H1023" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I1023" s="20" t="s">
-        <v>2175</v>
+      <c r="I1023" s="31" t="s">
+        <v>2155</v>
       </c>
     </row>
     <row r="1024" spans="1:9" ht="60">
       <c r="A1024" s="29" t="s">
-        <v>1009</v>
+        <v>1010</v>
       </c>
       <c r="B1024" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1024" s="20" t="s">
-        <v>2356</v>
+        <v>1997</v>
       </c>
       <c r="D1024" s="29" t="s">
         <v>2067</v>
@@ -34917,47 +34907,45 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="1025" spans="1:9" ht="60">
-      <c r="A1025" s="29" t="s">
-        <v>1010</v>
-      </c>
-      <c r="B1025" s="30" t="s">
+    <row r="1025" spans="1:9" ht="75">
+      <c r="A1025" s="34" t="s">
+        <v>2277</v>
+      </c>
+      <c r="B1025" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1025" s="20" t="s">
-        <v>1997</v>
-      </c>
-      <c r="D1025" s="29" t="s">
-        <v>2067</v>
+        <v>2354</v>
+      </c>
+      <c r="D1025" s="34" t="s">
+        <v>2280</v>
       </c>
       <c r="E1025" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1025" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1025" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1025" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1025" s="31" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="1026" spans="1:9" ht="75">
+      <c r="F1025" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1025" s="34" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1025" s="34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1025" s="31"/>
+    </row>
+    <row r="1026" spans="1:9" ht="60">
       <c r="A1026" s="34" t="s">
-        <v>2277</v>
+        <v>2278</v>
       </c>
       <c r="B1026" s="36" t="s">
         <v>1159</v>
       </c>
-      <c r="C1026" s="20" t="s">
-        <v>2357</v>
+      <c r="C1026" s="35" t="s">
+        <v>2276</v>
       </c>
       <c r="D1026" s="34" t="s">
-        <v>2280</v>
+        <v>2284</v>
       </c>
       <c r="E1026" s="29" t="s">
         <v>22</v>
@@ -34975,13 +34963,13 @@
     </row>
     <row r="1027" spans="1:9" ht="60">
       <c r="A1027" s="34" t="s">
-        <v>2278</v>
+        <v>2279</v>
       </c>
       <c r="B1027" s="36" t="s">
         <v>1159</v>
       </c>
       <c r="C1027" s="35" t="s">
-        <v>2276</v>
+        <v>2275</v>
       </c>
       <c r="D1027" s="34" t="s">
         <v>2284</v>
@@ -35001,41 +34989,43 @@
       <c r="I1027" s="31"/>
     </row>
     <row r="1028" spans="1:9" ht="60">
-      <c r="A1028" s="34" t="s">
-        <v>2279</v>
-      </c>
-      <c r="B1028" s="36" t="s">
+      <c r="A1028" s="22" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1028" s="30" t="s">
         <v>1159</v>
       </c>
-      <c r="C1028" s="35" t="s">
-        <v>2275</v>
-      </c>
-      <c r="D1028" s="34" t="s">
-        <v>2284</v>
+      <c r="C1028" s="20" t="s">
+        <v>2355</v>
+      </c>
+      <c r="D1028" s="29" t="s">
+        <v>2068</v>
       </c>
       <c r="E1028" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="F1028" s="34" t="s">
+      <c r="F1028" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="G1028" s="34" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1028" s="34" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1028" s="31"/>
-    </row>
-    <row r="1029" spans="1:9" ht="60">
+      <c r="G1028" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1028" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1028" s="31" t="s">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:9" ht="45">
       <c r="A1029" s="22" t="s">
-        <v>1011</v>
+        <v>2281</v>
       </c>
       <c r="B1029" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1029" s="20" t="s">
-        <v>2358</v>
+        <v>1998</v>
       </c>
       <c r="D1029" s="29" t="s">
         <v>2068</v>
@@ -35058,42 +35048,40 @@
     </row>
     <row r="1030" spans="1:9" ht="45">
       <c r="A1030" s="22" t="s">
-        <v>2281</v>
+        <v>2356</v>
       </c>
       <c r="B1030" s="30" t="s">
         <v>1159</v>
       </c>
       <c r="C1030" s="20" t="s">
-        <v>1998</v>
-      </c>
-      <c r="D1030" s="29" t="s">
-        <v>2068</v>
-      </c>
-      <c r="E1030" s="29" t="s">
+        <v>2359</v>
+      </c>
+      <c r="D1030" s="22"/>
+      <c r="E1030" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F1030" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1030" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1030" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1030" s="31" t="s">
-        <v>2155</v>
+      <c r="F1030" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1030" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1030" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I1030" s="20" t="s">
+        <v>2178</v>
       </c>
     </row>
     <row r="1031" spans="1:9" ht="45">
       <c r="A1031" s="22" t="s">
-        <v>2359</v>
-      </c>
-      <c r="B1031" s="30" t="s">
+        <v>2358</v>
+      </c>
+      <c r="B1031" s="24" t="s">
         <v>1159</v>
       </c>
       <c r="C1031" s="20" t="s">
-        <v>2362</v>
+        <v>2171</v>
       </c>
       <c r="D1031" s="22"/>
       <c r="E1031" s="22" t="s">
@@ -35109,52 +35097,50 @@
         <v>21</v>
       </c>
       <c r="I1031" s="20" t="s">
-        <v>2178</v>
-      </c>
-    </row>
-    <row r="1032" spans="1:9" ht="45">
+        <v>2155</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:9">
       <c r="A1032" s="22" t="s">
-        <v>2361</v>
-      </c>
-      <c r="B1032" s="24" t="s">
-        <v>1159</v>
+        <v>2357</v>
+      </c>
+      <c r="B1032" s="30" t="s">
+        <v>1063</v>
       </c>
       <c r="C1032" s="20" t="s">
-        <v>2171</v>
-      </c>
-      <c r="D1032" s="22"/>
-      <c r="E1032" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1032" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1032" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1032" s="22" t="s">
+        <v>1999</v>
+      </c>
+      <c r="D1032" s="29"/>
+      <c r="E1032" s="29" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1032" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1032" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1032" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="I1032" s="20" t="s">
-        <v>2155</v>
-      </c>
-    </row>
-    <row r="1033" spans="1:9">
-      <c r="A1033" s="22" t="s">
-        <v>2360</v>
+      <c r="I1032" s="31"/>
+    </row>
+    <row r="1033" spans="1:9" ht="45">
+      <c r="A1033" s="29" t="s">
+        <v>1012</v>
       </c>
       <c r="B1033" s="30" t="s">
-        <v>1063</v>
+        <v>1160</v>
       </c>
       <c r="C1033" s="20" t="s">
-        <v>1999</v>
+        <v>2000</v>
       </c>
       <c r="D1033" s="29"/>
       <c r="E1033" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1033" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1033" s="29" t="s">
         <v>15</v>
@@ -35166,13 +35152,13 @@
     </row>
     <row r="1034" spans="1:9" ht="45">
       <c r="A1034" s="29" t="s">
-        <v>1012</v>
+        <v>1013</v>
       </c>
       <c r="B1034" s="30" t="s">
         <v>1160</v>
       </c>
       <c r="C1034" s="20" t="s">
-        <v>2000</v>
+        <v>2001</v>
       </c>
       <c r="D1034" s="29"/>
       <c r="E1034" s="29" t="s">
@@ -35191,13 +35177,13 @@
     </row>
     <row r="1035" spans="1:9" ht="45">
       <c r="A1035" s="29" t="s">
-        <v>1013</v>
+        <v>1014</v>
       </c>
       <c r="B1035" s="30" t="s">
         <v>1160</v>
       </c>
       <c r="C1035" s="20" t="s">
-        <v>2001</v>
+        <v>2002</v>
       </c>
       <c r="D1035" s="29"/>
       <c r="E1035" s="29" t="s">
@@ -35214,15 +35200,15 @@
       </c>
       <c r="I1035" s="31"/>
     </row>
-    <row r="1036" spans="1:9" ht="45">
+    <row r="1036" spans="1:9" ht="60">
       <c r="A1036" s="29" t="s">
-        <v>1014</v>
+        <v>1015</v>
       </c>
       <c r="B1036" s="30" t="s">
         <v>1160</v>
       </c>
-      <c r="C1036" s="20" t="s">
-        <v>2002</v>
+      <c r="C1036" s="31" t="s">
+        <v>2003</v>
       </c>
       <c r="D1036" s="29"/>
       <c r="E1036" s="29" t="s">
@@ -35239,15 +35225,15 @@
       </c>
       <c r="I1036" s="31"/>
     </row>
-    <row r="1037" spans="1:9" ht="60">
-      <c r="A1037" s="29" t="s">
-        <v>1015</v>
+    <row r="1037" spans="1:9" ht="45">
+      <c r="A1037" s="22" t="s">
+        <v>1016</v>
       </c>
       <c r="B1037" s="30" t="s">
         <v>1160</v>
       </c>
       <c r="C1037" s="31" t="s">
-        <v>2003</v>
+        <v>2004</v>
       </c>
       <c r="D1037" s="29"/>
       <c r="E1037" s="29" t="s">
@@ -35264,15 +35250,15 @@
       </c>
       <c r="I1037" s="31"/>
     </row>
-    <row r="1038" spans="1:9" ht="45">
-      <c r="A1038" s="22" t="s">
-        <v>1016</v>
+    <row r="1038" spans="1:9" ht="75">
+      <c r="A1038" s="29" t="s">
+        <v>1017</v>
       </c>
       <c r="B1038" s="30" t="s">
         <v>1160</v>
       </c>
       <c r="C1038" s="31" t="s">
-        <v>2004</v>
+        <v>2005</v>
       </c>
       <c r="D1038" s="29"/>
       <c r="E1038" s="29" t="s">
@@ -35289,22 +35275,22 @@
       </c>
       <c r="I1038" s="31"/>
     </row>
-    <row r="1039" spans="1:9" ht="75">
+    <row r="1039" spans="1:9" ht="45">
       <c r="A1039" s="29" t="s">
-        <v>1017</v>
+        <v>1018</v>
       </c>
       <c r="B1039" s="30" t="s">
-        <v>1160</v>
-      </c>
-      <c r="C1039" s="31" t="s">
-        <v>2005</v>
+        <v>1161</v>
+      </c>
+      <c r="C1039" s="20" t="s">
+        <v>2360</v>
       </c>
       <c r="D1039" s="29"/>
       <c r="E1039" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1039" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1039" s="29" t="s">
         <v>15</v>
@@ -35314,15 +35300,15 @@
       </c>
       <c r="I1039" s="31"/>
     </row>
-    <row r="1040" spans="1:9" ht="45">
-      <c r="A1040" s="29" t="s">
-        <v>1018</v>
-      </c>
-      <c r="B1040" s="30" t="s">
-        <v>1161</v>
+    <row r="1040" spans="1:9">
+      <c r="A1040" s="22" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1040" s="24" t="s">
+        <v>2361</v>
       </c>
       <c r="C1040" s="20" t="s">
-        <v>2363</v>
+        <v>2006</v>
       </c>
       <c r="D1040" s="29"/>
       <c r="E1040" s="29" t="s">
@@ -35340,14 +35326,14 @@
       <c r="I1040" s="31"/>
     </row>
     <row r="1041" spans="1:9">
-      <c r="A1041" s="22" t="s">
-        <v>1019</v>
+      <c r="A1041" s="29" t="s">
+        <v>1020</v>
       </c>
       <c r="B1041" s="24" t="s">
-        <v>2364</v>
-      </c>
-      <c r="C1041" s="20" t="s">
-        <v>2006</v>
+        <v>2362</v>
+      </c>
+      <c r="C1041" s="31" t="s">
+        <v>2007</v>
       </c>
       <c r="D1041" s="29"/>
       <c r="E1041" s="29" t="s">
@@ -35366,20 +35352,20 @@
     </row>
     <row r="1042" spans="1:9">
       <c r="A1042" s="29" t="s">
-        <v>1020</v>
+        <v>1021</v>
       </c>
       <c r="B1042" s="24" t="s">
-        <v>2365</v>
-      </c>
-      <c r="C1042" s="31" t="s">
-        <v>2007</v>
+        <v>2363</v>
+      </c>
+      <c r="C1042" s="20" t="s">
+        <v>2008</v>
       </c>
       <c r="D1042" s="29"/>
       <c r="E1042" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1042" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1042" s="29" t="s">
         <v>15</v>
@@ -35391,20 +35377,20 @@
     </row>
     <row r="1043" spans="1:9">
       <c r="A1043" s="29" t="s">
-        <v>1021</v>
+        <v>1022</v>
       </c>
       <c r="B1043" s="24" t="s">
-        <v>2366</v>
-      </c>
-      <c r="C1043" s="20" t="s">
-        <v>2008</v>
+        <v>2364</v>
+      </c>
+      <c r="C1043" s="31" t="s">
+        <v>2009</v>
       </c>
       <c r="D1043" s="29"/>
       <c r="E1043" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1043" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1043" s="29" t="s">
         <v>15</v>
@@ -35416,13 +35402,13 @@
     </row>
     <row r="1044" spans="1:9">
       <c r="A1044" s="29" t="s">
-        <v>1022</v>
+        <v>1023</v>
       </c>
       <c r="B1044" s="24" t="s">
-        <v>2367</v>
-      </c>
-      <c r="C1044" s="31" t="s">
-        <v>2009</v>
+        <v>2365</v>
+      </c>
+      <c r="C1044" s="20" t="s">
+        <v>2010</v>
       </c>
       <c r="D1044" s="29"/>
       <c r="E1044" s="29" t="s">
@@ -35441,13 +35427,13 @@
     </row>
     <row r="1045" spans="1:9">
       <c r="A1045" s="29" t="s">
-        <v>1023</v>
+        <v>1024</v>
       </c>
       <c r="B1045" s="24" t="s">
-        <v>2368</v>
-      </c>
-      <c r="C1045" s="20" t="s">
-        <v>2010</v>
+        <v>2365</v>
+      </c>
+      <c r="C1045" s="31" t="s">
+        <v>2011</v>
       </c>
       <c r="D1045" s="29"/>
       <c r="E1045" s="29" t="s">
@@ -35465,14 +35451,14 @@
       <c r="I1045" s="31"/>
     </row>
     <row r="1046" spans="1:9">
-      <c r="A1046" s="29" t="s">
-        <v>1024</v>
+      <c r="A1046" s="22" t="s">
+        <v>1025</v>
       </c>
       <c r="B1046" s="24" t="s">
-        <v>2368</v>
-      </c>
-      <c r="C1046" s="31" t="s">
-        <v>2011</v>
+        <v>2366</v>
+      </c>
+      <c r="C1046" s="20" t="s">
+        <v>2012</v>
       </c>
       <c r="D1046" s="29"/>
       <c r="E1046" s="29" t="s">
@@ -35490,14 +35476,14 @@
       <c r="I1046" s="31"/>
     </row>
     <row r="1047" spans="1:9">
-      <c r="A1047" s="22" t="s">
-        <v>1025</v>
+      <c r="A1047" s="29" t="s">
+        <v>1026</v>
       </c>
       <c r="B1047" s="24" t="s">
-        <v>2369</v>
+        <v>2366</v>
       </c>
       <c r="C1047" s="20" t="s">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="D1047" s="29"/>
       <c r="E1047" s="29" t="s">
@@ -35516,13 +35502,13 @@
     </row>
     <row r="1048" spans="1:9">
       <c r="A1048" s="29" t="s">
-        <v>1026</v>
+        <v>1027</v>
       </c>
       <c r="B1048" s="24" t="s">
-        <v>2369</v>
+        <v>2368</v>
       </c>
       <c r="C1048" s="20" t="s">
-        <v>2013</v>
+        <v>2367</v>
       </c>
       <c r="D1048" s="29"/>
       <c r="E1048" s="29" t="s">
@@ -35541,13 +35527,13 @@
     </row>
     <row r="1049" spans="1:9">
       <c r="A1049" s="29" t="s">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B1049" s="24" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
       <c r="C1049" s="20" t="s">
-        <v>2370</v>
+        <v>2014</v>
       </c>
       <c r="D1049" s="29"/>
       <c r="E1049" s="29" t="s">
@@ -35566,20 +35552,20 @@
     </row>
     <row r="1050" spans="1:9">
       <c r="A1050" s="29" t="s">
-        <v>1028</v>
+        <v>1029</v>
       </c>
       <c r="B1050" s="24" t="s">
-        <v>2371</v>
+        <v>2369</v>
       </c>
       <c r="C1050" s="20" t="s">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="D1050" s="29"/>
       <c r="E1050" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1050" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1050" s="29" t="s">
         <v>15</v>
@@ -35591,20 +35577,20 @@
     </row>
     <row r="1051" spans="1:9">
       <c r="A1051" s="29" t="s">
-        <v>1029</v>
+        <v>1030</v>
       </c>
       <c r="B1051" s="24" t="s">
-        <v>2372</v>
-      </c>
-      <c r="C1051" s="20" t="s">
-        <v>2015</v>
+        <v>2369</v>
+      </c>
+      <c r="C1051" s="31" t="s">
+        <v>2016</v>
       </c>
       <c r="D1051" s="29"/>
       <c r="E1051" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1051" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1051" s="29" t="s">
         <v>15</v>
@@ -35616,13 +35602,13 @@
     </row>
     <row r="1052" spans="1:9">
       <c r="A1052" s="29" t="s">
-        <v>1030</v>
+        <v>1031</v>
       </c>
       <c r="B1052" s="24" t="s">
-        <v>2372</v>
-      </c>
-      <c r="C1052" s="31" t="s">
-        <v>2016</v>
+        <v>2370</v>
+      </c>
+      <c r="C1052" s="20" t="s">
+        <v>2017</v>
       </c>
       <c r="D1052" s="29"/>
       <c r="E1052" s="29" t="s">
@@ -35641,13 +35627,13 @@
     </row>
     <row r="1053" spans="1:9">
       <c r="A1053" s="29" t="s">
-        <v>1031</v>
+        <v>1032</v>
       </c>
       <c r="B1053" s="24" t="s">
-        <v>2373</v>
-      </c>
-      <c r="C1053" s="20" t="s">
-        <v>2017</v>
+        <v>2370</v>
+      </c>
+      <c r="C1053" s="31" t="s">
+        <v>2018</v>
       </c>
       <c r="D1053" s="29"/>
       <c r="E1053" s="29" t="s">
@@ -35666,13 +35652,13 @@
     </row>
     <row r="1054" spans="1:9">
       <c r="A1054" s="29" t="s">
-        <v>1032</v>
+        <v>1033</v>
       </c>
       <c r="B1054" s="24" t="s">
-        <v>2373</v>
-      </c>
-      <c r="C1054" s="31" t="s">
-        <v>2018</v>
+        <v>2371</v>
+      </c>
+      <c r="C1054" s="20" t="s">
+        <v>2019</v>
       </c>
       <c r="D1054" s="29"/>
       <c r="E1054" s="29" t="s">
@@ -35691,13 +35677,13 @@
     </row>
     <row r="1055" spans="1:9">
       <c r="A1055" s="29" t="s">
-        <v>1033</v>
+        <v>1034</v>
       </c>
       <c r="B1055" s="24" t="s">
-        <v>2374</v>
-      </c>
-      <c r="C1055" s="20" t="s">
-        <v>2019</v>
+        <v>2371</v>
+      </c>
+      <c r="C1055" s="31" t="s">
+        <v>2020</v>
       </c>
       <c r="D1055" s="29"/>
       <c r="E1055" s="29" t="s">
@@ -35716,13 +35702,13 @@
     </row>
     <row r="1056" spans="1:9">
       <c r="A1056" s="29" t="s">
-        <v>1034</v>
+        <v>1035</v>
       </c>
       <c r="B1056" s="24" t="s">
-        <v>2374</v>
-      </c>
-      <c r="C1056" s="31" t="s">
-        <v>2020</v>
+        <v>2372</v>
+      </c>
+      <c r="C1056" s="20" t="s">
+        <v>2021</v>
       </c>
       <c r="D1056" s="29"/>
       <c r="E1056" s="29" t="s">
@@ -35741,13 +35727,13 @@
     </row>
     <row r="1057" spans="1:9">
       <c r="A1057" s="29" t="s">
-        <v>1035</v>
+        <v>1036</v>
       </c>
       <c r="B1057" s="24" t="s">
-        <v>2375</v>
-      </c>
-      <c r="C1057" s="20" t="s">
-        <v>2021</v>
+        <v>2372</v>
+      </c>
+      <c r="C1057" s="31" t="s">
+        <v>2022</v>
       </c>
       <c r="D1057" s="29"/>
       <c r="E1057" s="29" t="s">
@@ -35766,13 +35752,13 @@
     </row>
     <row r="1058" spans="1:9">
       <c r="A1058" s="29" t="s">
-        <v>1036</v>
+        <v>1037</v>
       </c>
       <c r="B1058" s="24" t="s">
-        <v>2375</v>
-      </c>
-      <c r="C1058" s="31" t="s">
-        <v>2022</v>
+        <v>2373</v>
+      </c>
+      <c r="C1058" s="20" t="s">
+        <v>2023</v>
       </c>
       <c r="D1058" s="29"/>
       <c r="E1058" s="29" t="s">
@@ -35791,13 +35777,13 @@
     </row>
     <row r="1059" spans="1:9">
       <c r="A1059" s="29" t="s">
-        <v>1037</v>
+        <v>1038</v>
       </c>
       <c r="B1059" s="24" t="s">
-        <v>2376</v>
-      </c>
-      <c r="C1059" s="20" t="s">
-        <v>2023</v>
+        <v>2373</v>
+      </c>
+      <c r="C1059" s="31" t="s">
+        <v>2024</v>
       </c>
       <c r="D1059" s="29"/>
       <c r="E1059" s="29" t="s">
@@ -35816,13 +35802,13 @@
     </row>
     <row r="1060" spans="1:9">
       <c r="A1060" s="29" t="s">
-        <v>1038</v>
+        <v>1039</v>
       </c>
       <c r="B1060" s="24" t="s">
-        <v>2376</v>
-      </c>
-      <c r="C1060" s="31" t="s">
-        <v>2024</v>
+        <v>2374</v>
+      </c>
+      <c r="C1060" s="20" t="s">
+        <v>2025</v>
       </c>
       <c r="D1060" s="29"/>
       <c r="E1060" s="29" t="s">
@@ -35841,13 +35827,13 @@
     </row>
     <row r="1061" spans="1:9">
       <c r="A1061" s="29" t="s">
-        <v>1039</v>
+        <v>1040</v>
       </c>
       <c r="B1061" s="24" t="s">
-        <v>2377</v>
-      </c>
-      <c r="C1061" s="20" t="s">
-        <v>2025</v>
+        <v>2374</v>
+      </c>
+      <c r="C1061" s="31" t="s">
+        <v>2026</v>
       </c>
       <c r="D1061" s="29"/>
       <c r="E1061" s="29" t="s">
@@ -35866,13 +35852,13 @@
     </row>
     <row r="1062" spans="1:9">
       <c r="A1062" s="29" t="s">
-        <v>1040</v>
+        <v>1041</v>
       </c>
       <c r="B1062" s="24" t="s">
-        <v>2377</v>
-      </c>
-      <c r="C1062" s="31" t="s">
-        <v>2026</v>
+        <v>2375</v>
+      </c>
+      <c r="C1062" s="20" t="s">
+        <v>2027</v>
       </c>
       <c r="D1062" s="29"/>
       <c r="E1062" s="29" t="s">
@@ -35891,13 +35877,13 @@
     </row>
     <row r="1063" spans="1:9">
       <c r="A1063" s="29" t="s">
-        <v>1041</v>
+        <v>1042</v>
       </c>
       <c r="B1063" s="24" t="s">
-        <v>2378</v>
-      </c>
-      <c r="C1063" s="20" t="s">
-        <v>2027</v>
+        <v>2375</v>
+      </c>
+      <c r="C1063" s="31" t="s">
+        <v>2028</v>
       </c>
       <c r="D1063" s="29"/>
       <c r="E1063" s="29" t="s">
@@ -35916,13 +35902,13 @@
     </row>
     <row r="1064" spans="1:9">
       <c r="A1064" s="29" t="s">
-        <v>1042</v>
+        <v>1043</v>
       </c>
       <c r="B1064" s="24" t="s">
-        <v>2378</v>
-      </c>
-      <c r="C1064" s="31" t="s">
-        <v>2028</v>
+        <v>2376</v>
+      </c>
+      <c r="C1064" s="20" t="s">
+        <v>2029</v>
       </c>
       <c r="D1064" s="29"/>
       <c r="E1064" s="29" t="s">
@@ -35941,20 +35927,20 @@
     </row>
     <row r="1065" spans="1:9">
       <c r="A1065" s="29" t="s">
-        <v>1043</v>
+        <v>1044</v>
       </c>
       <c r="B1065" s="24" t="s">
-        <v>2379</v>
-      </c>
-      <c r="C1065" s="20" t="s">
-        <v>2029</v>
+        <v>2376</v>
+      </c>
+      <c r="C1065" s="31" t="s">
+        <v>2030</v>
       </c>
       <c r="D1065" s="29"/>
       <c r="E1065" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1065" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1065" s="29" t="s">
         <v>15</v>
@@ -35966,20 +35952,20 @@
     </row>
     <row r="1066" spans="1:9">
       <c r="A1066" s="29" t="s">
-        <v>1044</v>
+        <v>1045</v>
       </c>
       <c r="B1066" s="24" t="s">
-        <v>2379</v>
-      </c>
-      <c r="C1066" s="31" t="s">
-        <v>2030</v>
+        <v>2377</v>
+      </c>
+      <c r="C1066" s="20" t="s">
+        <v>2031</v>
       </c>
       <c r="D1066" s="29"/>
       <c r="E1066" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1066" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1066" s="29" t="s">
         <v>15</v>
@@ -35991,13 +35977,13 @@
     </row>
     <row r="1067" spans="1:9">
       <c r="A1067" s="29" t="s">
-        <v>1045</v>
+        <v>1046</v>
       </c>
       <c r="B1067" s="24" t="s">
-        <v>2380</v>
-      </c>
-      <c r="C1067" s="20" t="s">
-        <v>2031</v>
+        <v>2377</v>
+      </c>
+      <c r="C1067" s="31" t="s">
+        <v>2032</v>
       </c>
       <c r="D1067" s="29"/>
       <c r="E1067" s="29" t="s">
@@ -36016,13 +36002,13 @@
     </row>
     <row r="1068" spans="1:9">
       <c r="A1068" s="29" t="s">
-        <v>1046</v>
+        <v>1047</v>
       </c>
       <c r="B1068" s="24" t="s">
-        <v>2380</v>
-      </c>
-      <c r="C1068" s="31" t="s">
-        <v>2032</v>
+        <v>2378</v>
+      </c>
+      <c r="C1068" s="20" t="s">
+        <v>2033</v>
       </c>
       <c r="D1068" s="29"/>
       <c r="E1068" s="29" t="s">
@@ -36041,13 +36027,13 @@
     </row>
     <row r="1069" spans="1:9">
       <c r="A1069" s="29" t="s">
-        <v>1047</v>
+        <v>1048</v>
       </c>
       <c r="B1069" s="24" t="s">
-        <v>2381</v>
-      </c>
-      <c r="C1069" s="20" t="s">
-        <v>2033</v>
+        <v>2378</v>
+      </c>
+      <c r="C1069" s="31" t="s">
+        <v>2034</v>
       </c>
       <c r="D1069" s="29"/>
       <c r="E1069" s="29" t="s">
@@ -36065,14 +36051,14 @@
       <c r="I1069" s="31"/>
     </row>
     <row r="1070" spans="1:9">
-      <c r="A1070" s="29" t="s">
-        <v>1048</v>
+      <c r="A1070" s="22" t="s">
+        <v>1049</v>
       </c>
       <c r="B1070" s="24" t="s">
-        <v>2381</v>
-      </c>
-      <c r="C1070" s="31" t="s">
-        <v>2034</v>
+        <v>2379</v>
+      </c>
+      <c r="C1070" s="20" t="s">
+        <v>2035</v>
       </c>
       <c r="D1070" s="29"/>
       <c r="E1070" s="29" t="s">
@@ -36090,14 +36076,14 @@
       <c r="I1070" s="31"/>
     </row>
     <row r="1071" spans="1:9">
-      <c r="A1071" s="22" t="s">
-        <v>1049</v>
+      <c r="A1071" s="29" t="s">
+        <v>1050</v>
       </c>
       <c r="B1071" s="24" t="s">
-        <v>2382</v>
-      </c>
-      <c r="C1071" s="20" t="s">
-        <v>2035</v>
+        <v>2379</v>
+      </c>
+      <c r="C1071" s="31" t="s">
+        <v>2036</v>
       </c>
       <c r="D1071" s="29"/>
       <c r="E1071" s="29" t="s">
@@ -36116,13 +36102,13 @@
     </row>
     <row r="1072" spans="1:9">
       <c r="A1072" s="29" t="s">
-        <v>1050</v>
+        <v>1051</v>
       </c>
       <c r="B1072" s="24" t="s">
-        <v>2382</v>
-      </c>
-      <c r="C1072" s="31" t="s">
-        <v>2036</v>
+        <v>2380</v>
+      </c>
+      <c r="C1072" s="20" t="s">
+        <v>2037</v>
       </c>
       <c r="D1072" s="29"/>
       <c r="E1072" s="29" t="s">
@@ -36141,13 +36127,13 @@
     </row>
     <row r="1073" spans="1:9">
       <c r="A1073" s="29" t="s">
-        <v>1051</v>
+        <v>1052</v>
       </c>
       <c r="B1073" s="24" t="s">
-        <v>2383</v>
-      </c>
-      <c r="C1073" s="20" t="s">
-        <v>2037</v>
+        <v>2380</v>
+      </c>
+      <c r="C1073" s="31" t="s">
+        <v>2038</v>
       </c>
       <c r="D1073" s="29"/>
       <c r="E1073" s="29" t="s">
@@ -36165,14 +36151,14 @@
       <c r="I1073" s="31"/>
     </row>
     <row r="1074" spans="1:9">
-      <c r="A1074" s="29" t="s">
-        <v>1052</v>
+      <c r="A1074" s="22" t="s">
+        <v>1053</v>
       </c>
       <c r="B1074" s="24" t="s">
-        <v>2383</v>
-      </c>
-      <c r="C1074" s="31" t="s">
-        <v>2038</v>
+        <v>2381</v>
+      </c>
+      <c r="C1074" s="20" t="s">
+        <v>2039</v>
       </c>
       <c r="D1074" s="29"/>
       <c r="E1074" s="29" t="s">
@@ -36185,19 +36171,19 @@
         <v>15</v>
       </c>
       <c r="H1074" s="29" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I1074" s="31"/>
     </row>
     <row r="1075" spans="1:9">
-      <c r="A1075" s="22" t="s">
-        <v>1053</v>
+      <c r="A1075" s="29" t="s">
+        <v>1054</v>
       </c>
       <c r="B1075" s="24" t="s">
-        <v>2384</v>
-      </c>
-      <c r="C1075" s="20" t="s">
-        <v>2039</v>
+        <v>2381</v>
+      </c>
+      <c r="C1075" s="31" t="s">
+        <v>2040</v>
       </c>
       <c r="D1075" s="29"/>
       <c r="E1075" s="29" t="s">
@@ -36210,19 +36196,19 @@
         <v>15</v>
       </c>
       <c r="H1075" s="29" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="I1075" s="31"/>
     </row>
     <row r="1076" spans="1:9">
       <c r="A1076" s="29" t="s">
-        <v>1054</v>
+        <v>1055</v>
       </c>
       <c r="B1076" s="24" t="s">
-        <v>2384</v>
-      </c>
-      <c r="C1076" s="31" t="s">
-        <v>2040</v>
+        <v>2382</v>
+      </c>
+      <c r="C1076" s="20" t="s">
+        <v>2041</v>
       </c>
       <c r="D1076" s="29"/>
       <c r="E1076" s="29" t="s">
@@ -36241,13 +36227,13 @@
     </row>
     <row r="1077" spans="1:9">
       <c r="A1077" s="29" t="s">
-        <v>1055</v>
+        <v>1056</v>
       </c>
       <c r="B1077" s="24" t="s">
-        <v>2385</v>
-      </c>
-      <c r="C1077" s="20" t="s">
-        <v>2041</v>
+        <v>2382</v>
+      </c>
+      <c r="C1077" s="31" t="s">
+        <v>2042</v>
       </c>
       <c r="D1077" s="29"/>
       <c r="E1077" s="29" t="s">
@@ -36266,13 +36252,13 @@
     </row>
     <row r="1078" spans="1:9">
       <c r="A1078" s="29" t="s">
-        <v>1056</v>
+        <v>1057</v>
       </c>
       <c r="B1078" s="24" t="s">
-        <v>2385</v>
-      </c>
-      <c r="C1078" s="31" t="s">
-        <v>2042</v>
+        <v>2383</v>
+      </c>
+      <c r="C1078" s="20" t="s">
+        <v>2043</v>
       </c>
       <c r="D1078" s="29"/>
       <c r="E1078" s="29" t="s">
@@ -36291,20 +36277,20 @@
     </row>
     <row r="1079" spans="1:9">
       <c r="A1079" s="29" t="s">
-        <v>1057</v>
+        <v>1058</v>
       </c>
       <c r="B1079" s="24" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C1079" s="20" t="s">
-        <v>2043</v>
+        <v>2383</v>
+      </c>
+      <c r="C1079" s="31" t="s">
+        <v>2044</v>
       </c>
       <c r="D1079" s="29"/>
       <c r="E1079" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1079" s="29" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G1079" s="29" t="s">
         <v>15</v>
@@ -36316,20 +36302,20 @@
     </row>
     <row r="1080" spans="1:9">
       <c r="A1080" s="29" t="s">
-        <v>1058</v>
+        <v>1059</v>
       </c>
       <c r="B1080" s="24" t="s">
-        <v>2386</v>
-      </c>
-      <c r="C1080" s="31" t="s">
-        <v>2044</v>
+        <v>2384</v>
+      </c>
+      <c r="C1080" s="20" t="s">
+        <v>2045</v>
       </c>
       <c r="D1080" s="29"/>
       <c r="E1080" s="29" t="s">
         <v>19</v>
       </c>
       <c r="F1080" s="29" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G1080" s="29" t="s">
         <v>15</v>
@@ -36341,13 +36327,13 @@
     </row>
     <row r="1081" spans="1:9">
       <c r="A1081" s="29" t="s">
-        <v>1059</v>
+        <v>1060</v>
       </c>
       <c r="B1081" s="24" t="s">
-        <v>2387</v>
-      </c>
-      <c r="C1081" s="20" t="s">
-        <v>2045</v>
+        <v>2384</v>
+      </c>
+      <c r="C1081" s="31" t="s">
+        <v>2046</v>
       </c>
       <c r="D1081" s="29"/>
       <c r="E1081" s="29" t="s">
@@ -36365,33 +36351,8 @@
       <c r="I1081" s="31"/>
     </row>
     <row r="1082" spans="1:9">
-      <c r="A1082" s="29" t="s">
-        <v>1060</v>
-      </c>
-      <c r="B1082" s="24" t="s">
-        <v>2387</v>
-      </c>
-      <c r="C1082" s="31" t="s">
-        <v>2046</v>
-      </c>
-      <c r="D1082" s="29"/>
-      <c r="E1082" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1082" s="29" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1082" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1082" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1082" s="31"/>
-    </row>
-    <row r="1083" spans="1:9">
-      <c r="A1083" s="3"/>
-      <c r="B1083" s="10"/>
+      <c r="A1082" s="3"/>
+      <c r="B1082" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -36409,7 +36370,7 @@
     <mergeCell ref="B17:I17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">
+  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
     <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36420,7 +36381,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A246:I246 A1032:I1082 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1030">
+  <conditionalFormatting sqref="A246:I246 A1031:I1081 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1029">
     <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -36431,7 +36392,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F246 F1033:F1082 F20:F241 F251:F518 F521:F1030">
+  <conditionalFormatting sqref="F246 F1032:F1081 F20:F241 F251:F518 F521:F1029">
     <cfRule type="expression" dxfId="56" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
@@ -36439,7 +36400,7 @@
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I246 I1033:I1082 I230 I233:I241">
+  <conditionalFormatting sqref="I246 I1032:I1081 I230 I233:I241">
     <cfRule type="expression" dxfId="54" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36450,7 +36411,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I246 I1033:I1082 I230 I233:I241">
+  <conditionalFormatting sqref="I246 I1032:I1081 I230 I233:I241">
     <cfRule type="expression" dxfId="51" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -36461,15 +36422,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1032">
+  <conditionalFormatting sqref="F1031">
     <cfRule type="expression" dxfId="48" priority="38">
-      <formula>NOT(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="47" priority="39">
-      <formula>(VLOOKUP(F1032,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1032">
+  <conditionalFormatting sqref="I1031">
     <cfRule type="expression" dxfId="46" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36480,7 +36441,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I1032">
+  <conditionalFormatting sqref="I1031">
     <cfRule type="expression" dxfId="43" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -36491,7 +36452,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1031 C1031:I1031">
+  <conditionalFormatting sqref="A1030 C1030:I1030">
     <cfRule type="expression" dxfId="40" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36502,7 +36463,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1031 C1031:I1031">
+  <conditionalFormatting sqref="A1030 C1030:I1030">
     <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -36513,15 +36474,15 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F1031">
+  <conditionalFormatting sqref="F1030">
     <cfRule type="expression" dxfId="34" priority="24">
-      <formula>NOT(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>NOT(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
     <cfRule type="expression" dxfId="33" priority="25">
-      <formula>(VLOOKUP(F1031,$A$12:$C$15,2,FALSE)="In")</formula>
+      <formula>(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1031">
+  <conditionalFormatting sqref="B1030">
     <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
@@ -36532,7 +36493,7 @@
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1031">
+  <conditionalFormatting sqref="B1030">
     <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
@@ -36574,23 +36535,23 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1082" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F4 F20:F1081" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$A$13:$A$15</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1082" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4 E20:E1081" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Protocol,Product"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1082" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4 G20:G1081" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Informative,Normative"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:B15" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"In, Out"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H246 H1033:H1082 H20:H241 H251:H1030" xr:uid="{00000000-0002-0000-0000-000005000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H246 H1032:H1081 H20:H241 H251:H1029" xr:uid="{00000000-0002-0000-0000-000005000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H247:H250 H242:H245 H1031:H1032" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H247:H250 H242:H245 H1030:H1031" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>"Non-testable, Unverified, Adapter, Test Case, Deleted"</formula1>
     </dataValidation>
   </dataValidations>
@@ -36600,7 +36561,7 @@
     <oddFooter>&amp;F&amp;RPage &amp;P</oddFooter>
   </headerFooter>
   <ignoredErrors>
-    <ignoredError sqref="B1019:B1082 B991:B997 B19:B990 B1083 B998:B1017" numberStoredAsText="1"/>
+    <ignoredError sqref="B1018:B1081 B990:B996 B19:B989 B1082 B997:B1016" numberStoredAsText="1"/>
   </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Updated RS and config files for MS-OXCFOLD and MS-ONESTORE.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25225"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3294447D-2FCC-4BCC-A3BF-6B571B90C988}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{186408CE-DC75-4FB3-BF28-E2BB94EE948F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -7593,9 +7593,6 @@
     <t>[In Appendix A: Product Behavior] If this bit [DELETE_HARD_DELETE] is set, implement does hard delete the folder. &lt;4&gt; Section 2.2.1.3.1:  For Exchange 2003 and later, if DELETE_HARD_DELETE is set, the folder is hard deleted.</t>
   </si>
   <si>
-    <t>23.0</t>
-  </si>
-  <si>
     <t>[In Appendix A: Product Behavior] The implementation does not support the PidTagAddressBookEntryId property. &lt;10&gt; Section 2.2.2.2.1.4:  Exchange 2013 and later do not support the PidTagAddressBookEntryId property.</t>
   </si>
   <si>
@@ -7603,6 +7600,9 @@
   </si>
   <si>
     <t>[In Appendix A: Product Behavior] Implementation does return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder. &lt;20&gt; Section 3.2.5.9: Update Rollup 4 for Exchange Server 2010 Service Pack 2 (SP2) and later return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder.</t>
+  </si>
+  <si>
+    <t>23.1</t>
   </si>
 </sst>
 </file>
@@ -9030,8 +9030,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L1082"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" topLeftCell="A1001" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -9075,7 +9075,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="33" t="s">
-        <v>2424</v>
+        <v>2427</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>26</v>
@@ -34225,7 +34225,7 @@
         <v>1159</v>
       </c>
       <c r="C1001" s="20" t="s">
-        <v>2425</v>
+        <v>2424</v>
       </c>
       <c r="D1001" s="34" t="s">
         <v>2288</v>
@@ -34484,7 +34484,7 @@
         <v>1159</v>
       </c>
       <c r="C1010" s="20" t="s">
-        <v>2426</v>
+        <v>2425</v>
       </c>
       <c r="D1010" s="22" t="s">
         <v>2062</v>
@@ -34772,7 +34772,7 @@
         <v>1159</v>
       </c>
       <c r="C1020" s="20" t="s">
-        <v>2427</v>
+        <v>2426</v>
       </c>
       <c r="D1020" s="22" t="s">
         <v>2065</v>

</xml_diff>

<commit_message>
Updated files for MS-OXCFOLD、MS-OXCRPC and MS-OFFICIALFILE.
</commit_message>
<xml_diff>
--- a/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
+++ b/ExchangeMAPI/Docs/MS-OXCFOLD/MS-OXCFOLD_RequirementSpecification.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89153F30-BE6C-43C5-8E8D-C249A2B9CA22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3039DB0-3DC1-437D-8F4E-1C15F22CFE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="2" r:id="rId1"/>
@@ -7587,10 +7587,10 @@
     <t>[In Appendix A: Product Behavior] Implementation does return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder. &lt;20&gt; Section 3.2.5.9: Update Rollup 4 for Exchange Server 2010 Service Pack 2 (SP2) and later return ecNotSupported when the RopEmptyFolder ROP is called on the Root folder.</t>
   </si>
   <si>
-    <t>23.2</t>
-  </si>
-  <si>
     <t>[In RopDeleteFolder ROP Request Buffer] DeleteFolderFlags (1 byte): If this bit [DELETE_HARD_DELETE (0x10)] is set, the folder SHOULD be hard deleted.</t>
+  </si>
+  <si>
+    <t>23.1</t>
   </si>
 </sst>
 </file>
@@ -7891,6 +7891,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -7915,262 +7930,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="63">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -8509,6 +8273,242 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike/>
+      </font>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -8638,34 +8638,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1080" tableType="xml" totalsRowShown="0" headerRowDxfId="62" dataDxfId="61" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Requirement" displayName="Requirement" ref="A19:I1080" tableType="xml" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17" connectionId="1">
   <autoFilter ref="A19:I1080" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="60">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" uniqueName="ns1:REQ_ID" name="Req ID" dataDxfId="16">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:REQ_ID" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="59">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" uniqueName="ns1:Doc_Sect" name="Doc Sect" dataDxfId="15">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Doc_Sect" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="58">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" uniqueName="ns1:Description" name="Description" dataDxfId="14">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Description" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="57">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" uniqueName="ns1:Derived" name="Derived" dataDxfId="13">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Derived" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="56">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" uniqueName="ns1:Behavior" name="Behavior" dataDxfId="12">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Behavior" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="55">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" uniqueName="ns1:Scope" name="Scope" dataDxfId="11">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Scope" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="54">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" uniqueName="ns1:IsNormative" name="Informative_x000a_/Normative" dataDxfId="10">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:IsNormative" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" uniqueName="ns1:Verification" name="Verification" dataDxfId="9">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:Verification" xmlDataType="string"/>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="52">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" uniqueName="ns1:VerificationComment" name="Verification Comment" dataDxfId="8">
       <xmlColumnPr mapId="12" xpath="/ns1:ReqTable/ns1:Requirement/ns1:VerificationComment" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
@@ -8674,12 +8674,12 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="49" headerRowBorderDxfId="50" tableBorderDxfId="48" totalsRowBorderDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Scope" displayName="Scope" ref="A12:C15" totalsRowShown="0" headerRowDxfId="7" dataDxfId="5" headerRowBorderDxfId="6" tableBorderDxfId="4" totalsRowBorderDxfId="3">
   <autoFilter ref="A12:C15" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="44"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Scope" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Test" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9009,8 +9009,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J1081"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A987" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A990" sqref="A990:XFD990"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -9053,138 +9053,138 @@
         <v>25</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>2422</v>
+        <v>2423</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>26</v>
       </c>
       <c r="F3" s="9">
-        <v>44698</v>
+        <v>44789</v>
       </c>
       <c r="J3" s="4"/>
     </row>
     <row r="4" spans="1:10" ht="21">
-      <c r="A4" s="43" t="s">
+      <c r="A4" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
       <c r="J4" s="4"/>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="47"/>
-      <c r="E5" s="47"/>
-      <c r="F5" s="47"/>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="47"/>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39"/>
       <c r="J5" s="4"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="45" t="s">
+      <c r="B6" s="37" t="s">
         <v>2307</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="45"/>
+      <c r="C6" s="37"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="37"/>
+      <c r="I6" s="37"/>
       <c r="J6" s="4"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="36"/>
+      <c r="I7" s="36"/>
       <c r="J7" s="4"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="44"/>
-      <c r="E8" s="44"/>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="44"/>
-      <c r="I8" s="44"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="H8" s="36"/>
+      <c r="I8" s="36"/>
       <c r="J8" s="4"/>
     </row>
     <row r="9" spans="1:10" ht="78.75" customHeight="1">
       <c r="A9" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="39" t="s">
+      <c r="B9" s="44" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
+      <c r="C9" s="45"/>
+      <c r="D9" s="45"/>
+      <c r="E9" s="45"/>
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="H9" s="45"/>
+      <c r="I9" s="45"/>
       <c r="J9" s="4"/>
     </row>
     <row r="10" spans="1:10" ht="33.75" customHeight="1">
       <c r="A10" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="40"/>
-      <c r="I10" s="40"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
-      <c r="H11" s="35"/>
-      <c r="I11" s="35"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
       <c r="J11" s="4"/>
     </row>
     <row r="12" spans="1:10">
@@ -9197,12 +9197,12 @@
       <c r="C12" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="36"/>
-      <c r="E12" s="36"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36"/>
-      <c r="H12" s="36"/>
-      <c r="I12" s="36"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="15" customHeight="1">
@@ -9215,12 +9215,12 @@
       <c r="C13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
+      <c r="D13" s="42"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
+      <c r="G13" s="42"/>
+      <c r="H13" s="42"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="4"/>
     </row>
     <row r="14" spans="1:10">
@@ -9233,12 +9233,12 @@
       <c r="C14" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="37"/>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="42"/>
       <c r="J14" s="4"/>
     </row>
     <row r="15" spans="1:10" ht="30">
@@ -9251,60 +9251,60 @@
       <c r="C15" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
       <c r="J15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="30" customHeight="1">
       <c r="A16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="35" t="s">
+      <c r="B16" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
       <c r="J16" s="4"/>
     </row>
     <row r="17" spans="1:10" ht="64.5" customHeight="1">
       <c r="A17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="46" t="s">
         <v>2305</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
-      <c r="H17" s="42"/>
-      <c r="I17" s="42"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="47"/>
+      <c r="G17" s="47"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
       <c r="J17" s="4"/>
     </row>
     <row r="18" spans="1:10" ht="30" customHeight="1">
       <c r="A18" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="35" t="s">
+      <c r="B18" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="35"/>
-      <c r="H18" s="35"/>
-      <c r="I18" s="35"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40"/>
+      <c r="E18" s="40"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="40"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
       <c r="J18" s="4"/>
     </row>
     <row r="19" spans="1:10" ht="30">
@@ -12197,7 +12197,7 @@
         <v>1070</v>
       </c>
       <c r="C133" s="17" t="s">
-        <v>2423</v>
+        <v>2422</v>
       </c>
       <c r="D133" s="25"/>
       <c r="E133" s="25" t="s">
@@ -36300,11 +36300,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="B8:I8"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="B5:I5"/>
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="D12:I15"/>
     <mergeCell ref="B16:I16"/>
@@ -36312,169 +36307,174 @@
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="B5:I5"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="A246:I246 A1030:I1080 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1028">
-    <cfRule type="expression" dxfId="43" priority="107">
+    <cfRule type="expression" dxfId="62" priority="107">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="108">
+    <cfRule type="expression" dxfId="61" priority="108">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="41" priority="115">
+    <cfRule type="expression" dxfId="60" priority="115">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A246:I246 A1030:I1080 E230:I230 E233:I241 A247:J250 A242:J245 E34:I224 I20:I224 E226:I227 A20:H241 A251:I518 A521:I1028">
-    <cfRule type="expression" dxfId="40" priority="61">
+    <cfRule type="expression" dxfId="59" priority="61">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="62">
+    <cfRule type="expression" dxfId="58" priority="62">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="38" priority="63">
+    <cfRule type="expression" dxfId="57" priority="63">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F246 F1031:F1080 F20:F241 F251:F518 F521:F1028">
-    <cfRule type="expression" dxfId="37" priority="67">
+    <cfRule type="expression" dxfId="56" priority="67">
       <formula>NOT(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="68">
+    <cfRule type="expression" dxfId="55" priority="68">
       <formula>(VLOOKUP(F20,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1031:I1080 I230 I233:I241">
-    <cfRule type="expression" dxfId="35" priority="58">
+    <cfRule type="expression" dxfId="54" priority="58">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="59">
+    <cfRule type="expression" dxfId="53" priority="59">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="60">
+    <cfRule type="expression" dxfId="52" priority="60">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I246 I1031:I1080 I230 I233:I241">
-    <cfRule type="expression" dxfId="32" priority="55">
+    <cfRule type="expression" dxfId="51" priority="55">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="56">
+    <cfRule type="expression" dxfId="50" priority="56">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="57">
+    <cfRule type="expression" dxfId="49" priority="57">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1030">
-    <cfRule type="expression" dxfId="29" priority="38">
+    <cfRule type="expression" dxfId="48" priority="38">
       <formula>NOT(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="39">
+    <cfRule type="expression" dxfId="47" priority="39">
       <formula>(VLOOKUP(F1030,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1030">
-    <cfRule type="expression" dxfId="27" priority="32">
+    <cfRule type="expression" dxfId="46" priority="32">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="33">
+    <cfRule type="expression" dxfId="45" priority="33">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="34">
+    <cfRule type="expression" dxfId="44" priority="34">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1030">
-    <cfRule type="expression" dxfId="24" priority="29">
+    <cfRule type="expression" dxfId="43" priority="29">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="30">
+    <cfRule type="expression" dxfId="42" priority="30">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="31">
+    <cfRule type="expression" dxfId="41" priority="31">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1029 C1029:I1029">
-    <cfRule type="expression" dxfId="21" priority="26">
+    <cfRule type="expression" dxfId="40" priority="26">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="20" priority="27">
+    <cfRule type="expression" dxfId="39" priority="27">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="28">
+    <cfRule type="expression" dxfId="38" priority="28">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1029 C1029:I1029">
-    <cfRule type="expression" dxfId="18" priority="21">
+    <cfRule type="expression" dxfId="37" priority="21">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="22">
+    <cfRule type="expression" dxfId="36" priority="22">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="23">
+    <cfRule type="expression" dxfId="35" priority="23">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1029">
-    <cfRule type="expression" dxfId="15" priority="24">
+    <cfRule type="expression" dxfId="34" priority="24">
       <formula>NOT(VLOOKUP(F1029,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="25">
+    <cfRule type="expression" dxfId="33" priority="25">
       <formula>(VLOOKUP(F1029,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1029">
-    <cfRule type="expression" dxfId="13" priority="12">
+    <cfRule type="expression" dxfId="32" priority="12">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="13">
+    <cfRule type="expression" dxfId="31" priority="13">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="14">
+    <cfRule type="expression" dxfId="30" priority="14">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1029">
-    <cfRule type="expression" dxfId="10" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="10">
+    <cfRule type="expression" dxfId="28" priority="10">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="27" priority="11">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="7" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Section Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="25" priority="7">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="24" priority="8">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A519:I520">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"SectionDeleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="22" priority="2">
       <formula>EXACT(INDIRECT("P"&amp;ROW()),"Deleted")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="21" priority="3">
       <formula>EXACT(INDIRECT("L"&amp;ROW()),"Deleted")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F519:F520">
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="20" priority="4">
       <formula>NOT(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="5">
+    <cfRule type="expression" dxfId="19" priority="5">
       <formula>(VLOOKUP(F519,$A$12:$C$15,2,FALSE)="In")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>